<commit_message>
dmft and merging databases
</commit_message>
<xml_diff>
--- a/data dictionary/DICC_A434_M3_NINOS.RID.xlsx
+++ b/data dictionary/DICC_A434_M3_NINOS.RID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a5584703a9932d8/Documentos/RStudio/thesis/data dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{76951DC6-D1D1-4F7A-8241-5F94A5EAB1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4756B28B-AD5B-47D0-A29D-240F4316A16E}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{76951DC6-D1D1-4F7A-8241-5F94A5EAB1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF790EBF-033E-4A9D-896A-D9A083F1C813}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="491">
   <si>
     <r>
       <rPr>
@@ -5638,6 +5638,12 @@
   </si>
   <si>
     <t>determinante social</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Given name</t>
   </si>
 </sst>
 </file>
@@ -5921,47 +5927,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5975,8 +5951,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5984,17 +5999,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6300,10 +6306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="L121" sqref="L121"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6314,15 +6320,15 @@
     <col min="4" max="4" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6335,12 +6341,14 @@
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -6353,12 +6361,8 @@
       <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -6372,7 +6376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -6386,8 +6390,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>484</v>
       </c>
       <c r="B6" s="16">
@@ -6400,7 +6404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -6414,7 +6418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -6428,7 +6432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -6442,7 +6446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -6456,7 +6460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
@@ -6470,7 +6474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
@@ -6484,7 +6488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
@@ -6498,7 +6502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -6512,7 +6516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
@@ -6526,7 +6530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>28</v>
       </c>
@@ -6541,7 +6545,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="21" t="s">
         <v>485</v>
       </c>
       <c r="B17" s="16">
@@ -8157,8 +8161,18 @@
     </row>
     <row r="130" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="131" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="19"/>
+      <c r="B132" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="20"/>
+      <c r="B133" t="s">
+        <v>468</v>
+      </c>
+    </row>
     <row r="134" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="135" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="136" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8195,25 +8209,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>245</v>
       </c>
       <c r="B3" s="8">
@@ -8222,20 +8236,20 @@
       <c r="C3" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="28"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="29" t="s">
         <v>248</v>
       </c>
       <c r="B5" s="8">
@@ -8244,30 +8258,30 @@
       <c r="C5" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="28"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="8">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D6" s="38"/>
+      <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="8">
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="23" t="s">
         <v>252</v>
       </c>
       <c r="B8" s="8">
@@ -8276,20 +8290,20 @@
       <c r="C8" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="D8" s="38"/>
+      <c r="D8" s="28"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="8">
@@ -8298,20 +8312,20 @@
       <c r="C10" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D10" s="38"/>
+      <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="8">
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D11" s="38"/>
+      <c r="D11" s="28"/>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="8">
@@ -8320,30 +8334,30 @@
       <c r="C12" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D12" s="38"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="8">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="D13" s="38"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="8">
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="28"/>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="8">
@@ -8352,20 +8366,20 @@
       <c r="C15" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="28"/>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="8">
         <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="D16" s="38"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="8">
@@ -8376,7 +8390,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="8">
         <v>2</v>
       </c>
@@ -8385,7 +8399,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="8">
         <v>3</v>
       </c>
@@ -8394,7 +8408,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="8">
         <v>4</v>
       </c>
@@ -8403,7 +8417,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
@@ -8412,7 +8426,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="8">
         <v>6</v>
       </c>
@@ -8421,7 +8435,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="8">
@@ -8432,7 +8446,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -8441,7 +8455,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -8450,7 +8464,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="8">
         <v>4</v>
       </c>
@@ -8459,7 +8473,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="8">
         <v>5</v>
       </c>
@@ -8468,7 +8482,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="8">
         <v>6</v>
       </c>
@@ -8477,7 +8491,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="23" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="8">
@@ -8488,7 +8502,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="8">
         <v>2</v>
       </c>
@@ -8497,7 +8511,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="8">
@@ -8508,7 +8522,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="8">
         <v>2</v>
       </c>
@@ -8517,7 +8531,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="8">
@@ -8528,7 +8542,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="8">
         <v>8</v>
       </c>
@@ -8537,7 +8551,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="8">
         <v>9</v>
       </c>
@@ -8546,7 +8560,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="8">
         <v>11</v>
       </c>
@@ -8555,7 +8569,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="8">
         <v>12</v>
       </c>
@@ -8564,7 +8578,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="8">
         <v>13</v>
       </c>
@@ -8573,7 +8587,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="29" t="s">
         <v>28</v>
       </c>
       <c r="B39" s="8">
@@ -8584,7 +8598,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="8">
         <v>2</v>
       </c>
@@ -8593,7 +8607,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="8">
         <v>3</v>
       </c>
@@ -8602,7 +8616,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="8">
         <v>4</v>
       </c>
@@ -8611,7 +8625,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="8">
         <v>5</v>
       </c>
@@ -8620,7 +8634,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="8">
         <v>6</v>
       </c>
@@ -8629,7 +8643,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="8">
         <v>7</v>
       </c>
@@ -8638,7 +8652,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="8">
         <v>8</v>
       </c>
@@ -8647,7 +8661,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="8">
         <v>9</v>
       </c>
@@ -8656,7 +8670,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="8">
         <v>10</v>
       </c>
@@ -8665,7 +8679,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="29" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="8">
@@ -8676,7 +8690,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="8">
         <v>2</v>
       </c>
@@ -8685,7 +8699,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
+      <c r="A51" s="30"/>
       <c r="B51" s="8">
         <v>3</v>
       </c>
@@ -8694,7 +8708,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="8">
         <v>4</v>
       </c>
@@ -8703,7 +8717,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="8">
         <v>5</v>
       </c>
@@ -8712,7 +8726,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="24"/>
+      <c r="A54" s="31"/>
       <c r="B54" s="8">
         <v>6</v>
       </c>
@@ -8721,7 +8735,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="29" t="s">
         <v>31</v>
       </c>
       <c r="B55" s="8">
@@ -8732,7 +8746,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
+      <c r="A56" s="30"/>
       <c r="B56" s="8">
         <v>2</v>
       </c>
@@ -8741,7 +8755,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="8">
         <v>3</v>
       </c>
@@ -8750,7 +8764,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="8">
         <v>4</v>
       </c>
@@ -8759,7 +8773,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="8">
         <v>5</v>
       </c>
@@ -8768,7 +8782,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="8">
         <v>6</v>
       </c>
@@ -8777,7 +8791,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="8">
         <v>7</v>
       </c>
@@ -8786,7 +8800,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="24"/>
+      <c r="A62" s="31"/>
       <c r="B62" s="8">
         <v>8</v>
       </c>
@@ -8795,7 +8809,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="27"/>
+      <c r="A63" s="39"/>
       <c r="B63" s="8">
         <v>1</v>
       </c>
@@ -8804,7 +8818,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="28"/>
+      <c r="A64" s="37"/>
       <c r="B64" s="8">
         <v>2</v>
       </c>
@@ -8813,7 +8827,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="28"/>
+      <c r="A65" s="37"/>
       <c r="B65" s="8">
         <v>3</v>
       </c>
@@ -8822,7 +8836,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="23" t="s">
+      <c r="A66" s="30" t="s">
         <v>34</v>
       </c>
       <c r="B66" s="8">
@@ -8833,7 +8847,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="8">
         <v>5</v>
       </c>
@@ -8842,7 +8856,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="8">
         <v>6</v>
       </c>
@@ -8851,7 +8865,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
+      <c r="A69" s="30"/>
       <c r="B69" s="8">
         <v>7</v>
       </c>
@@ -8860,7 +8874,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="8">
         <v>8</v>
       </c>
@@ -8869,7 +8883,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="8">
         <v>9</v>
       </c>
@@ -8878,7 +8892,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="8">
         <v>10</v>
       </c>
@@ -8887,7 +8901,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
+      <c r="A73" s="30"/>
       <c r="B73" s="8">
         <v>11</v>
       </c>
@@ -8896,7 +8910,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="8">
         <v>12</v>
       </c>
@@ -8905,7 +8919,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
+      <c r="A75" s="30"/>
       <c r="B75" s="8">
         <v>13</v>
       </c>
@@ -8914,7 +8928,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="8">
         <v>14</v>
       </c>
@@ -8923,7 +8937,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
+      <c r="A77" s="30"/>
       <c r="B77" s="8">
         <v>15</v>
       </c>
@@ -8932,7 +8946,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
+      <c r="A78" s="30"/>
       <c r="B78" s="8">
         <v>16</v>
       </c>
@@ -8941,7 +8955,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
+      <c r="A79" s="30"/>
       <c r="B79" s="8">
         <v>17</v>
       </c>
@@ -8950,7 +8964,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="24"/>
+      <c r="A80" s="31"/>
       <c r="B80" s="8">
         <v>18</v>
       </c>
@@ -8959,7 +8973,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="25" t="s">
+      <c r="A81" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B81" s="8">
@@ -8970,7 +8984,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
+      <c r="A82" s="24"/>
       <c r="B82" s="8">
         <v>2</v>
       </c>
@@ -8979,7 +8993,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="22" t="s">
+      <c r="A83" s="29" t="s">
         <v>40</v>
       </c>
       <c r="B83" s="8">
@@ -8990,7 +9004,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="23"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="8">
         <v>2</v>
       </c>
@@ -8999,7 +9013,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="23"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="8">
         <v>3</v>
       </c>
@@ -9008,7 +9022,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="23"/>
+      <c r="A86" s="30"/>
       <c r="B86" s="8">
         <v>4</v>
       </c>
@@ -9017,7 +9031,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="23"/>
+      <c r="A87" s="30"/>
       <c r="B87" s="8">
         <v>5</v>
       </c>
@@ -9026,7 +9040,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="23"/>
+      <c r="A88" s="30"/>
       <c r="B88" s="8">
         <v>6</v>
       </c>
@@ -9035,7 +9049,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="23"/>
+      <c r="A89" s="30"/>
       <c r="B89" s="8">
         <v>7</v>
       </c>
@@ -9044,7 +9058,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="23"/>
+      <c r="A90" s="30"/>
       <c r="B90" s="8">
         <v>8</v>
       </c>
@@ -9053,7 +9067,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="23"/>
+      <c r="A91" s="30"/>
       <c r="B91" s="8">
         <v>9</v>
       </c>
@@ -9062,7 +9076,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="23"/>
+      <c r="A92" s="30"/>
       <c r="B92" s="8">
         <v>10</v>
       </c>
@@ -9071,7 +9085,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="23"/>
+      <c r="A93" s="30"/>
       <c r="B93" s="8">
         <v>11</v>
       </c>
@@ -9080,7 +9094,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="23"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="8">
         <v>12</v>
       </c>
@@ -9089,7 +9103,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="23"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="8">
         <v>13</v>
       </c>
@@ -9098,7 +9112,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="23"/>
+      <c r="A96" s="30"/>
       <c r="B96" s="8">
         <v>14</v>
       </c>
@@ -9107,7 +9121,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="23"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="8">
         <v>15</v>
       </c>
@@ -9116,7 +9130,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="23"/>
+      <c r="A98" s="30"/>
       <c r="B98" s="8">
         <v>16</v>
       </c>
@@ -9125,7 +9139,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="24"/>
+      <c r="A99" s="31"/>
       <c r="B99" s="8">
         <v>18</v>
       </c>
@@ -9134,7 +9148,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="25" t="s">
+      <c r="A100" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B100" s="8">
@@ -9145,7 +9159,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="29"/>
+      <c r="A101" s="32"/>
       <c r="B101" s="8">
         <v>2</v>
       </c>
@@ -9154,7 +9168,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
+      <c r="A102" s="32"/>
       <c r="B102" s="8">
         <v>3</v>
       </c>
@@ -9163,7 +9177,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="26"/>
+      <c r="A103" s="24"/>
       <c r="B103" s="8">
         <v>4</v>
       </c>
@@ -9172,7 +9186,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="s">
+      <c r="A104" s="35" t="s">
         <v>46</v>
       </c>
       <c r="B104" s="8">
@@ -9183,7 +9197,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="31"/>
+      <c r="A105" s="36"/>
       <c r="B105" s="8">
         <v>2</v>
       </c>
@@ -9192,7 +9206,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="31"/>
+      <c r="A106" s="36"/>
       <c r="B106" s="8">
         <v>3</v>
       </c>
@@ -9201,7 +9215,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="31"/>
+      <c r="A107" s="36"/>
       <c r="B107" s="8">
         <v>4</v>
       </c>
@@ -9210,7 +9224,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
+      <c r="A108" s="36"/>
       <c r="B108" s="8">
         <v>5</v>
       </c>
@@ -9219,7 +9233,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="31"/>
+      <c r="A109" s="36"/>
       <c r="B109" s="8">
         <v>6</v>
       </c>
@@ -9228,7 +9242,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="31"/>
+      <c r="A110" s="36"/>
       <c r="B110" s="8">
         <v>7</v>
       </c>
@@ -9237,7 +9251,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="31"/>
+      <c r="A111" s="36"/>
       <c r="B111" s="8">
         <v>8</v>
       </c>
@@ -9246,7 +9260,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="31"/>
+      <c r="A112" s="36"/>
       <c r="B112" s="8">
         <v>9</v>
       </c>
@@ -9255,7 +9269,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
+      <c r="A113" s="36"/>
       <c r="B113" s="8">
         <v>10</v>
       </c>
@@ -9264,7 +9278,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="31"/>
+      <c r="A114" s="36"/>
       <c r="B114" s="8">
         <v>11</v>
       </c>
@@ -9273,7 +9287,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="28"/>
+      <c r="A115" s="37"/>
       <c r="B115" s="8">
         <v>12</v>
       </c>
@@ -9282,7 +9296,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="28"/>
+      <c r="A116" s="37"/>
       <c r="B116" s="8">
         <v>13</v>
       </c>
@@ -9291,7 +9305,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="28"/>
+      <c r="A117" s="37"/>
       <c r="B117" s="8">
         <v>14</v>
       </c>
@@ -9300,7 +9314,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="28"/>
+      <c r="A118" s="37"/>
       <c r="B118" s="8">
         <v>15</v>
       </c>
@@ -9309,7 +9323,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="28"/>
+      <c r="A119" s="37"/>
       <c r="B119" s="8">
         <v>16</v>
       </c>
@@ -9318,7 +9332,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
+      <c r="A120" s="38"/>
       <c r="B120" s="8">
         <v>17</v>
       </c>
@@ -9327,7 +9341,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="22" t="s">
+      <c r="A121" s="29" t="s">
         <v>50</v>
       </c>
       <c r="B121" s="8">
@@ -9338,7 +9352,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="23"/>
+      <c r="A122" s="30"/>
       <c r="B122" s="8">
         <v>2</v>
       </c>
@@ -9347,7 +9361,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="23"/>
+      <c r="A123" s="30"/>
       <c r="B123" s="8">
         <v>3</v>
       </c>
@@ -9356,7 +9370,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="23"/>
+      <c r="A124" s="30"/>
       <c r="B124" s="8">
         <v>4</v>
       </c>
@@ -9365,7 +9379,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="23"/>
+      <c r="A125" s="30"/>
       <c r="B125" s="8">
         <v>5</v>
       </c>
@@ -9374,7 +9388,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="23"/>
+      <c r="A126" s="30"/>
       <c r="B126" s="8">
         <v>6</v>
       </c>
@@ -9383,7 +9397,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="23"/>
+      <c r="A127" s="30"/>
       <c r="B127" s="8">
         <v>7</v>
       </c>
@@ -9392,7 +9406,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="24"/>
+      <c r="A128" s="31"/>
       <c r="B128" s="8">
         <v>8</v>
       </c>
@@ -9401,7 +9415,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="25" t="s">
+      <c r="A129" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B129" s="8">
@@ -9412,7 +9426,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="26"/>
+      <c r="A130" s="24"/>
       <c r="B130" s="8">
         <v>1</v>
       </c>
@@ -9421,7 +9435,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="25" t="s">
+      <c r="A131" s="23" t="s">
         <v>53</v>
       </c>
       <c r="B131" s="8">
@@ -9432,7 +9446,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="26"/>
+      <c r="A132" s="24"/>
       <c r="B132" s="8">
         <v>1</v>
       </c>
@@ -9441,7 +9455,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="25" t="s">
+      <c r="A133" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B133" s="8">
@@ -9452,7 +9466,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="26"/>
+      <c r="A134" s="24"/>
       <c r="B134" s="8">
         <v>1</v>
       </c>
@@ -9461,7 +9475,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="25" t="s">
+      <c r="A135" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B135" s="8">
@@ -9472,7 +9486,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="26"/>
+      <c r="A136" s="24"/>
       <c r="B136" s="8">
         <v>1</v>
       </c>
@@ -9481,7 +9495,7 @@
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="25" t="s">
+      <c r="A137" s="23" t="s">
         <v>59</v>
       </c>
       <c r="B137" s="8">
@@ -9492,7 +9506,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="26"/>
+      <c r="A138" s="24"/>
       <c r="B138" s="8">
         <v>1</v>
       </c>
@@ -9501,7 +9515,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="25" t="s">
+      <c r="A139" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B139" s="8">
@@ -9512,7 +9526,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="26"/>
+      <c r="A140" s="24"/>
       <c r="B140" s="8">
         <v>1</v>
       </c>
@@ -9521,7 +9535,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="25" t="s">
+      <c r="A141" s="23" t="s">
         <v>63</v>
       </c>
       <c r="B141" s="8">
@@ -9532,7 +9546,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="26"/>
+      <c r="A142" s="24"/>
       <c r="B142" s="8">
         <v>1</v>
       </c>
@@ -9541,7 +9555,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="25" t="s">
+      <c r="A143" s="23" t="s">
         <v>65</v>
       </c>
       <c r="B143" s="8">
@@ -9552,7 +9566,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="29"/>
+      <c r="A144" s="32"/>
       <c r="B144" s="8">
         <v>2</v>
       </c>
@@ -9561,7 +9575,7 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="29"/>
+      <c r="A145" s="32"/>
       <c r="B145" s="8">
         <v>3</v>
       </c>
@@ -9570,7 +9584,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="26"/>
+      <c r="A146" s="24"/>
       <c r="B146" s="8">
         <v>4</v>
       </c>
@@ -9579,7 +9593,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="22" t="s">
+      <c r="A147" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B147" s="8">
@@ -9590,7 +9604,7 @@
       </c>
     </row>
     <row r="148" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="23"/>
+      <c r="A148" s="30"/>
       <c r="B148" s="8">
         <v>2</v>
       </c>
@@ -9599,7 +9613,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="23"/>
+      <c r="A149" s="30"/>
       <c r="B149" s="8">
         <v>3</v>
       </c>
@@ -9608,7 +9622,7 @@
       </c>
     </row>
     <row r="150" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="23"/>
+      <c r="A150" s="30"/>
       <c r="B150" s="8">
         <v>4</v>
       </c>
@@ -9617,7 +9631,7 @@
       </c>
     </row>
     <row r="151" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="23"/>
+      <c r="A151" s="30"/>
       <c r="B151" s="8">
         <v>5</v>
       </c>
@@ -9626,7 +9640,7 @@
       </c>
     </row>
     <row r="152" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="24"/>
+      <c r="A152" s="31"/>
       <c r="B152" s="8">
         <v>6</v>
       </c>
@@ -9635,7 +9649,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="25" t="s">
+      <c r="A153" s="23" t="s">
         <v>68</v>
       </c>
       <c r="B153" s="8">
@@ -9646,7 +9660,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="26"/>
+      <c r="A154" s="24"/>
       <c r="B154" s="8">
         <v>2</v>
       </c>
@@ -9655,7 +9669,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="22" t="s">
+      <c r="A155" s="29" t="s">
         <v>70</v>
       </c>
       <c r="B155" s="8">
@@ -9666,7 +9680,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="23"/>
+      <c r="A156" s="30"/>
       <c r="B156" s="8">
         <v>2</v>
       </c>
@@ -9675,7 +9689,7 @@
       </c>
     </row>
     <row r="157" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="23"/>
+      <c r="A157" s="30"/>
       <c r="B157" s="8">
         <v>3</v>
       </c>
@@ -9684,7 +9698,7 @@
       </c>
     </row>
     <row r="158" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="23"/>
+      <c r="A158" s="30"/>
       <c r="B158" s="8">
         <v>4</v>
       </c>
@@ -9693,7 +9707,7 @@
       </c>
     </row>
     <row r="159" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="23"/>
+      <c r="A159" s="30"/>
       <c r="B159" s="8">
         <v>5</v>
       </c>
@@ -9702,7 +9716,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="23"/>
+      <c r="A160" s="30"/>
       <c r="B160" s="8">
         <v>6</v>
       </c>
@@ -9711,7 +9725,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="23"/>
+      <c r="A161" s="30"/>
       <c r="B161" s="8">
         <v>7</v>
       </c>
@@ -9720,7 +9734,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="24"/>
+      <c r="A162" s="31"/>
       <c r="B162" s="8">
         <v>8</v>
       </c>
@@ -9738,7 +9752,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="29" t="s">
+      <c r="A164" s="32" t="s">
         <v>73</v>
       </c>
       <c r="B164" s="8">
@@ -9749,7 +9763,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="26"/>
+      <c r="A165" s="24"/>
       <c r="B165" s="8">
         <v>3</v>
       </c>
@@ -9758,7 +9772,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="25" t="s">
+      <c r="A166" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B166" s="8">
@@ -9769,7 +9783,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="26"/>
+      <c r="A167" s="24"/>
       <c r="B167" s="8">
         <v>2</v>
       </c>
@@ -9778,7 +9792,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="25" t="s">
+      <c r="A168" s="23" t="s">
         <v>76</v>
       </c>
       <c r="B168" s="8">
@@ -9789,7 +9803,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="29"/>
+      <c r="A169" s="32"/>
       <c r="B169" s="8">
         <v>2</v>
       </c>
@@ -9798,7 +9812,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="29"/>
+      <c r="A170" s="32"/>
       <c r="B170" s="8">
         <v>3</v>
       </c>
@@ -9807,7 +9821,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="26"/>
+      <c r="A171" s="24"/>
       <c r="B171" s="8">
         <v>4</v>
       </c>
@@ -9816,7 +9830,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="22" t="s">
+      <c r="A172" s="29" t="s">
         <v>77</v>
       </c>
       <c r="B172" s="8">
@@ -9827,7 +9841,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="23"/>
+      <c r="A173" s="30"/>
       <c r="B173" s="8">
         <v>2</v>
       </c>
@@ -9836,7 +9850,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="24"/>
+      <c r="A174" s="31"/>
       <c r="B174" s="8">
         <v>3</v>
       </c>
@@ -9845,7 +9859,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="25" t="s">
+      <c r="A175" s="23" t="s">
         <v>79</v>
       </c>
       <c r="B175" s="8">
@@ -9856,7 +9870,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="29"/>
+      <c r="A176" s="32"/>
       <c r="B176" s="8">
         <v>2</v>
       </c>
@@ -9865,7 +9879,7 @@
       </c>
     </row>
     <row r="177" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="29"/>
+      <c r="A177" s="32"/>
       <c r="B177" s="8">
         <v>3</v>
       </c>
@@ -9874,7 +9888,7 @@
       </c>
     </row>
     <row r="178" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="26"/>
+      <c r="A178" s="24"/>
       <c r="B178" s="8">
         <v>4</v>
       </c>
@@ -9883,7 +9897,7 @@
       </c>
     </row>
     <row r="179" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="22" t="s">
+      <c r="A179" s="29" t="s">
         <v>81</v>
       </c>
       <c r="B179" s="8">
@@ -9894,7 +9908,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="23"/>
+      <c r="A180" s="30"/>
       <c r="B180" s="8">
         <v>2</v>
       </c>
@@ -9903,7 +9917,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="24"/>
+      <c r="A181" s="31"/>
       <c r="B181" s="8">
         <v>3</v>
       </c>
@@ -9912,7 +9926,7 @@
       </c>
     </row>
     <row r="182" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="22" t="s">
+      <c r="A182" s="29" t="s">
         <v>82</v>
       </c>
       <c r="B182" s="8">
@@ -9923,7 +9937,7 @@
       </c>
     </row>
     <row r="183" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="23"/>
+      <c r="A183" s="30"/>
       <c r="B183" s="8">
         <v>2</v>
       </c>
@@ -9932,7 +9946,7 @@
       </c>
     </row>
     <row r="184" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="23"/>
+      <c r="A184" s="30"/>
       <c r="B184" s="8">
         <v>3</v>
       </c>
@@ -9941,7 +9955,7 @@
       </c>
     </row>
     <row r="185" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="23"/>
+      <c r="A185" s="30"/>
       <c r="B185" s="8">
         <v>4</v>
       </c>
@@ -9950,7 +9964,7 @@
       </c>
     </row>
     <row r="186" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="24"/>
+      <c r="A186" s="31"/>
       <c r="B186" s="8">
         <v>5</v>
       </c>
@@ -9959,7 +9973,7 @@
       </c>
     </row>
     <row r="187" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="25" t="s">
+      <c r="A187" s="23" t="s">
         <v>86</v>
       </c>
       <c r="B187" s="8">
@@ -9970,7 +9984,7 @@
       </c>
     </row>
     <row r="188" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="26"/>
+      <c r="A188" s="24"/>
       <c r="B188" s="8">
         <v>1</v>
       </c>
@@ -9979,7 +9993,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="25" t="s">
+      <c r="A189" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B189" s="8">
@@ -9990,7 +10004,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="26"/>
+      <c r="A190" s="24"/>
       <c r="B190" s="8">
         <v>1</v>
       </c>
@@ -9999,7 +10013,7 @@
       </c>
     </row>
     <row r="191" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="25" t="s">
+      <c r="A191" s="23" t="s">
         <v>90</v>
       </c>
       <c r="B191" s="8">
@@ -10010,7 +10024,7 @@
       </c>
     </row>
     <row r="192" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="26"/>
+      <c r="A192" s="24"/>
       <c r="B192" s="8">
         <v>1</v>
       </c>
@@ -10019,7 +10033,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="25" t="s">
+      <c r="A193" s="23" t="s">
         <v>92</v>
       </c>
       <c r="B193" s="8">
@@ -10030,7 +10044,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="26"/>
+      <c r="A194" s="24"/>
       <c r="B194" s="8">
         <v>1</v>
       </c>
@@ -10039,7 +10053,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="25" t="s">
+      <c r="A195" s="23" t="s">
         <v>94</v>
       </c>
       <c r="B195" s="8">
@@ -10050,7 +10064,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="26"/>
+      <c r="A196" s="24"/>
       <c r="B196" s="8">
         <v>1</v>
       </c>
@@ -10059,7 +10073,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A197" s="25" t="s">
+      <c r="A197" s="23" t="s">
         <v>96</v>
       </c>
       <c r="B197" s="8">
@@ -10070,7 +10084,7 @@
       </c>
     </row>
     <row r="198" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A198" s="26"/>
+      <c r="A198" s="24"/>
       <c r="B198" s="8">
         <v>1</v>
       </c>
@@ -10079,7 +10093,7 @@
       </c>
     </row>
     <row r="199" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A199" s="25" t="s">
+      <c r="A199" s="23" t="s">
         <v>98</v>
       </c>
       <c r="B199" s="8">
@@ -10090,7 +10104,7 @@
       </c>
     </row>
     <row r="200" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A200" s="26"/>
+      <c r="A200" s="24"/>
       <c r="B200" s="8">
         <v>1</v>
       </c>
@@ -10099,7 +10113,7 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A201" s="25" t="s">
+      <c r="A201" s="23" t="s">
         <v>100</v>
       </c>
       <c r="B201" s="8">
@@ -10110,7 +10124,7 @@
       </c>
     </row>
     <row r="202" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A202" s="26"/>
+      <c r="A202" s="24"/>
       <c r="B202" s="8">
         <v>1</v>
       </c>
@@ -10119,7 +10133,7 @@
       </c>
     </row>
     <row r="203" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A203" s="25" t="s">
+      <c r="A203" s="23" t="s">
         <v>102</v>
       </c>
       <c r="B203" s="8">
@@ -10130,7 +10144,7 @@
       </c>
     </row>
     <row r="204" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A204" s="26"/>
+      <c r="A204" s="24"/>
       <c r="B204" s="8">
         <v>1</v>
       </c>
@@ -10139,7 +10153,7 @@
       </c>
     </row>
     <row r="205" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A205" s="25" t="s">
+      <c r="A205" s="23" t="s">
         <v>104</v>
       </c>
       <c r="B205" s="8">
@@ -10150,7 +10164,7 @@
       </c>
     </row>
     <row r="206" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A206" s="26"/>
+      <c r="A206" s="24"/>
       <c r="B206" s="8">
         <v>1</v>
       </c>
@@ -10159,7 +10173,7 @@
       </c>
     </row>
     <row r="207" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A207" s="25" t="s">
+      <c r="A207" s="23" t="s">
         <v>106</v>
       </c>
       <c r="B207" s="8">
@@ -10170,7 +10184,7 @@
       </c>
     </row>
     <row r="208" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A208" s="26"/>
+      <c r="A208" s="24"/>
       <c r="B208" s="8">
         <v>1</v>
       </c>
@@ -10179,7 +10193,7 @@
       </c>
     </row>
     <row r="209" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A209" s="25" t="s">
+      <c r="A209" s="23" t="s">
         <v>108</v>
       </c>
       <c r="B209" s="8">
@@ -10190,7 +10204,7 @@
       </c>
     </row>
     <row r="210" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A210" s="26"/>
+      <c r="A210" s="24"/>
       <c r="B210" s="8">
         <v>1</v>
       </c>
@@ -10199,7 +10213,7 @@
       </c>
     </row>
     <row r="211" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A211" s="25" t="s">
+      <c r="A211" s="23" t="s">
         <v>110</v>
       </c>
       <c r="B211" s="8">
@@ -10210,7 +10224,7 @@
       </c>
     </row>
     <row r="212" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A212" s="26"/>
+      <c r="A212" s="24"/>
       <c r="B212" s="8">
         <v>1</v>
       </c>
@@ -10220,6 +10234,47 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A39:A48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A55:A62"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A128"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="A133:A134"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A146"/>
+    <mergeCell ref="A147:A152"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="A155:A162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="A168:A171"/>
+    <mergeCell ref="A172:A174"/>
+    <mergeCell ref="A175:A178"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A182:A186"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A187:A188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="A193:A194"/>
+    <mergeCell ref="A195:A196"/>
     <mergeCell ref="A207:A208"/>
     <mergeCell ref="A209:A210"/>
     <mergeCell ref="A211:A212"/>
@@ -10236,47 +10291,6 @@
     <mergeCell ref="A199:A200"/>
     <mergeCell ref="A201:A202"/>
     <mergeCell ref="A203:A204"/>
-    <mergeCell ref="A205:A206"/>
-    <mergeCell ref="A187:A188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="A193:A194"/>
-    <mergeCell ref="A195:A196"/>
-    <mergeCell ref="A168:A171"/>
-    <mergeCell ref="A172:A174"/>
-    <mergeCell ref="A175:A178"/>
-    <mergeCell ref="A179:A181"/>
-    <mergeCell ref="A182:A186"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="A155:A162"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A146"/>
-    <mergeCell ref="A147:A152"/>
-    <mergeCell ref="A121:A128"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="A133:A134"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A99"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="A104:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A39:A48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="A55:A62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A80"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10298,7 +10312,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>112</v>
       </c>
       <c r="B1" s="8">
@@ -10309,7 +10323,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="8">
         <v>92</v>
       </c>
@@ -10318,7 +10332,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="29" t="s">
         <v>113</v>
       </c>
       <c r="B3" s="8">
@@ -10329,7 +10343,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -10338,7 +10352,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="8">
         <v>3</v>
       </c>
@@ -10347,7 +10361,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="23" t="s">
         <v>114</v>
       </c>
       <c r="B6" s="8">
@@ -10358,7 +10372,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="8">
         <v>1</v>
       </c>
@@ -10367,7 +10381,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="23" t="s">
         <v>116</v>
       </c>
       <c r="B8" s="8">
@@ -10378,7 +10392,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="8">
         <v>1</v>
       </c>
@@ -10387,7 +10401,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>118</v>
       </c>
       <c r="B10" s="8">
@@ -10398,7 +10412,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="8">
         <v>1</v>
       </c>
@@ -10407,7 +10421,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="23" t="s">
         <v>120</v>
       </c>
       <c r="B12" s="8">
@@ -10418,7 +10432,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="8">
         <v>1</v>
       </c>
@@ -10427,7 +10441,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="23" t="s">
         <v>122</v>
       </c>
       <c r="B14" s="8">
@@ -10438,7 +10452,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="8">
         <v>1</v>
       </c>
@@ -10447,7 +10461,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="23" t="s">
         <v>124</v>
       </c>
       <c r="B16" s="8">
@@ -10458,7 +10472,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="8">
         <v>2</v>
       </c>
@@ -10467,7 +10481,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="23" t="s">
         <v>126</v>
       </c>
       <c r="B18" s="8">
@@ -10478,7 +10492,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="8">
         <v>92</v>
       </c>
@@ -10487,7 +10501,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="29" t="s">
         <v>128</v>
       </c>
       <c r="B20" s="8">
@@ -10498,7 +10512,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="8">
         <v>2</v>
       </c>
@@ -10507,7 +10521,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="8">
         <v>3</v>
       </c>
@@ -10516,7 +10530,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="29" t="s">
         <v>130</v>
       </c>
       <c r="B23" s="8">
@@ -10527,7 +10541,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -10536,7 +10550,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -10545,7 +10559,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="23" t="s">
         <v>374</v>
       </c>
       <c r="B26" s="8">
@@ -10556,7 +10570,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="8">
         <v>2</v>
       </c>
@@ -10565,7 +10579,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="23" t="s">
         <v>132</v>
       </c>
       <c r="B28" s="8">
@@ -10576,7 +10590,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="8">
         <v>1</v>
       </c>
@@ -10585,7 +10599,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="23" t="s">
         <v>134</v>
       </c>
       <c r="B30" s="8">
@@ -10596,7 +10610,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="8">
         <v>1</v>
       </c>
@@ -10605,7 +10619,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="23" t="s">
         <v>136</v>
       </c>
       <c r="B32" s="8">
@@ -10616,7 +10630,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="8">
         <v>1</v>
       </c>
@@ -10625,7 +10639,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="23" t="s">
         <v>138</v>
       </c>
       <c r="B34" s="8">
@@ -10636,7 +10650,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="8">
         <v>1</v>
       </c>
@@ -10645,7 +10659,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="23" t="s">
         <v>140</v>
       </c>
       <c r="B36" s="8">
@@ -10656,7 +10670,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="8">
         <v>1</v>
       </c>
@@ -10665,7 +10679,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="23" t="s">
         <v>142</v>
       </c>
       <c r="B38" s="8">
@@ -10676,7 +10690,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="8">
         <v>1</v>
       </c>
@@ -10685,7 +10699,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="23" t="s">
         <v>144</v>
       </c>
       <c r="B40" s="8">
@@ -10696,7 +10710,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="8">
         <v>1</v>
       </c>
@@ -10705,7 +10719,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="23" t="s">
         <v>375</v>
       </c>
       <c r="B42" s="8">
@@ -10716,7 +10730,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="8">
         <v>2</v>
       </c>
@@ -10725,7 +10739,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="23" t="s">
         <v>148</v>
       </c>
       <c r="B44" s="8">
@@ -10736,7 +10750,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
+      <c r="A45" s="32"/>
       <c r="B45" s="8">
         <v>2</v>
       </c>
@@ -10745,7 +10759,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
+      <c r="A46" s="32"/>
       <c r="B46" s="8">
         <v>3</v>
       </c>
@@ -10754,7 +10768,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+      <c r="A47" s="24"/>
       <c r="B47" s="8">
         <v>4</v>
       </c>
@@ -10763,7 +10777,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="29" t="s">
         <v>150</v>
       </c>
       <c r="B48" s="8">
@@ -10774,7 +10788,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="8">
         <v>2</v>
       </c>
@@ -10783,12 +10797,27 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="39"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:C50"/>
@@ -10797,21 +10826,6 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10833,7 +10847,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40"/>
+      <c r="A1" s="43"/>
       <c r="B1" s="8">
         <v>3</v>
       </c>
@@ -10842,7 +10856,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
+      <c r="A2" s="44"/>
       <c r="B2" s="8">
         <v>4</v>
       </c>
@@ -10851,7 +10865,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>152</v>
       </c>
       <c r="B3" s="8">
@@ -10862,7 +10876,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="8">
         <v>92</v>
       </c>
@@ -10871,7 +10885,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="23" t="s">
         <v>153</v>
       </c>
       <c r="B5" s="8">
@@ -10882,7 +10896,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="8">
         <v>2</v>
       </c>
@@ -10891,7 +10905,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="23" t="s">
         <v>154</v>
       </c>
       <c r="B7" s="8">
@@ -10902,7 +10916,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="8">
         <v>92</v>
       </c>
@@ -10911,7 +10925,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="23" t="s">
         <v>158</v>
       </c>
       <c r="B9" s="8">
@@ -10922,7 +10936,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="8">
         <v>1</v>
       </c>
@@ -10931,7 +10945,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>160</v>
       </c>
       <c r="B11" s="8">
@@ -10942,7 +10956,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="8">
         <v>1</v>
       </c>
@@ -10951,7 +10965,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="23" t="s">
         <v>162</v>
       </c>
       <c r="B13" s="8">
@@ -10962,7 +10976,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="8">
         <v>1</v>
       </c>
@@ -10971,7 +10985,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="23" t="s">
         <v>164</v>
       </c>
       <c r="B15" s="8">
@@ -10982,7 +10996,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="8">
         <v>1</v>
       </c>
@@ -10991,7 +11005,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="23" t="s">
         <v>166</v>
       </c>
       <c r="B17" s="8">
@@ -11002,7 +11016,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="8">
         <v>1</v>
       </c>
@@ -11011,7 +11025,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="23" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="8">
@@ -11022,7 +11036,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="8">
         <v>1</v>
       </c>
@@ -11031,7 +11045,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="23" t="s">
         <v>170</v>
       </c>
       <c r="B21" s="8">
@@ -11042,7 +11056,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="8">
         <v>1</v>
       </c>
@@ -11051,7 +11065,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="29" t="s">
         <v>174</v>
       </c>
       <c r="B23" s="8">
@@ -11062,7 +11076,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -11071,7 +11085,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -11080,7 +11094,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="23" t="s">
         <v>176</v>
       </c>
       <c r="B26" s="8">
@@ -11091,7 +11105,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="8">
         <v>2</v>
       </c>
@@ -11100,7 +11114,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="8">
         <v>3</v>
       </c>
@@ -11109,7 +11123,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="8">
         <v>4</v>
       </c>
@@ -11118,7 +11132,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="29" t="s">
         <v>178</v>
       </c>
       <c r="B30" s="8">
@@ -11129,7 +11143,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="8">
         <v>2</v>
       </c>
@@ -11138,7 +11152,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="8">
         <v>3</v>
       </c>
@@ -11147,7 +11161,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="23" t="s">
         <v>180</v>
       </c>
       <c r="B33" s="8">
@@ -11158,7 +11172,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="8">
         <v>2</v>
       </c>
@@ -11167,7 +11181,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="8">
         <v>3</v>
       </c>
@@ -11176,7 +11190,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="8">
         <v>4</v>
       </c>
@@ -11185,7 +11199,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="29" t="s">
         <v>182</v>
       </c>
       <c r="B37" s="8">
@@ -11196,7 +11210,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="8">
         <v>2</v>
       </c>
@@ -11205,7 +11219,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="8">
         <v>3</v>
       </c>
@@ -11214,7 +11228,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="23" t="s">
         <v>184</v>
       </c>
       <c r="B40" s="8">
@@ -11225,7 +11239,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="8">
         <v>2</v>
       </c>
@@ -11234,7 +11248,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
+      <c r="A42" s="32"/>
       <c r="B42" s="8">
         <v>3</v>
       </c>
@@ -11243,7 +11257,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="8">
         <v>4</v>
       </c>
@@ -11252,7 +11266,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="29" t="s">
         <v>186</v>
       </c>
       <c r="B44" s="8">
@@ -11263,7 +11277,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="8">
         <v>2</v>
       </c>
@@ -11272,7 +11286,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="8">
         <v>3</v>
       </c>
@@ -11281,7 +11295,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="29" t="s">
         <v>188</v>
       </c>
       <c r="B47" s="8">
@@ -11292,7 +11306,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="8">
         <v>2</v>
       </c>
@@ -11301,7 +11315,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="8">
         <v>3</v>
       </c>
@@ -11310,16 +11324,16 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="42">
+      <c r="A50" s="41">
         <v>4</v>
       </c>
-      <c r="B50" s="43"/>
+      <c r="B50" s="42"/>
       <c r="C50" s="7" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="29" t="s">
         <v>190</v>
       </c>
       <c r="B51" s="8">
@@ -11330,7 +11344,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="8">
         <v>2</v>
       </c>
@@ -11339,7 +11353,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="24"/>
+      <c r="A53" s="31"/>
       <c r="B53" s="8">
         <v>3</v>
       </c>
@@ -11348,7 +11362,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="23" t="s">
         <v>192</v>
       </c>
       <c r="B54" s="8">
@@ -11359,7 +11373,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="29"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="8">
         <v>2</v>
       </c>
@@ -11368,7 +11382,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="8">
         <v>3</v>
       </c>
@@ -11377,7 +11391,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="8">
         <v>4</v>
       </c>
@@ -11386,7 +11400,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
+      <c r="A58" s="29" t="s">
         <v>194</v>
       </c>
       <c r="B58" s="8">
@@ -11397,7 +11411,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="8">
         <v>2</v>
       </c>
@@ -11406,7 +11420,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
+      <c r="A60" s="31"/>
       <c r="B60" s="8">
         <v>3</v>
       </c>
@@ -11415,7 +11429,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="25" t="s">
+      <c r="A61" s="23" t="s">
         <v>196</v>
       </c>
       <c r="B61" s="8">
@@ -11426,7 +11440,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="29"/>
+      <c r="A62" s="32"/>
       <c r="B62" s="8">
         <v>2</v>
       </c>
@@ -11435,7 +11449,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="29"/>
+      <c r="A63" s="32"/>
       <c r="B63" s="8">
         <v>3</v>
       </c>
@@ -11444,7 +11458,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="8">
         <v>4</v>
       </c>
@@ -11453,7 +11467,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="22" t="s">
+      <c r="A65" s="29" t="s">
         <v>198</v>
       </c>
       <c r="B65" s="8">
@@ -11464,7 +11478,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="8">
         <v>2</v>
       </c>
@@ -11473,7 +11487,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="24"/>
+      <c r="A67" s="31"/>
       <c r="B67" s="8">
         <v>3</v>
       </c>
@@ -11482,7 +11496,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="23" t="s">
         <v>200</v>
       </c>
       <c r="B68" s="8">
@@ -11493,7 +11507,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="29"/>
+      <c r="A69" s="32"/>
       <c r="B69" s="8">
         <v>2</v>
       </c>
@@ -11502,7 +11516,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="29"/>
+      <c r="A70" s="32"/>
       <c r="B70" s="8">
         <v>3</v>
       </c>
@@ -11511,7 +11525,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="8">
         <v>4</v>
       </c>
@@ -11520,7 +11534,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="22" t="s">
+      <c r="A72" s="29" t="s">
         <v>202</v>
       </c>
       <c r="B72" s="8">
@@ -11531,7 +11545,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
+      <c r="A73" s="30"/>
       <c r="B73" s="8">
         <v>2</v>
       </c>
@@ -11540,7 +11554,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="24"/>
+      <c r="A74" s="31"/>
       <c r="B74" s="8">
         <v>3</v>
       </c>
@@ -11549,7 +11563,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="25" t="s">
+      <c r="A75" s="23" t="s">
         <v>204</v>
       </c>
       <c r="B75" s="8">
@@ -11560,7 +11574,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="A76" s="32"/>
       <c r="B76" s="8">
         <v>2</v>
       </c>
@@ -11569,7 +11583,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="8">
         <v>3</v>
       </c>
@@ -11578,7 +11592,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="26"/>
+      <c r="A78" s="24"/>
       <c r="B78" s="8">
         <v>4</v>
       </c>
@@ -11587,7 +11601,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="22" t="s">
+      <c r="A79" s="29" t="s">
         <v>206</v>
       </c>
       <c r="B79" s="8">
@@ -11598,7 +11612,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="8">
         <v>2</v>
       </c>
@@ -11607,7 +11621,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="24"/>
+      <c r="A81" s="31"/>
       <c r="B81" s="8">
         <v>3</v>
       </c>
@@ -11616,7 +11630,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="25" t="s">
+      <c r="A82" s="23" t="s">
         <v>208</v>
       </c>
       <c r="B82" s="8">
@@ -11627,7 +11641,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="29"/>
+      <c r="A83" s="32"/>
       <c r="B83" s="8">
         <v>2</v>
       </c>
@@ -11636,7 +11650,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
+      <c r="A84" s="32"/>
       <c r="B84" s="8">
         <v>3</v>
       </c>
@@ -11645,7 +11659,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
+      <c r="A85" s="24"/>
       <c r="B85" s="8">
         <v>4</v>
       </c>
@@ -11654,7 +11668,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="22" t="s">
+      <c r="A86" s="29" t="s">
         <v>210</v>
       </c>
       <c r="B86" s="8">
@@ -11665,7 +11679,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="23"/>
+      <c r="A87" s="30"/>
       <c r="B87" s="8">
         <v>2</v>
       </c>
@@ -11674,7 +11688,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="24"/>
+      <c r="A88" s="31"/>
       <c r="B88" s="8">
         <v>3</v>
       </c>
@@ -11683,7 +11697,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="29" t="s">
         <v>214</v>
       </c>
       <c r="B89" s="8">
@@ -11694,7 +11708,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="23"/>
+      <c r="A90" s="30"/>
       <c r="B90" s="8">
         <v>2</v>
       </c>
@@ -11703,7 +11717,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="24"/>
+      <c r="A91" s="31"/>
       <c r="B91" s="8">
         <v>3</v>
       </c>
@@ -11712,7 +11726,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="22" t="s">
+      <c r="A92" s="29" t="s">
         <v>216</v>
       </c>
       <c r="B92" s="8">
@@ -11723,7 +11737,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="23"/>
+      <c r="A93" s="30"/>
       <c r="B93" s="8">
         <v>2</v>
       </c>
@@ -11732,7 +11746,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="23"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="8">
         <v>3</v>
       </c>
@@ -11741,7 +11755,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="23"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="8">
         <v>4</v>
       </c>
@@ -11750,7 +11764,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="23"/>
+      <c r="A96" s="30"/>
       <c r="B96" s="8">
         <v>5</v>
       </c>
@@ -11759,7 +11773,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="24"/>
+      <c r="A97" s="31"/>
       <c r="B97" s="8">
         <v>6</v>
       </c>
@@ -11777,7 +11791,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="23" t="s">
+      <c r="A99" s="30" t="s">
         <v>218</v>
       </c>
       <c r="B99" s="8">
@@ -11788,7 +11802,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="23"/>
+      <c r="A100" s="30"/>
       <c r="B100" s="8">
         <v>3</v>
       </c>
@@ -11797,7 +11811,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="23"/>
+      <c r="A101" s="30"/>
       <c r="B101" s="8">
         <v>4</v>
       </c>
@@ -11806,7 +11820,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="23"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="8">
         <v>5</v>
       </c>
@@ -11815,7 +11829,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="23"/>
+      <c r="A103" s="30"/>
       <c r="B103" s="8">
         <v>6</v>
       </c>
@@ -11824,7 +11838,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="23"/>
+      <c r="A104" s="30"/>
       <c r="B104" s="8">
         <v>7</v>
       </c>
@@ -11833,7 +11847,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="23"/>
+      <c r="A105" s="30"/>
       <c r="B105" s="8">
         <v>8</v>
       </c>
@@ -11842,7 +11856,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="23"/>
+      <c r="A106" s="30"/>
       <c r="B106" s="8">
         <v>9</v>
       </c>
@@ -11851,7 +11865,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="23"/>
+      <c r="A107" s="30"/>
       <c r="B107" s="8">
         <v>10</v>
       </c>
@@ -11860,7 +11874,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="23"/>
+      <c r="A108" s="30"/>
       <c r="B108" s="8">
         <v>11</v>
       </c>
@@ -11869,7 +11883,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="23"/>
+      <c r="A109" s="30"/>
       <c r="B109" s="8">
         <v>12</v>
       </c>
@@ -11878,7 +11892,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="23"/>
+      <c r="A110" s="30"/>
       <c r="B110" s="8">
         <v>13</v>
       </c>
@@ -11887,7 +11901,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="23"/>
+      <c r="A111" s="30"/>
       <c r="B111" s="8">
         <v>14</v>
       </c>
@@ -11896,7 +11910,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="23"/>
+      <c r="A112" s="30"/>
       <c r="B112" s="8">
         <v>15</v>
       </c>
@@ -11905,7 +11919,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="24"/>
+      <c r="A113" s="31"/>
       <c r="B113" s="8">
         <v>16</v>
       </c>
@@ -11914,7 +11928,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="25" t="s">
+      <c r="A114" s="23" t="s">
         <v>228</v>
       </c>
       <c r="B114" s="8">
@@ -11925,7 +11939,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="26"/>
+      <c r="A115" s="24"/>
       <c r="B115" s="8">
         <v>2</v>
       </c>
@@ -11934,7 +11948,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="25" t="s">
+      <c r="A116" s="23" t="s">
         <v>232</v>
       </c>
       <c r="B116" s="8">
@@ -11945,7 +11959,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="29"/>
+      <c r="A117" s="32"/>
       <c r="B117" s="8">
         <v>2</v>
       </c>
@@ -11954,7 +11968,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="29"/>
+      <c r="A118" s="32"/>
       <c r="B118" s="8">
         <v>3</v>
       </c>
@@ -11963,7 +11977,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="26"/>
+      <c r="A119" s="24"/>
       <c r="B119" s="8">
         <v>4</v>
       </c>
@@ -11972,7 +11986,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="22" t="s">
+      <c r="A120" s="29" t="s">
         <v>234</v>
       </c>
       <c r="B120" s="8">
@@ -11983,7 +11997,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="23"/>
+      <c r="A121" s="30"/>
       <c r="B121" s="8">
         <v>2</v>
       </c>
@@ -11992,7 +12006,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="23"/>
+      <c r="A122" s="30"/>
       <c r="B122" s="8">
         <v>3</v>
       </c>
@@ -12001,7 +12015,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="23"/>
+      <c r="A123" s="30"/>
       <c r="B123" s="8">
         <v>4</v>
       </c>
@@ -12010,7 +12024,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="23"/>
+      <c r="A124" s="30"/>
       <c r="B124" s="8">
         <v>5</v>
       </c>
@@ -12019,7 +12033,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="23"/>
+      <c r="A125" s="30"/>
       <c r="B125" s="8">
         <v>6</v>
       </c>
@@ -12028,7 +12042,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="23"/>
+      <c r="A126" s="30"/>
       <c r="B126" s="8">
         <v>7</v>
       </c>
@@ -12037,7 +12051,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="23"/>
+      <c r="A127" s="30"/>
       <c r="B127" s="8">
         <v>8</v>
       </c>
@@ -12046,7 +12060,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="23"/>
+      <c r="A128" s="30"/>
       <c r="B128" s="8">
         <v>9</v>
       </c>
@@ -12055,7 +12069,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="23"/>
+      <c r="A129" s="30"/>
       <c r="B129" s="8">
         <v>10</v>
       </c>
@@ -12064,7 +12078,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="23"/>
+      <c r="A130" s="30"/>
       <c r="B130" s="8">
         <v>11</v>
       </c>
@@ -12073,7 +12087,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="23"/>
+      <c r="A131" s="30"/>
       <c r="B131" s="8">
         <v>12</v>
       </c>
@@ -12082,7 +12096,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="24"/>
+      <c r="A132" s="31"/>
       <c r="B132" s="8">
         <v>13</v>
       </c>
@@ -12091,7 +12105,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="25" t="s">
+      <c r="A133" s="23" t="s">
         <v>237</v>
       </c>
       <c r="B133" s="8">
@@ -12102,7 +12116,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="29"/>
+      <c r="A134" s="32"/>
       <c r="B134" s="8">
         <v>2</v>
       </c>
@@ -12111,7 +12125,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="29"/>
+      <c r="A135" s="32"/>
       <c r="B135" s="8">
         <v>3</v>
       </c>
@@ -12120,7 +12134,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="26"/>
+      <c r="A136" s="24"/>
       <c r="B136" s="8">
         <v>4</v>
       </c>
@@ -12130,6 +12144,36 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A82:A85"/>
     <mergeCell ref="A114:A115"/>
     <mergeCell ref="A116:A119"/>
     <mergeCell ref="A120:A132"/>
@@ -12139,36 +12183,6 @@
     <mergeCell ref="A92:A97"/>
     <mergeCell ref="A98:B98"/>
     <mergeCell ref="A99:A113"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12193,14 +12207,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>435</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
regression agefdv and info_tp
</commit_message>
<xml_diff>
--- a/data dictionary/DICC_A434_M3_NINOS.RID.xlsx
+++ b/data dictionary/DICC_A434_M3_NINOS.RID.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a5584703a9932d8/Documentos/RStudio/thesis/data dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{76951DC6-D1D1-4F7A-8241-5F94A5EAB1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E66E0E7-F92D-4B25-BCFB-8D885162E2C9}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{76951DC6-D1D1-4F7A-8241-5F94A5EAB1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD4F463F-5993-4C92-9929-2D49BF61F48A}"/>
   <bookViews>
-    <workbookView xWindow="28920" yWindow="0" windowWidth="17280" windowHeight="15585" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,12 @@
     <sheet name="Table 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="503">
   <si>
     <r>
       <rPr>
@@ -5660,6 +5661,9 @@
   </si>
   <si>
     <t>location</t>
+  </si>
+  <si>
+    <t>tp_info</t>
   </si>
 </sst>
 </file>
@@ -5958,78 +5962,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6044,6 +5976,78 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6351,8 +6355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6364,12 +6368,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -6591,16 +6595,16 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="22" t="s">
         <v>483</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B17" s="23">
         <v>40</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="25" t="s">
         <v>10</v>
       </c>
       <c r="F17" t="s">
@@ -7295,7 +7299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>112</v>
       </c>
@@ -7309,7 +7313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>114</v>
       </c>
@@ -7323,7 +7327,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>116</v>
       </c>
@@ -7337,7 +7341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>118</v>
       </c>
@@ -7351,7 +7355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>120</v>
       </c>
@@ -7365,7 +7369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>122</v>
       </c>
@@ -7379,7 +7383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>124</v>
       </c>
@@ -7393,21 +7397,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+    <row r="72" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="16">
         <v>95</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>128</v>
       </c>
@@ -7421,7 +7428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>130</v>
       </c>
@@ -7435,7 +7442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>132</v>
       </c>
@@ -7449,7 +7456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>134</v>
       </c>
@@ -7463,7 +7470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>136</v>
       </c>
@@ -7477,7 +7484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>138</v>
       </c>
@@ -7491,7 +7498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>140</v>
       </c>
@@ -7505,7 +7512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>142</v>
       </c>
@@ -8016,16 +8023,16 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="50" t="s">
+      <c r="A116" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="B116" s="47">
+      <c r="B116" s="23">
         <v>141</v>
       </c>
-      <c r="C116" s="49" t="s">
+      <c r="C116" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="D116" s="49" t="s">
+      <c r="D116" s="25" t="s">
         <v>10</v>
       </c>
       <c r="F116" t="s">
@@ -8282,25 +8289,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="41" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="43"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="31" t="s">
         <v>243</v>
       </c>
       <c r="B3" s="8">
@@ -8309,20 +8316,20 @@
       <c r="C3" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D3" s="28"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="D4" s="28"/>
+      <c r="D4" s="44"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>246</v>
       </c>
       <c r="B5" s="8">
@@ -8331,30 +8338,30 @@
       <c r="C5" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="8">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D6" s="28"/>
+      <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="8">
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="44"/>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="31" t="s">
         <v>250</v>
       </c>
       <c r="B8" s="8">
@@ -8363,20 +8370,20 @@
       <c r="C8" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="44"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="D9" s="28"/>
+      <c r="D9" s="44"/>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="8">
@@ -8385,20 +8392,20 @@
       <c r="C10" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="44"/>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="8">
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="8">
@@ -8407,30 +8414,30 @@
       <c r="C12" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="8">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="8">
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="44"/>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="8">
@@ -8439,20 +8446,20 @@
       <c r="C15" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="44"/>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="8">
         <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="44"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="8">
@@ -8463,7 +8470,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="8">
         <v>2</v>
       </c>
@@ -8472,7 +8479,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="8">
         <v>3</v>
       </c>
@@ -8481,7 +8488,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="8">
         <v>4</v>
       </c>
@@ -8490,7 +8497,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
@@ -8499,7 +8506,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="8">
         <v>6</v>
       </c>
@@ -8508,7 +8515,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="8">
@@ -8519,7 +8526,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -8528,7 +8535,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -8537,7 +8544,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="8">
         <v>4</v>
       </c>
@@ -8546,7 +8553,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="8">
         <v>5</v>
       </c>
@@ -8555,7 +8562,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="8">
         <v>6</v>
       </c>
@@ -8564,7 +8571,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="31" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="8">
@@ -8575,7 +8582,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="8">
         <v>2</v>
       </c>
@@ -8584,7 +8591,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="31" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="8">
@@ -8595,7 +8602,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="8">
         <v>2</v>
       </c>
@@ -8604,7 +8611,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="28" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="8">
@@ -8615,7 +8622,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="8">
         <v>8</v>
       </c>
@@ -8624,7 +8631,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="8">
         <v>9</v>
       </c>
@@ -8633,7 +8640,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="8">
         <v>11</v>
       </c>
@@ -8642,7 +8649,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="8">
         <v>12</v>
       </c>
@@ -8651,7 +8658,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="8">
         <v>13</v>
       </c>
@@ -8660,7 +8667,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B39" s="8">
@@ -8671,7 +8678,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="8">
         <v>2</v>
       </c>
@@ -8680,7 +8687,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="8">
         <v>3</v>
       </c>
@@ -8689,7 +8696,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="8">
         <v>4</v>
       </c>
@@ -8698,7 +8705,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="8">
         <v>5</v>
       </c>
@@ -8707,7 +8714,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="8">
         <v>6</v>
       </c>
@@ -8716,7 +8723,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="8">
         <v>7</v>
       </c>
@@ -8725,7 +8732,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="8">
         <v>8</v>
       </c>
@@ -8734,7 +8741,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="8">
         <v>9</v>
       </c>
@@ -8743,7 +8750,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="8">
         <v>10</v>
       </c>
@@ -8752,7 +8759,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="28" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="8">
@@ -8763,7 +8770,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="8">
         <v>2</v>
       </c>
@@ -8772,7 +8779,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
+      <c r="A51" s="29"/>
       <c r="B51" s="8">
         <v>3</v>
       </c>
@@ -8781,7 +8788,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="8">
         <v>4</v>
       </c>
@@ -8790,7 +8797,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="29"/>
       <c r="B53" s="8">
         <v>5</v>
       </c>
@@ -8799,7 +8806,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="31"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="8">
         <v>6</v>
       </c>
@@ -8808,7 +8815,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="28" t="s">
         <v>31</v>
       </c>
       <c r="B55" s="8">
@@ -8819,7 +8826,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
+      <c r="A56" s="29"/>
       <c r="B56" s="8">
         <v>2</v>
       </c>
@@ -8828,7 +8835,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="29"/>
       <c r="B57" s="8">
         <v>3</v>
       </c>
@@ -8837,7 +8844,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="30"/>
+      <c r="A58" s="29"/>
       <c r="B58" s="8">
         <v>4</v>
       </c>
@@ -8846,7 +8853,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="8">
         <v>5</v>
       </c>
@@ -8855,7 +8862,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+      <c r="A60" s="29"/>
       <c r="B60" s="8">
         <v>6</v>
       </c>
@@ -8864,7 +8871,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="29"/>
       <c r="B61" s="8">
         <v>7</v>
       </c>
@@ -8873,7 +8880,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="8">
         <v>8</v>
       </c>
@@ -8882,7 +8889,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="39"/>
+      <c r="A63" s="33"/>
       <c r="B63" s="8">
         <v>1</v>
       </c>
@@ -8891,7 +8898,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="37"/>
+      <c r="A64" s="34"/>
       <c r="B64" s="8">
         <v>2</v>
       </c>
@@ -8900,7 +8907,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="37"/>
+      <c r="A65" s="34"/>
       <c r="B65" s="8">
         <v>3</v>
       </c>
@@ -8909,7 +8916,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="30" t="s">
+      <c r="A66" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B66" s="8">
@@ -8920,7 +8927,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
+      <c r="A67" s="29"/>
       <c r="B67" s="8">
         <v>5</v>
       </c>
@@ -8929,7 +8936,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
+      <c r="A68" s="29"/>
       <c r="B68" s="8">
         <v>6</v>
       </c>
@@ -8938,7 +8945,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
+      <c r="A69" s="29"/>
       <c r="B69" s="8">
         <v>7</v>
       </c>
@@ -8947,7 +8954,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
+      <c r="A70" s="29"/>
       <c r="B70" s="8">
         <v>8</v>
       </c>
@@ -8956,7 +8963,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
+      <c r="A71" s="29"/>
       <c r="B71" s="8">
         <v>9</v>
       </c>
@@ -8965,7 +8972,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="29"/>
       <c r="B72" s="8">
         <v>10</v>
       </c>
@@ -8974,7 +8981,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="30"/>
+      <c r="A73" s="29"/>
       <c r="B73" s="8">
         <v>11</v>
       </c>
@@ -8983,7 +8990,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="29"/>
       <c r="B74" s="8">
         <v>12</v>
       </c>
@@ -8992,7 +8999,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
+      <c r="A75" s="29"/>
       <c r="B75" s="8">
         <v>13</v>
       </c>
@@ -9001,7 +9008,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="29"/>
       <c r="B76" s="8">
         <v>14</v>
       </c>
@@ -9010,7 +9017,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
+      <c r="A77" s="29"/>
       <c r="B77" s="8">
         <v>15</v>
       </c>
@@ -9019,7 +9026,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="30"/>
+      <c r="A78" s="29"/>
       <c r="B78" s="8">
         <v>16</v>
       </c>
@@ -9028,7 +9035,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="30"/>
+      <c r="A79" s="29"/>
       <c r="B79" s="8">
         <v>17</v>
       </c>
@@ -9037,7 +9044,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="31"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="8">
         <v>18</v>
       </c>
@@ -9046,7 +9053,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="23" t="s">
+      <c r="A81" s="31" t="s">
         <v>38</v>
       </c>
       <c r="B81" s="8">
@@ -9057,7 +9064,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="24"/>
+      <c r="A82" s="32"/>
       <c r="B82" s="8">
         <v>2</v>
       </c>
@@ -9066,7 +9073,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="29" t="s">
+      <c r="A83" s="28" t="s">
         <v>40</v>
       </c>
       <c r="B83" s="8">
@@ -9077,7 +9084,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="30"/>
+      <c r="A84" s="29"/>
       <c r="B84" s="8">
         <v>2</v>
       </c>
@@ -9086,7 +9093,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
+      <c r="A85" s="29"/>
       <c r="B85" s="8">
         <v>3</v>
       </c>
@@ -9095,7 +9102,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="30"/>
+      <c r="A86" s="29"/>
       <c r="B86" s="8">
         <v>4</v>
       </c>
@@ -9104,7 +9111,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
+      <c r="A87" s="29"/>
       <c r="B87" s="8">
         <v>5</v>
       </c>
@@ -9113,7 +9120,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+      <c r="A88" s="29"/>
       <c r="B88" s="8">
         <v>6</v>
       </c>
@@ -9122,7 +9129,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
+      <c r="A89" s="29"/>
       <c r="B89" s="8">
         <v>7</v>
       </c>
@@ -9131,7 +9138,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="8">
         <v>8</v>
       </c>
@@ -9140,7 +9147,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="30"/>
+      <c r="A91" s="29"/>
       <c r="B91" s="8">
         <v>9</v>
       </c>
@@ -9149,7 +9156,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="30"/>
+      <c r="A92" s="29"/>
       <c r="B92" s="8">
         <v>10</v>
       </c>
@@ -9158,7 +9165,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="8">
         <v>11</v>
       </c>
@@ -9167,7 +9174,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="8">
         <v>12</v>
       </c>
@@ -9176,7 +9183,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="8">
         <v>13</v>
       </c>
@@ -9185,7 +9192,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="30"/>
+      <c r="A96" s="29"/>
       <c r="B96" s="8">
         <v>14</v>
       </c>
@@ -9194,7 +9201,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
+      <c r="A97" s="29"/>
       <c r="B97" s="8">
         <v>15</v>
       </c>
@@ -9203,7 +9210,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="30"/>
+      <c r="A98" s="29"/>
       <c r="B98" s="8">
         <v>16</v>
       </c>
@@ -9212,7 +9219,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="31"/>
+      <c r="A99" s="30"/>
       <c r="B99" s="8">
         <v>18</v>
       </c>
@@ -9221,7 +9228,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="23" t="s">
+      <c r="A100" s="31" t="s">
         <v>44</v>
       </c>
       <c r="B100" s="8">
@@ -9232,7 +9239,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="32"/>
+      <c r="A101" s="35"/>
       <c r="B101" s="8">
         <v>2</v>
       </c>
@@ -9241,7 +9248,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="32"/>
+      <c r="A102" s="35"/>
       <c r="B102" s="8">
         <v>3</v>
       </c>
@@ -9250,7 +9257,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="24"/>
+      <c r="A103" s="32"/>
       <c r="B103" s="8">
         <v>4</v>
       </c>
@@ -9259,7 +9266,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="35" t="s">
+      <c r="A104" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B104" s="8">
@@ -9270,7 +9277,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="36"/>
+      <c r="A105" s="37"/>
       <c r="B105" s="8">
         <v>2</v>
       </c>
@@ -9279,7 +9286,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="36"/>
+      <c r="A106" s="37"/>
       <c r="B106" s="8">
         <v>3</v>
       </c>
@@ -9288,7 +9295,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="36"/>
+      <c r="A107" s="37"/>
       <c r="B107" s="8">
         <v>4</v>
       </c>
@@ -9297,7 +9304,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="36"/>
+      <c r="A108" s="37"/>
       <c r="B108" s="8">
         <v>5</v>
       </c>
@@ -9306,7 +9313,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="36"/>
+      <c r="A109" s="37"/>
       <c r="B109" s="8">
         <v>6</v>
       </c>
@@ -9315,7 +9322,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="36"/>
+      <c r="A110" s="37"/>
       <c r="B110" s="8">
         <v>7</v>
       </c>
@@ -9324,7 +9331,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="36"/>
+      <c r="A111" s="37"/>
       <c r="B111" s="8">
         <v>8</v>
       </c>
@@ -9333,7 +9340,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="36"/>
+      <c r="A112" s="37"/>
       <c r="B112" s="8">
         <v>9</v>
       </c>
@@ -9342,7 +9349,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="36"/>
+      <c r="A113" s="37"/>
       <c r="B113" s="8">
         <v>10</v>
       </c>
@@ -9351,7 +9358,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="36"/>
+      <c r="A114" s="37"/>
       <c r="B114" s="8">
         <v>11</v>
       </c>
@@ -9360,7 +9367,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="37"/>
+      <c r="A115" s="34"/>
       <c r="B115" s="8">
         <v>12</v>
       </c>
@@ -9369,7 +9376,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="37"/>
+      <c r="A116" s="34"/>
       <c r="B116" s="8">
         <v>13</v>
       </c>
@@ -9378,7 +9385,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="37"/>
+      <c r="A117" s="34"/>
       <c r="B117" s="8">
         <v>14</v>
       </c>
@@ -9387,7 +9394,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="37"/>
+      <c r="A118" s="34"/>
       <c r="B118" s="8">
         <v>15</v>
       </c>
@@ -9396,7 +9403,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="37"/>
+      <c r="A119" s="34"/>
       <c r="B119" s="8">
         <v>16</v>
       </c>
@@ -9414,7 +9421,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="29" t="s">
+      <c r="A121" s="28" t="s">
         <v>50</v>
       </c>
       <c r="B121" s="8">
@@ -9425,7 +9432,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="30"/>
+      <c r="A122" s="29"/>
       <c r="B122" s="8">
         <v>2</v>
       </c>
@@ -9434,7 +9441,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
+      <c r="A123" s="29"/>
       <c r="B123" s="8">
         <v>3</v>
       </c>
@@ -9443,7 +9450,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="30"/>
+      <c r="A124" s="29"/>
       <c r="B124" s="8">
         <v>4</v>
       </c>
@@ -9452,7 +9459,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="30"/>
+      <c r="A125" s="29"/>
       <c r="B125" s="8">
         <v>5</v>
       </c>
@@ -9461,7 +9468,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="30"/>
+      <c r="A126" s="29"/>
       <c r="B126" s="8">
         <v>6</v>
       </c>
@@ -9470,7 +9477,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="30"/>
+      <c r="A127" s="29"/>
       <c r="B127" s="8">
         <v>7</v>
       </c>
@@ -9479,7 +9486,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="31"/>
+      <c r="A128" s="30"/>
       <c r="B128" s="8">
         <v>8</v>
       </c>
@@ -9488,7 +9495,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="23" t="s">
+      <c r="A129" s="31" t="s">
         <v>51</v>
       </c>
       <c r="B129" s="8">
@@ -9499,7 +9506,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="24"/>
+      <c r="A130" s="32"/>
       <c r="B130" s="8">
         <v>1</v>
       </c>
@@ -9508,7 +9515,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="23" t="s">
+      <c r="A131" s="31" t="s">
         <v>53</v>
       </c>
       <c r="B131" s="8">
@@ -9519,7 +9526,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="24"/>
+      <c r="A132" s="32"/>
       <c r="B132" s="8">
         <v>1</v>
       </c>
@@ -9528,7 +9535,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="23" t="s">
+      <c r="A133" s="31" t="s">
         <v>55</v>
       </c>
       <c r="B133" s="8">
@@ -9539,7 +9546,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="24"/>
+      <c r="A134" s="32"/>
       <c r="B134" s="8">
         <v>1</v>
       </c>
@@ -9548,7 +9555,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="23" t="s">
+      <c r="A135" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B135" s="8">
@@ -9559,7 +9566,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="24"/>
+      <c r="A136" s="32"/>
       <c r="B136" s="8">
         <v>1</v>
       </c>
@@ -9568,7 +9575,7 @@
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="23" t="s">
+      <c r="A137" s="31" t="s">
         <v>59</v>
       </c>
       <c r="B137" s="8">
@@ -9579,7 +9586,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="24"/>
+      <c r="A138" s="32"/>
       <c r="B138" s="8">
         <v>1</v>
       </c>
@@ -9588,7 +9595,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="31" t="s">
         <v>61</v>
       </c>
       <c r="B139" s="8">
@@ -9599,7 +9606,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="24"/>
+      <c r="A140" s="32"/>
       <c r="B140" s="8">
         <v>1</v>
       </c>
@@ -9608,7 +9615,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="23" t="s">
+      <c r="A141" s="31" t="s">
         <v>63</v>
       </c>
       <c r="B141" s="8">
@@ -9619,7 +9626,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="24"/>
+      <c r="A142" s="32"/>
       <c r="B142" s="8">
         <v>1</v>
       </c>
@@ -9628,7 +9635,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="23" t="s">
+      <c r="A143" s="31" t="s">
         <v>65</v>
       </c>
       <c r="B143" s="8">
@@ -9639,7 +9646,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="32"/>
+      <c r="A144" s="35"/>
       <c r="B144" s="8">
         <v>2</v>
       </c>
@@ -9648,7 +9655,7 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="32"/>
+      <c r="A145" s="35"/>
       <c r="B145" s="8">
         <v>3</v>
       </c>
@@ -9657,7 +9664,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="24"/>
+      <c r="A146" s="32"/>
       <c r="B146" s="8">
         <v>4</v>
       </c>
@@ -9666,7 +9673,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="29" t="s">
+      <c r="A147" s="28" t="s">
         <v>66</v>
       </c>
       <c r="B147" s="8">
@@ -9677,7 +9684,7 @@
       </c>
     </row>
     <row r="148" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="30"/>
+      <c r="A148" s="29"/>
       <c r="B148" s="8">
         <v>2</v>
       </c>
@@ -9686,7 +9693,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="30"/>
+      <c r="A149" s="29"/>
       <c r="B149" s="8">
         <v>3</v>
       </c>
@@ -9695,7 +9702,7 @@
       </c>
     </row>
     <row r="150" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="30"/>
+      <c r="A150" s="29"/>
       <c r="B150" s="8">
         <v>4</v>
       </c>
@@ -9704,7 +9711,7 @@
       </c>
     </row>
     <row r="151" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="30"/>
+      <c r="A151" s="29"/>
       <c r="B151" s="8">
         <v>5</v>
       </c>
@@ -9713,7 +9720,7 @@
       </c>
     </row>
     <row r="152" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="31"/>
+      <c r="A152" s="30"/>
       <c r="B152" s="8">
         <v>6</v>
       </c>
@@ -9722,7 +9729,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="23" t="s">
+      <c r="A153" s="31" t="s">
         <v>68</v>
       </c>
       <c r="B153" s="8">
@@ -9733,7 +9740,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="24"/>
+      <c r="A154" s="32"/>
       <c r="B154" s="8">
         <v>2</v>
       </c>
@@ -9742,7 +9749,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="29" t="s">
+      <c r="A155" s="28" t="s">
         <v>70</v>
       </c>
       <c r="B155" s="8">
@@ -9753,7 +9760,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="30"/>
+      <c r="A156" s="29"/>
       <c r="B156" s="8">
         <v>2</v>
       </c>
@@ -9762,7 +9769,7 @@
       </c>
     </row>
     <row r="157" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="30"/>
+      <c r="A157" s="29"/>
       <c r="B157" s="8">
         <v>3</v>
       </c>
@@ -9771,7 +9778,7 @@
       </c>
     </row>
     <row r="158" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="30"/>
+      <c r="A158" s="29"/>
       <c r="B158" s="8">
         <v>4</v>
       </c>
@@ -9780,7 +9787,7 @@
       </c>
     </row>
     <row r="159" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="30"/>
+      <c r="A159" s="29"/>
       <c r="B159" s="8">
         <v>5</v>
       </c>
@@ -9789,7 +9796,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="30"/>
+      <c r="A160" s="29"/>
       <c r="B160" s="8">
         <v>6</v>
       </c>
@@ -9798,7 +9805,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="30"/>
+      <c r="A161" s="29"/>
       <c r="B161" s="8">
         <v>7</v>
       </c>
@@ -9807,7 +9814,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="31"/>
+      <c r="A162" s="30"/>
       <c r="B162" s="8">
         <v>8</v>
       </c>
@@ -9816,16 +9823,16 @@
       </c>
     </row>
     <row r="163" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="33">
+      <c r="A163" s="39">
         <v>1</v>
       </c>
-      <c r="B163" s="34"/>
+      <c r="B163" s="40"/>
       <c r="C163" s="7" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="32" t="s">
+      <c r="A164" s="35" t="s">
         <v>73</v>
       </c>
       <c r="B164" s="8">
@@ -9836,7 +9843,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="24"/>
+      <c r="A165" s="32"/>
       <c r="B165" s="8">
         <v>3</v>
       </c>
@@ -9845,7 +9852,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="23" t="s">
+      <c r="A166" s="31" t="s">
         <v>74</v>
       </c>
       <c r="B166" s="8">
@@ -9856,7 +9863,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="24"/>
+      <c r="A167" s="32"/>
       <c r="B167" s="8">
         <v>2</v>
       </c>
@@ -9865,7 +9872,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="23" t="s">
+      <c r="A168" s="31" t="s">
         <v>75</v>
       </c>
       <c r="B168" s="8">
@@ -9876,7 +9883,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="32"/>
+      <c r="A169" s="35"/>
       <c r="B169" s="8">
         <v>2</v>
       </c>
@@ -9885,7 +9892,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="32"/>
+      <c r="A170" s="35"/>
       <c r="B170" s="8">
         <v>3</v>
       </c>
@@ -9894,7 +9901,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="24"/>
+      <c r="A171" s="32"/>
       <c r="B171" s="8">
         <v>4</v>
       </c>
@@ -9903,7 +9910,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="29" t="s">
+      <c r="A172" s="28" t="s">
         <v>76</v>
       </c>
       <c r="B172" s="8">
@@ -9914,7 +9921,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="30"/>
+      <c r="A173" s="29"/>
       <c r="B173" s="8">
         <v>2</v>
       </c>
@@ -9923,7 +9930,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="31"/>
+      <c r="A174" s="30"/>
       <c r="B174" s="8">
         <v>3</v>
       </c>
@@ -9932,7 +9939,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="23" t="s">
+      <c r="A175" s="31" t="s">
         <v>78</v>
       </c>
       <c r="B175" s="8">
@@ -9943,7 +9950,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="32"/>
+      <c r="A176" s="35"/>
       <c r="B176" s="8">
         <v>2</v>
       </c>
@@ -9952,7 +9959,7 @@
       </c>
     </row>
     <row r="177" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="32"/>
+      <c r="A177" s="35"/>
       <c r="B177" s="8">
         <v>3</v>
       </c>
@@ -9961,7 +9968,7 @@
       </c>
     </row>
     <row r="178" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="24"/>
+      <c r="A178" s="32"/>
       <c r="B178" s="8">
         <v>4</v>
       </c>
@@ -9970,7 +9977,7 @@
       </c>
     </row>
     <row r="179" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="29" t="s">
+      <c r="A179" s="28" t="s">
         <v>79</v>
       </c>
       <c r="B179" s="8">
@@ -9981,7 +9988,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="30"/>
+      <c r="A180" s="29"/>
       <c r="B180" s="8">
         <v>2</v>
       </c>
@@ -9990,7 +9997,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="31"/>
+      <c r="A181" s="30"/>
       <c r="B181" s="8">
         <v>3</v>
       </c>
@@ -9999,7 +10006,7 @@
       </c>
     </row>
     <row r="182" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="29" t="s">
+      <c r="A182" s="28" t="s">
         <v>80</v>
       </c>
       <c r="B182" s="8">
@@ -10010,7 +10017,7 @@
       </c>
     </row>
     <row r="183" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="30"/>
+      <c r="A183" s="29"/>
       <c r="B183" s="8">
         <v>2</v>
       </c>
@@ -10019,7 +10026,7 @@
       </c>
     </row>
     <row r="184" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="30"/>
+      <c r="A184" s="29"/>
       <c r="B184" s="8">
         <v>3</v>
       </c>
@@ -10028,7 +10035,7 @@
       </c>
     </row>
     <row r="185" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="30"/>
+      <c r="A185" s="29"/>
       <c r="B185" s="8">
         <v>4</v>
       </c>
@@ -10037,7 +10044,7 @@
       </c>
     </row>
     <row r="186" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="31"/>
+      <c r="A186" s="30"/>
       <c r="B186" s="8">
         <v>5</v>
       </c>
@@ -10046,7 +10053,7 @@
       </c>
     </row>
     <row r="187" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="23" t="s">
+      <c r="A187" s="31" t="s">
         <v>84</v>
       </c>
       <c r="B187" s="8">
@@ -10057,7 +10064,7 @@
       </c>
     </row>
     <row r="188" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="24"/>
+      <c r="A188" s="32"/>
       <c r="B188" s="8">
         <v>1</v>
       </c>
@@ -10066,7 +10073,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="23" t="s">
+      <c r="A189" s="31" t="s">
         <v>86</v>
       </c>
       <c r="B189" s="8">
@@ -10077,7 +10084,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="24"/>
+      <c r="A190" s="32"/>
       <c r="B190" s="8">
         <v>1</v>
       </c>
@@ -10086,7 +10093,7 @@
       </c>
     </row>
     <row r="191" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="23" t="s">
+      <c r="A191" s="31" t="s">
         <v>88</v>
       </c>
       <c r="B191" s="8">
@@ -10097,7 +10104,7 @@
       </c>
     </row>
     <row r="192" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="24"/>
+      <c r="A192" s="32"/>
       <c r="B192" s="8">
         <v>1</v>
       </c>
@@ -10106,7 +10113,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="23" t="s">
+      <c r="A193" s="31" t="s">
         <v>90</v>
       </c>
       <c r="B193" s="8">
@@ -10117,7 +10124,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="24"/>
+      <c r="A194" s="32"/>
       <c r="B194" s="8">
         <v>1</v>
       </c>
@@ -10126,7 +10133,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="23" t="s">
+      <c r="A195" s="31" t="s">
         <v>92</v>
       </c>
       <c r="B195" s="8">
@@ -10137,7 +10144,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="24"/>
+      <c r="A196" s="32"/>
       <c r="B196" s="8">
         <v>1</v>
       </c>
@@ -10146,7 +10153,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A197" s="23" t="s">
+      <c r="A197" s="31" t="s">
         <v>94</v>
       </c>
       <c r="B197" s="8">
@@ -10157,7 +10164,7 @@
       </c>
     </row>
     <row r="198" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A198" s="24"/>
+      <c r="A198" s="32"/>
       <c r="B198" s="8">
         <v>1</v>
       </c>
@@ -10166,7 +10173,7 @@
       </c>
     </row>
     <row r="199" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A199" s="23" t="s">
+      <c r="A199" s="31" t="s">
         <v>96</v>
       </c>
       <c r="B199" s="8">
@@ -10177,7 +10184,7 @@
       </c>
     </row>
     <row r="200" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A200" s="24"/>
+      <c r="A200" s="32"/>
       <c r="B200" s="8">
         <v>1</v>
       </c>
@@ -10186,7 +10193,7 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A201" s="23" t="s">
+      <c r="A201" s="31" t="s">
         <v>98</v>
       </c>
       <c r="B201" s="8">
@@ -10197,7 +10204,7 @@
       </c>
     </row>
     <row r="202" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A202" s="24"/>
+      <c r="A202" s="32"/>
       <c r="B202" s="8">
         <v>1</v>
       </c>
@@ -10206,7 +10213,7 @@
       </c>
     </row>
     <row r="203" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A203" s="23" t="s">
+      <c r="A203" s="31" t="s">
         <v>100</v>
       </c>
       <c r="B203" s="8">
@@ -10217,7 +10224,7 @@
       </c>
     </row>
     <row r="204" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A204" s="24"/>
+      <c r="A204" s="32"/>
       <c r="B204" s="8">
         <v>1</v>
       </c>
@@ -10226,7 +10233,7 @@
       </c>
     </row>
     <row r="205" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A205" s="23" t="s">
+      <c r="A205" s="31" t="s">
         <v>102</v>
       </c>
       <c r="B205" s="8">
@@ -10237,7 +10244,7 @@
       </c>
     </row>
     <row r="206" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A206" s="24"/>
+      <c r="A206" s="32"/>
       <c r="B206" s="8">
         <v>1</v>
       </c>
@@ -10246,7 +10253,7 @@
       </c>
     </row>
     <row r="207" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A207" s="23" t="s">
+      <c r="A207" s="31" t="s">
         <v>104</v>
       </c>
       <c r="B207" s="8">
@@ -10257,7 +10264,7 @@
       </c>
     </row>
     <row r="208" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A208" s="24"/>
+      <c r="A208" s="32"/>
       <c r="B208" s="8">
         <v>1</v>
       </c>
@@ -10266,7 +10273,7 @@
       </c>
     </row>
     <row r="209" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A209" s="23" t="s">
+      <c r="A209" s="31" t="s">
         <v>106</v>
       </c>
       <c r="B209" s="8">
@@ -10277,7 +10284,7 @@
       </c>
     </row>
     <row r="210" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A210" s="24"/>
+      <c r="A210" s="32"/>
       <c r="B210" s="8">
         <v>1</v>
       </c>
@@ -10286,7 +10293,7 @@
       </c>
     </row>
     <row r="211" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A211" s="23" t="s">
+      <c r="A211" s="31" t="s">
         <v>108</v>
       </c>
       <c r="B211" s="8">
@@ -10297,7 +10304,7 @@
       </c>
     </row>
     <row r="212" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A212" s="24"/>
+      <c r="A212" s="32"/>
       <c r="B212" s="8">
         <v>1</v>
       </c>
@@ -10307,47 +10314,6 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A39:A48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="A55:A62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A99"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="A104:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A128"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="A133:A134"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A146"/>
-    <mergeCell ref="A147:A152"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="A155:A162"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="A168:A171"/>
-    <mergeCell ref="A172:A174"/>
-    <mergeCell ref="A175:A178"/>
-    <mergeCell ref="A179:A181"/>
-    <mergeCell ref="A182:A186"/>
-    <mergeCell ref="A205:A206"/>
-    <mergeCell ref="A187:A188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="A193:A194"/>
-    <mergeCell ref="A195:A196"/>
     <mergeCell ref="A207:A208"/>
     <mergeCell ref="A209:A210"/>
     <mergeCell ref="A211:A212"/>
@@ -10364,6 +10330,47 @@
     <mergeCell ref="A199:A200"/>
     <mergeCell ref="A201:A202"/>
     <mergeCell ref="A203:A204"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A187:A188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="A193:A194"/>
+    <mergeCell ref="A195:A196"/>
+    <mergeCell ref="A168:A171"/>
+    <mergeCell ref="A172:A174"/>
+    <mergeCell ref="A175:A178"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A182:A186"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="A155:A162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A146"/>
+    <mergeCell ref="A147:A152"/>
+    <mergeCell ref="A121:A128"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="A133:A134"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A39:A48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A55:A62"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A80"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10385,7 +10392,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>110</v>
       </c>
       <c r="B1" s="8">
@@ -10396,7 +10403,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="8">
         <v>92</v>
       </c>
@@ -10405,7 +10412,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="8">
@@ -10416,7 +10423,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -10425,7 +10432,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="8">
         <v>3</v>
       </c>
@@ -10434,7 +10441,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="31" t="s">
         <v>112</v>
       </c>
       <c r="B6" s="8">
@@ -10445,7 +10452,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="8">
         <v>1</v>
       </c>
@@ -10454,7 +10461,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="31" t="s">
         <v>114</v>
       </c>
       <c r="B8" s="8">
@@ -10465,7 +10472,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="8">
         <v>1</v>
       </c>
@@ -10474,7 +10481,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="31" t="s">
         <v>116</v>
       </c>
       <c r="B10" s="8">
@@ -10485,7 +10492,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="8">
         <v>1</v>
       </c>
@@ -10494,7 +10501,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="31" t="s">
         <v>118</v>
       </c>
       <c r="B12" s="8">
@@ -10505,7 +10512,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="8">
         <v>1</v>
       </c>
@@ -10514,7 +10521,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="31" t="s">
         <v>120</v>
       </c>
       <c r="B14" s="8">
@@ -10525,7 +10532,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="8">
         <v>1</v>
       </c>
@@ -10534,7 +10541,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="31" t="s">
         <v>122</v>
       </c>
       <c r="B16" s="8">
@@ -10545,7 +10552,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="8">
         <v>2</v>
       </c>
@@ -10554,7 +10561,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="31" t="s">
         <v>124</v>
       </c>
       <c r="B18" s="8">
@@ -10565,7 +10572,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="8">
         <v>92</v>
       </c>
@@ -10574,7 +10581,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>126</v>
       </c>
       <c r="B20" s="8">
@@ -10585,7 +10592,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="8">
         <v>2</v>
       </c>
@@ -10594,7 +10601,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="8">
         <v>3</v>
       </c>
@@ -10603,7 +10610,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="28" t="s">
         <v>128</v>
       </c>
       <c r="B23" s="8">
@@ -10614,7 +10621,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -10623,7 +10630,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -10632,7 +10639,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="31" t="s">
         <v>372</v>
       </c>
       <c r="B26" s="8">
@@ -10643,7 +10650,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="8">
         <v>2</v>
       </c>
@@ -10652,7 +10659,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="31" t="s">
         <v>130</v>
       </c>
       <c r="B28" s="8">
@@ -10663,7 +10670,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="8">
         <v>1</v>
       </c>
@@ -10672,7 +10679,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="31" t="s">
         <v>132</v>
       </c>
       <c r="B30" s="8">
@@ -10683,7 +10690,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="8">
         <v>1</v>
       </c>
@@ -10692,7 +10699,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="31" t="s">
         <v>134</v>
       </c>
       <c r="B32" s="8">
@@ -10703,7 +10710,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="8">
         <v>1</v>
       </c>
@@ -10712,7 +10719,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="31" t="s">
         <v>136</v>
       </c>
       <c r="B34" s="8">
@@ -10723,7 +10730,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="8">
         <v>1</v>
       </c>
@@ -10732,7 +10739,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="31" t="s">
         <v>138</v>
       </c>
       <c r="B36" s="8">
@@ -10743,7 +10750,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
+      <c r="A37" s="32"/>
       <c r="B37" s="8">
         <v>1</v>
       </c>
@@ -10752,7 +10759,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="31" t="s">
         <v>140</v>
       </c>
       <c r="B38" s="8">
@@ -10763,7 +10770,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="8">
         <v>1</v>
       </c>
@@ -10772,7 +10779,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="31" t="s">
         <v>142</v>
       </c>
       <c r="B40" s="8">
@@ -10783,7 +10790,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="8">
         <v>1</v>
       </c>
@@ -10792,7 +10799,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="31" t="s">
         <v>373</v>
       </c>
       <c r="B42" s="8">
@@ -10803,7 +10810,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="8">
         <v>2</v>
       </c>
@@ -10812,7 +10819,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="31" t="s">
         <v>146</v>
       </c>
       <c r="B44" s="8">
@@ -10823,7 +10830,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="8">
         <v>2</v>
       </c>
@@ -10832,7 +10839,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="8">
         <v>3</v>
       </c>
@@ -10841,7 +10848,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="8">
         <v>4</v>
       </c>
@@ -10850,7 +10857,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="28" t="s">
         <v>148</v>
       </c>
       <c r="B48" s="8">
@@ -10861,7 +10868,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="8">
         <v>2</v>
       </c>
@@ -10870,27 +10877,12 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="40"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
+      <c r="A50" s="45"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:C50"/>
@@ -10899,6 +10891,21 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10908,7 +10915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+    <sheetView topLeftCell="A104" workbookViewId="0">
       <selection activeCell="C89" sqref="C89:C91"/>
     </sheetView>
   </sheetViews>
@@ -10920,7 +10927,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43"/>
+      <c r="A1" s="46"/>
       <c r="B1" s="8">
         <v>3</v>
       </c>
@@ -10929,7 +10936,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
+      <c r="A2" s="47"/>
       <c r="B2" s="8">
         <v>4</v>
       </c>
@@ -10938,7 +10945,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="31" t="s">
         <v>150</v>
       </c>
       <c r="B3" s="8">
@@ -10949,7 +10956,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="8">
         <v>92</v>
       </c>
@@ -10958,7 +10965,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="31" t="s">
         <v>151</v>
       </c>
       <c r="B5" s="8">
@@ -10969,7 +10976,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="8">
         <v>2</v>
       </c>
@@ -10978,7 +10985,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="31" t="s">
         <v>152</v>
       </c>
       <c r="B7" s="8">
@@ -10989,7 +10996,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="8">
         <v>92</v>
       </c>
@@ -10998,7 +11005,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="31" t="s">
         <v>156</v>
       </c>
       <c r="B9" s="8">
@@ -11009,7 +11016,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="8">
         <v>1</v>
       </c>
@@ -11018,7 +11025,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>158</v>
       </c>
       <c r="B11" s="8">
@@ -11029,7 +11036,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="8">
         <v>1</v>
       </c>
@@ -11038,7 +11045,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="31" t="s">
         <v>160</v>
       </c>
       <c r="B13" s="8">
@@ -11049,7 +11056,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="8">
         <v>1</v>
       </c>
@@ -11058,7 +11065,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="31" t="s">
         <v>162</v>
       </c>
       <c r="B15" s="8">
@@ -11069,7 +11076,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="8">
         <v>1</v>
       </c>
@@ -11078,7 +11085,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="31" t="s">
         <v>164</v>
       </c>
       <c r="B17" s="8">
@@ -11089,7 +11096,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="8">
         <v>1</v>
       </c>
@@ -11098,7 +11105,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="31" t="s">
         <v>166</v>
       </c>
       <c r="B19" s="8">
@@ -11109,7 +11116,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="8">
         <v>1</v>
       </c>
@@ -11118,7 +11125,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="31" t="s">
         <v>168</v>
       </c>
       <c r="B21" s="8">
@@ -11129,7 +11136,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="8">
         <v>1</v>
       </c>
@@ -11138,7 +11145,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="28" t="s">
         <v>172</v>
       </c>
       <c r="B23" s="8">
@@ -11149,7 +11156,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -11158,7 +11165,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -11167,7 +11174,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="31" t="s">
         <v>174</v>
       </c>
       <c r="B26" s="8">
@@ -11178,7 +11185,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="8">
         <v>2</v>
       </c>
@@ -11187,7 +11194,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="8">
         <v>3</v>
       </c>
@@ -11196,7 +11203,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="8">
         <v>4</v>
       </c>
@@ -11205,7 +11212,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>176</v>
       </c>
       <c r="B30" s="8">
@@ -11216,7 +11223,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="8">
         <v>2</v>
       </c>
@@ -11225,7 +11232,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="8">
         <v>3</v>
       </c>
@@ -11234,7 +11241,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="31" t="s">
         <v>178</v>
       </c>
       <c r="B33" s="8">
@@ -11245,7 +11252,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="8">
         <v>2</v>
       </c>
@@ -11254,7 +11261,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="8">
         <v>3</v>
       </c>
@@ -11263,7 +11270,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="8">
         <v>4</v>
       </c>
@@ -11272,7 +11279,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="28" t="s">
         <v>180</v>
       </c>
       <c r="B37" s="8">
@@ -11283,7 +11290,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="8">
         <v>2</v>
       </c>
@@ -11292,7 +11299,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="8">
         <v>3</v>
       </c>
@@ -11301,7 +11308,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="31" t="s">
         <v>182</v>
       </c>
       <c r="B40" s="8">
@@ -11312,7 +11319,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="35"/>
       <c r="B41" s="8">
         <v>2</v>
       </c>
@@ -11321,7 +11328,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="8">
         <v>3</v>
       </c>
@@ -11330,7 +11337,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="8">
         <v>4</v>
       </c>
@@ -11339,7 +11346,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="28" t="s">
         <v>184</v>
       </c>
       <c r="B44" s="8">
@@ -11350,7 +11357,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="8">
         <v>2</v>
       </c>
@@ -11359,7 +11366,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="8">
         <v>3</v>
       </c>
@@ -11368,7 +11375,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="28" t="s">
         <v>186</v>
       </c>
       <c r="B47" s="8">
@@ -11379,7 +11386,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="8">
         <v>2</v>
       </c>
@@ -11388,7 +11395,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="8">
         <v>3</v>
       </c>
@@ -11397,16 +11404,16 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="41">
+      <c r="A50" s="48">
         <v>4</v>
       </c>
-      <c r="B50" s="42"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="7" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="28" t="s">
         <v>188</v>
       </c>
       <c r="B51" s="8">
@@ -11417,7 +11424,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="8">
         <v>2</v>
       </c>
@@ -11426,7 +11433,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="8">
         <v>3</v>
       </c>
@@ -11435,7 +11442,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="31" t="s">
         <v>190</v>
       </c>
       <c r="B54" s="8">
@@ -11446,7 +11453,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="32"/>
+      <c r="A55" s="35"/>
       <c r="B55" s="8">
         <v>2</v>
       </c>
@@ -11455,7 +11462,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="32"/>
+      <c r="A56" s="35"/>
       <c r="B56" s="8">
         <v>3</v>
       </c>
@@ -11464,7 +11471,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="24"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="8">
         <v>4</v>
       </c>
@@ -11473,7 +11480,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="29" t="s">
+      <c r="A58" s="28" t="s">
         <v>192</v>
       </c>
       <c r="B58" s="8">
@@ -11484,7 +11491,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="8">
         <v>2</v>
       </c>
@@ -11493,7 +11500,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="31"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="8">
         <v>3</v>
       </c>
@@ -11502,7 +11509,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="31" t="s">
         <v>194</v>
       </c>
       <c r="B61" s="8">
@@ -11513,7 +11520,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="32"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="8">
         <v>2</v>
       </c>
@@ -11522,7 +11529,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="32"/>
+      <c r="A63" s="35"/>
       <c r="B63" s="8">
         <v>3</v>
       </c>
@@ -11531,7 +11538,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="24"/>
+      <c r="A64" s="32"/>
       <c r="B64" s="8">
         <v>4</v>
       </c>
@@ -11540,7 +11547,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="29" t="s">
+      <c r="A65" s="28" t="s">
         <v>196</v>
       </c>
       <c r="B65" s="8">
@@ -11551,7 +11558,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
+      <c r="A66" s="29"/>
       <c r="B66" s="8">
         <v>2</v>
       </c>
@@ -11560,7 +11567,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="31"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="8">
         <v>3</v>
       </c>
@@ -11569,7 +11576,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="31" t="s">
         <v>198</v>
       </c>
       <c r="B68" s="8">
@@ -11580,7 +11587,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="32"/>
+      <c r="A69" s="35"/>
       <c r="B69" s="8">
         <v>2</v>
       </c>
@@ -11589,7 +11596,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="32"/>
+      <c r="A70" s="35"/>
       <c r="B70" s="8">
         <v>3</v>
       </c>
@@ -11598,7 +11605,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="24"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="8">
         <v>4</v>
       </c>
@@ -11607,7 +11614,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="29" t="s">
+      <c r="A72" s="28" t="s">
         <v>200</v>
       </c>
       <c r="B72" s="8">
@@ -11618,7 +11625,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="30"/>
+      <c r="A73" s="29"/>
       <c r="B73" s="8">
         <v>2</v>
       </c>
@@ -11627,7 +11634,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="8">
         <v>3</v>
       </c>
@@ -11636,7 +11643,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="31" t="s">
         <v>202</v>
       </c>
       <c r="B75" s="8">
@@ -11647,7 +11654,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="32"/>
+      <c r="A76" s="35"/>
       <c r="B76" s="8">
         <v>2</v>
       </c>
@@ -11656,7 +11663,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
+      <c r="A77" s="35"/>
       <c r="B77" s="8">
         <v>3</v>
       </c>
@@ -11665,7 +11672,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="24"/>
+      <c r="A78" s="32"/>
       <c r="B78" s="8">
         <v>4</v>
       </c>
@@ -11674,7 +11681,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="29" t="s">
+      <c r="A79" s="28" t="s">
         <v>204</v>
       </c>
       <c r="B79" s="8">
@@ -11685,7 +11692,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
+      <c r="A80" s="29"/>
       <c r="B80" s="8">
         <v>2</v>
       </c>
@@ -11694,7 +11701,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="31"/>
+      <c r="A81" s="30"/>
       <c r="B81" s="8">
         <v>3</v>
       </c>
@@ -11703,7 +11710,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="23" t="s">
+      <c r="A82" s="31" t="s">
         <v>206</v>
       </c>
       <c r="B82" s="8">
@@ -11714,7 +11721,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="32"/>
+      <c r="A83" s="35"/>
       <c r="B83" s="8">
         <v>2</v>
       </c>
@@ -11723,7 +11730,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="32"/>
+      <c r="A84" s="35"/>
       <c r="B84" s="8">
         <v>3</v>
       </c>
@@ -11732,7 +11739,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="24"/>
+      <c r="A85" s="32"/>
       <c r="B85" s="8">
         <v>4</v>
       </c>
@@ -11741,7 +11748,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="29" t="s">
+      <c r="A86" s="28" t="s">
         <v>208</v>
       </c>
       <c r="B86" s="8">
@@ -11752,7 +11759,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
+      <c r="A87" s="29"/>
       <c r="B87" s="8">
         <v>2</v>
       </c>
@@ -11761,7 +11768,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
+      <c r="A88" s="30"/>
       <c r="B88" s="8">
         <v>3</v>
       </c>
@@ -11770,7 +11777,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="29" t="s">
+      <c r="A89" s="28" t="s">
         <v>212</v>
       </c>
       <c r="B89" s="8">
@@ -11781,7 +11788,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="8">
         <v>2</v>
       </c>
@@ -11790,7 +11797,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="31"/>
+      <c r="A91" s="30"/>
       <c r="B91" s="8">
         <v>3</v>
       </c>
@@ -11799,7 +11806,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="29" t="s">
+      <c r="A92" s="28" t="s">
         <v>214</v>
       </c>
       <c r="B92" s="8">
@@ -11810,7 +11817,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="8">
         <v>2</v>
       </c>
@@ -11819,7 +11826,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="8">
         <v>3</v>
       </c>
@@ -11828,7 +11835,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="8">
         <v>4</v>
       </c>
@@ -11837,7 +11844,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="30"/>
+      <c r="A96" s="29"/>
       <c r="B96" s="8">
         <v>5</v>
       </c>
@@ -11846,7 +11853,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="31"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="8">
         <v>6</v>
       </c>
@@ -11855,16 +11862,16 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="33">
+      <c r="A98" s="39">
         <v>1</v>
       </c>
-      <c r="B98" s="34"/>
+      <c r="B98" s="40"/>
       <c r="C98" s="7" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="30" t="s">
+      <c r="A99" s="29" t="s">
         <v>216</v>
       </c>
       <c r="B99" s="8">
@@ -11875,7 +11882,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
+      <c r="A100" s="29"/>
       <c r="B100" s="8">
         <v>3</v>
       </c>
@@ -11884,7 +11891,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
+      <c r="A101" s="29"/>
       <c r="B101" s="8">
         <v>4</v>
       </c>
@@ -11893,7 +11900,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
+      <c r="A102" s="29"/>
       <c r="B102" s="8">
         <v>5</v>
       </c>
@@ -11902,7 +11909,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="30"/>
+      <c r="A103" s="29"/>
       <c r="B103" s="8">
         <v>6</v>
       </c>
@@ -11911,7 +11918,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="30"/>
+      <c r="A104" s="29"/>
       <c r="B104" s="8">
         <v>7</v>
       </c>
@@ -11920,7 +11927,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="30"/>
+      <c r="A105" s="29"/>
       <c r="B105" s="8">
         <v>8</v>
       </c>
@@ -11929,7 +11936,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
+      <c r="A106" s="29"/>
       <c r="B106" s="8">
         <v>9</v>
       </c>
@@ -11938,7 +11945,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="30"/>
+      <c r="A107" s="29"/>
       <c r="B107" s="8">
         <v>10</v>
       </c>
@@ -11947,7 +11954,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="30"/>
+      <c r="A108" s="29"/>
       <c r="B108" s="8">
         <v>11</v>
       </c>
@@ -11956,7 +11963,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="30"/>
+      <c r="A109" s="29"/>
       <c r="B109" s="8">
         <v>12</v>
       </c>
@@ -11965,7 +11972,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="30"/>
+      <c r="A110" s="29"/>
       <c r="B110" s="8">
         <v>13</v>
       </c>
@@ -11974,7 +11981,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="30"/>
+      <c r="A111" s="29"/>
       <c r="B111" s="8">
         <v>14</v>
       </c>
@@ -11983,7 +11990,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
+      <c r="A112" s="29"/>
       <c r="B112" s="8">
         <v>15</v>
       </c>
@@ -11992,7 +11999,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
+      <c r="A113" s="30"/>
       <c r="B113" s="8">
         <v>16</v>
       </c>
@@ -12001,7 +12008,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="23" t="s">
+      <c r="A114" s="31" t="s">
         <v>226</v>
       </c>
       <c r="B114" s="8">
@@ -12012,7 +12019,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="24"/>
+      <c r="A115" s="32"/>
       <c r="B115" s="8">
         <v>2</v>
       </c>
@@ -12021,7 +12028,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="23" t="s">
+      <c r="A116" s="31" t="s">
         <v>230</v>
       </c>
       <c r="B116" s="8">
@@ -12032,7 +12039,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="32"/>
+      <c r="A117" s="35"/>
       <c r="B117" s="8">
         <v>2</v>
       </c>
@@ -12041,7 +12048,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="32"/>
+      <c r="A118" s="35"/>
       <c r="B118" s="8">
         <v>3</v>
       </c>
@@ -12050,7 +12057,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="24"/>
+      <c r="A119" s="32"/>
       <c r="B119" s="8">
         <v>4</v>
       </c>
@@ -12059,7 +12066,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="29" t="s">
+      <c r="A120" s="28" t="s">
         <v>232</v>
       </c>
       <c r="B120" s="8">
@@ -12070,7 +12077,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="30"/>
+      <c r="A121" s="29"/>
       <c r="B121" s="8">
         <v>2</v>
       </c>
@@ -12079,7 +12086,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="30"/>
+      <c r="A122" s="29"/>
       <c r="B122" s="8">
         <v>3</v>
       </c>
@@ -12088,7 +12095,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
+      <c r="A123" s="29"/>
       <c r="B123" s="8">
         <v>4</v>
       </c>
@@ -12097,7 +12104,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="30"/>
+      <c r="A124" s="29"/>
       <c r="B124" s="8">
         <v>5</v>
       </c>
@@ -12106,7 +12113,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="30"/>
+      <c r="A125" s="29"/>
       <c r="B125" s="8">
         <v>6</v>
       </c>
@@ -12115,7 +12122,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="30"/>
+      <c r="A126" s="29"/>
       <c r="B126" s="8">
         <v>7</v>
       </c>
@@ -12124,7 +12131,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="30"/>
+      <c r="A127" s="29"/>
       <c r="B127" s="8">
         <v>8</v>
       </c>
@@ -12133,7 +12140,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="30"/>
+      <c r="A128" s="29"/>
       <c r="B128" s="8">
         <v>9</v>
       </c>
@@ -12142,7 +12149,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="30"/>
+      <c r="A129" s="29"/>
       <c r="B129" s="8">
         <v>10</v>
       </c>
@@ -12151,7 +12158,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="30"/>
+      <c r="A130" s="29"/>
       <c r="B130" s="8">
         <v>11</v>
       </c>
@@ -12160,7 +12167,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="30"/>
+      <c r="A131" s="29"/>
       <c r="B131" s="8">
         <v>12</v>
       </c>
@@ -12169,7 +12176,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="31"/>
+      <c r="A132" s="30"/>
       <c r="B132" s="8">
         <v>13</v>
       </c>
@@ -12178,7 +12185,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="23" t="s">
+      <c r="A133" s="31" t="s">
         <v>235</v>
       </c>
       <c r="B133" s="8">
@@ -12189,7 +12196,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="32"/>
+      <c r="A134" s="35"/>
       <c r="B134" s="8">
         <v>2</v>
       </c>
@@ -12198,7 +12205,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="32"/>
+      <c r="A135" s="35"/>
       <c r="B135" s="8">
         <v>3</v>
       </c>
@@ -12207,7 +12214,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="24"/>
+      <c r="A136" s="32"/>
       <c r="B136" s="8">
         <v>4</v>
       </c>
@@ -12217,36 +12224,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A82:A85"/>
     <mergeCell ref="A114:A115"/>
     <mergeCell ref="A116:A119"/>
     <mergeCell ref="A120:A132"/>
@@ -12256,6 +12233,36 @@
     <mergeCell ref="A92:A97"/>
     <mergeCell ref="A98:B98"/>
     <mergeCell ref="A99:A113"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12280,14 +12287,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>433</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
separate file for thesis exploration
</commit_message>
<xml_diff>
--- a/data dictionary/DICC_A434_M3_NINOS.RID.xlsx
+++ b/data dictionary/DICC_A434_M3_NINOS.RID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a5584703a9932d8/Documentos/RStudio/thesis/data dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{76951DC6-D1D1-4F7A-8241-5F94A5EAB1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F510571-C95B-4559-B3FE-847F9F9077CD}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{76951DC6-D1D1-4F7A-8241-5F94A5EAB1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39676F81-80B3-48B7-A816-9D19F0A32DE9}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="506">
   <si>
     <r>
       <rPr>
@@ -5596,9 +5596,6 @@
     </r>
   </si>
   <si>
-    <t>que es eso</t>
-  </si>
-  <si>
     <t>diferencia con estrato?</t>
   </si>
   <si>
@@ -5669,6 +5666,12 @@
   </si>
   <si>
     <t>bottle</t>
+  </si>
+  <si>
+    <t>Debe ser igual a MPIO</t>
+  </si>
+  <si>
+    <t>grupo de edad, no necesario para niños</t>
   </si>
 </sst>
 </file>
@@ -5986,10 +5989,43 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -6003,53 +6039,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -6360,8 +6363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="K122" sqref="K122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6394,10 +6397,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6444,7 +6447,7 @@
     </row>
     <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B6" s="16">
         <v>15</v>
@@ -6456,7 +6459,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -6601,7 +6604,7 @@
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B17" s="23">
         <v>40</v>
@@ -6613,7 +6616,7 @@
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6624,7 +6627,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>10</v>
@@ -6770,7 +6773,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6958,12 +6961,12 @@
         <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B42" s="16">
         <v>65</v>
@@ -6975,7 +6978,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F42" t="s">
         <v>471</v>
@@ -6995,7 +6998,7 @@
         <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7012,7 +7015,7 @@
         <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7040,7 +7043,7 @@
         <v>69</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>10</v>
@@ -7416,7 +7419,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7587,7 +7590,7 @@
         <v>7</v>
       </c>
       <c r="E84" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F84" t="s">
         <v>476</v>
@@ -7638,7 +7641,7 @@
         <v>10</v>
       </c>
       <c r="E87" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7646,7 +7649,7 @@
         <v>156</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C88" s="18" t="s">
         <v>157</v>
@@ -8047,7 +8050,7 @@
         <v>10</v>
       </c>
       <c r="F116" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8064,35 +8067,38 @@
         <v>10</v>
       </c>
       <c r="E117" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="B118" s="6">
+      <c r="B118" s="16">
         <v>146</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="C118" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D118" s="7" t="s">
+      <c r="D118" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="B119" s="6">
+      <c r="B119" s="16">
         <v>148</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="D119" s="7" t="s">
+      <c r="D119" s="18" t="s">
         <v>10</v>
+      </c>
+      <c r="E119" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8110,16 +8116,16 @@
       </c>
     </row>
     <row r="121" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="B121" s="6">
+      <c r="B121" s="16">
         <v>197</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="C121" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="D121" s="7" t="s">
+      <c r="D121" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -8151,7 +8157,7 @@
         <v>10</v>
       </c>
       <c r="E123" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8168,7 +8174,7 @@
         <v>10</v>
       </c>
       <c r="F124" t="s">
-        <v>480</v>
+        <v>505</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8185,10 +8191,10 @@
         <v>10</v>
       </c>
       <c r="E125" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F125" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8205,7 +8211,7 @@
         <v>234</v>
       </c>
       <c r="F126" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8300,25 +8306,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="43"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="33"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>243</v>
       </c>
       <c r="B3" s="8">
@@ -8327,20 +8333,20 @@
       <c r="C3" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="44"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="28" t="s">
         <v>246</v>
       </c>
       <c r="B5" s="8">
@@ -8349,30 +8355,30 @@
       <c r="C5" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="8">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D6" s="33"/>
+      <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="8">
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="44"/>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>250</v>
       </c>
       <c r="B8" s="8">
@@ -8381,20 +8387,20 @@
       <c r="C8" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="44"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="44"/>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="8">
@@ -8403,20 +8409,20 @@
       <c r="C10" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="44"/>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="8">
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="8">
@@ -8425,30 +8431,30 @@
       <c r="C12" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D12" s="33"/>
+      <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="8">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D13" s="33"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="8">
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D14" s="33"/>
+      <c r="D14" s="44"/>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="8">
@@ -8457,20 +8463,20 @@
       <c r="C15" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="D15" s="33"/>
+      <c r="D15" s="44"/>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="8">
         <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D16" s="33"/>
+      <c r="D16" s="44"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="8">
@@ -8481,7 +8487,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="8">
         <v>2</v>
       </c>
@@ -8490,7 +8496,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="8">
         <v>3</v>
       </c>
@@ -8499,7 +8505,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="8">
         <v>4</v>
       </c>
@@ -8508,7 +8514,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
@@ -8517,7 +8523,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="8">
         <v>6</v>
       </c>
@@ -8526,7 +8532,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="8">
@@ -8537,7 +8543,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -8546,7 +8552,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -8555,7 +8561,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="8">
         <v>4</v>
       </c>
@@ -8564,7 +8570,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="8">
         <v>5</v>
       </c>
@@ -8573,7 +8579,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="8">
         <v>6</v>
       </c>
@@ -8582,7 +8588,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="31" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="8">
@@ -8593,7 +8599,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="8">
         <v>2</v>
       </c>
@@ -8602,7 +8608,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="31" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="8">
@@ -8613,7 +8619,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="8">
         <v>2</v>
       </c>
@@ -8622,7 +8628,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="28" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="8">
@@ -8633,7 +8639,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="8">
         <v>8</v>
       </c>
@@ -8642,7 +8648,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="8">
         <v>9</v>
       </c>
@@ -8651,7 +8657,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="8">
         <v>11</v>
       </c>
@@ -8660,7 +8666,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="8">
         <v>12</v>
       </c>
@@ -8669,7 +8675,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="8">
         <v>13</v>
       </c>
@@ -8678,7 +8684,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B39" s="8">
@@ -8689,7 +8695,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="8">
         <v>2</v>
       </c>
@@ -8698,7 +8704,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="8">
         <v>3</v>
       </c>
@@ -8707,7 +8713,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="8">
         <v>4</v>
       </c>
@@ -8716,7 +8722,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="8">
         <v>5</v>
       </c>
@@ -8725,7 +8731,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="8">
         <v>6</v>
       </c>
@@ -8734,7 +8740,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="8">
         <v>7</v>
       </c>
@@ -8743,7 +8749,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="8">
         <v>8</v>
       </c>
@@ -8752,7 +8758,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="8">
         <v>9</v>
       </c>
@@ -8761,7 +8767,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="36"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="8">
         <v>10</v>
       </c>
@@ -8770,7 +8776,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="28" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="8">
@@ -8781,7 +8787,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="8">
         <v>2</v>
       </c>
@@ -8790,7 +8796,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+      <c r="A51" s="29"/>
       <c r="B51" s="8">
         <v>3</v>
       </c>
@@ -8799,7 +8805,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="8">
         <v>4</v>
       </c>
@@ -8808,7 +8814,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
+      <c r="A53" s="29"/>
       <c r="B53" s="8">
         <v>5</v>
       </c>
@@ -8817,7 +8823,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="36"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="8">
         <v>6</v>
       </c>
@@ -8826,7 +8832,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="28" t="s">
         <v>31</v>
       </c>
       <c r="B55" s="8">
@@ -8837,7 +8843,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35"/>
+      <c r="A56" s="29"/>
       <c r="B56" s="8">
         <v>2</v>
       </c>
@@ -8846,7 +8852,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35"/>
+      <c r="A57" s="29"/>
       <c r="B57" s="8">
         <v>3</v>
       </c>
@@ -8855,7 +8861,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
+      <c r="A58" s="29"/>
       <c r="B58" s="8">
         <v>4</v>
       </c>
@@ -8864,7 +8870,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="8">
         <v>5</v>
       </c>
@@ -8873,7 +8879,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+      <c r="A60" s="29"/>
       <c r="B60" s="8">
         <v>6</v>
       </c>
@@ -8882,7 +8888,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
+      <c r="A61" s="29"/>
       <c r="B61" s="8">
         <v>7</v>
       </c>
@@ -8891,7 +8897,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="36"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="8">
         <v>8</v>
       </c>
@@ -8900,7 +8906,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
+      <c r="A63" s="33"/>
       <c r="B63" s="8">
         <v>1</v>
       </c>
@@ -8909,7 +8915,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="42"/>
+      <c r="A64" s="34"/>
       <c r="B64" s="8">
         <v>2</v>
       </c>
@@ -8918,7 +8924,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="42"/>
+      <c r="A65" s="34"/>
       <c r="B65" s="8">
         <v>3</v>
       </c>
@@ -8927,7 +8933,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B66" s="8">
@@ -8938,7 +8944,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35"/>
+      <c r="A67" s="29"/>
       <c r="B67" s="8">
         <v>5</v>
       </c>
@@ -8947,7 +8953,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="35"/>
+      <c r="A68" s="29"/>
       <c r="B68" s="8">
         <v>6</v>
       </c>
@@ -8956,7 +8962,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="35"/>
+      <c r="A69" s="29"/>
       <c r="B69" s="8">
         <v>7</v>
       </c>
@@ -8965,7 +8971,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="35"/>
+      <c r="A70" s="29"/>
       <c r="B70" s="8">
         <v>8</v>
       </c>
@@ -8974,7 +8980,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="35"/>
+      <c r="A71" s="29"/>
       <c r="B71" s="8">
         <v>9</v>
       </c>
@@ -8983,7 +8989,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="35"/>
+      <c r="A72" s="29"/>
       <c r="B72" s="8">
         <v>10</v>
       </c>
@@ -8992,7 +8998,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="35"/>
+      <c r="A73" s="29"/>
       <c r="B73" s="8">
         <v>11</v>
       </c>
@@ -9001,7 +9007,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="35"/>
+      <c r="A74" s="29"/>
       <c r="B74" s="8">
         <v>12</v>
       </c>
@@ -9010,7 +9016,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
+      <c r="A75" s="29"/>
       <c r="B75" s="8">
         <v>13</v>
       </c>
@@ -9019,7 +9025,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="35"/>
+      <c r="A76" s="29"/>
       <c r="B76" s="8">
         <v>14</v>
       </c>
@@ -9028,7 +9034,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="35"/>
+      <c r="A77" s="29"/>
       <c r="B77" s="8">
         <v>15</v>
       </c>
@@ -9037,7 +9043,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="35"/>
+      <c r="A78" s="29"/>
       <c r="B78" s="8">
         <v>16</v>
       </c>
@@ -9046,7 +9052,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="35"/>
+      <c r="A79" s="29"/>
       <c r="B79" s="8">
         <v>17</v>
       </c>
@@ -9055,7 +9061,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="36"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="8">
         <v>18</v>
       </c>
@@ -9064,7 +9070,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="28" t="s">
+      <c r="A81" s="31" t="s">
         <v>38</v>
       </c>
       <c r="B81" s="8">
@@ -9075,7 +9081,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="29"/>
+      <c r="A82" s="32"/>
       <c r="B82" s="8">
         <v>2</v>
       </c>
@@ -9084,7 +9090,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="34" t="s">
+      <c r="A83" s="28" t="s">
         <v>40</v>
       </c>
       <c r="B83" s="8">
@@ -9095,7 +9101,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="35"/>
+      <c r="A84" s="29"/>
       <c r="B84" s="8">
         <v>2</v>
       </c>
@@ -9104,7 +9110,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="35"/>
+      <c r="A85" s="29"/>
       <c r="B85" s="8">
         <v>3</v>
       </c>
@@ -9113,7 +9119,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="35"/>
+      <c r="A86" s="29"/>
       <c r="B86" s="8">
         <v>4</v>
       </c>
@@ -9122,7 +9128,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="35"/>
+      <c r="A87" s="29"/>
       <c r="B87" s="8">
         <v>5</v>
       </c>
@@ -9131,7 +9137,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="35"/>
+      <c r="A88" s="29"/>
       <c r="B88" s="8">
         <v>6</v>
       </c>
@@ -9140,7 +9146,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="35"/>
+      <c r="A89" s="29"/>
       <c r="B89" s="8">
         <v>7</v>
       </c>
@@ -9149,7 +9155,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="35"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="8">
         <v>8</v>
       </c>
@@ -9158,7 +9164,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="35"/>
+      <c r="A91" s="29"/>
       <c r="B91" s="8">
         <v>9</v>
       </c>
@@ -9167,7 +9173,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="35"/>
+      <c r="A92" s="29"/>
       <c r="B92" s="8">
         <v>10</v>
       </c>
@@ -9176,7 +9182,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="35"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="8">
         <v>11</v>
       </c>
@@ -9185,7 +9191,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="35"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="8">
         <v>12</v>
       </c>
@@ -9194,7 +9200,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="35"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="8">
         <v>13</v>
       </c>
@@ -9203,7 +9209,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="35"/>
+      <c r="A96" s="29"/>
       <c r="B96" s="8">
         <v>14</v>
       </c>
@@ -9212,7 +9218,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="35"/>
+      <c r="A97" s="29"/>
       <c r="B97" s="8">
         <v>15</v>
       </c>
@@ -9221,7 +9227,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="35"/>
+      <c r="A98" s="29"/>
       <c r="B98" s="8">
         <v>16</v>
       </c>
@@ -9230,7 +9236,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="36"/>
+      <c r="A99" s="30"/>
       <c r="B99" s="8">
         <v>18</v>
       </c>
@@ -9239,7 +9245,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="28" t="s">
+      <c r="A100" s="31" t="s">
         <v>44</v>
       </c>
       <c r="B100" s="8">
@@ -9250,7 +9256,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="37"/>
+      <c r="A101" s="35"/>
       <c r="B101" s="8">
         <v>2</v>
       </c>
@@ -9259,7 +9265,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="37"/>
+      <c r="A102" s="35"/>
       <c r="B102" s="8">
         <v>3</v>
       </c>
@@ -9268,7 +9274,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="29"/>
+      <c r="A103" s="32"/>
       <c r="B103" s="8">
         <v>4</v>
       </c>
@@ -9277,7 +9283,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="40" t="s">
+      <c r="A104" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B104" s="8">
@@ -9288,7 +9294,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="41"/>
+      <c r="A105" s="37"/>
       <c r="B105" s="8">
         <v>2</v>
       </c>
@@ -9297,7 +9303,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="41"/>
+      <c r="A106" s="37"/>
       <c r="B106" s="8">
         <v>3</v>
       </c>
@@ -9306,7 +9312,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="41"/>
+      <c r="A107" s="37"/>
       <c r="B107" s="8">
         <v>4</v>
       </c>
@@ -9315,7 +9321,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="41"/>
+      <c r="A108" s="37"/>
       <c r="B108" s="8">
         <v>5</v>
       </c>
@@ -9324,7 +9330,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="41"/>
+      <c r="A109" s="37"/>
       <c r="B109" s="8">
         <v>6</v>
       </c>
@@ -9333,7 +9339,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="41"/>
+      <c r="A110" s="37"/>
       <c r="B110" s="8">
         <v>7</v>
       </c>
@@ -9342,7 +9348,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="41"/>
+      <c r="A111" s="37"/>
       <c r="B111" s="8">
         <v>8</v>
       </c>
@@ -9351,7 +9357,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="41"/>
+      <c r="A112" s="37"/>
       <c r="B112" s="8">
         <v>9</v>
       </c>
@@ -9360,7 +9366,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="41"/>
+      <c r="A113" s="37"/>
       <c r="B113" s="8">
         <v>10</v>
       </c>
@@ -9369,7 +9375,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="41"/>
+      <c r="A114" s="37"/>
       <c r="B114" s="8">
         <v>11</v>
       </c>
@@ -9378,7 +9384,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="42"/>
+      <c r="A115" s="34"/>
       <c r="B115" s="8">
         <v>12</v>
       </c>
@@ -9387,7 +9393,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="42"/>
+      <c r="A116" s="34"/>
       <c r="B116" s="8">
         <v>13</v>
       </c>
@@ -9396,7 +9402,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="42"/>
+      <c r="A117" s="34"/>
       <c r="B117" s="8">
         <v>14</v>
       </c>
@@ -9405,7 +9411,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="42"/>
+      <c r="A118" s="34"/>
       <c r="B118" s="8">
         <v>15</v>
       </c>
@@ -9414,7 +9420,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="42"/>
+      <c r="A119" s="34"/>
       <c r="B119" s="8">
         <v>16</v>
       </c>
@@ -9423,7 +9429,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="43"/>
+      <c r="A120" s="38"/>
       <c r="B120" s="8">
         <v>17</v>
       </c>
@@ -9432,7 +9438,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="34" t="s">
+      <c r="A121" s="28" t="s">
         <v>50</v>
       </c>
       <c r="B121" s="8">
@@ -9443,7 +9449,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="35"/>
+      <c r="A122" s="29"/>
       <c r="B122" s="8">
         <v>2</v>
       </c>
@@ -9452,7 +9458,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="35"/>
+      <c r="A123" s="29"/>
       <c r="B123" s="8">
         <v>3</v>
       </c>
@@ -9461,7 +9467,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="35"/>
+      <c r="A124" s="29"/>
       <c r="B124" s="8">
         <v>4</v>
       </c>
@@ -9470,7 +9476,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="35"/>
+      <c r="A125" s="29"/>
       <c r="B125" s="8">
         <v>5</v>
       </c>
@@ -9479,7 +9485,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="35"/>
+      <c r="A126" s="29"/>
       <c r="B126" s="8">
         <v>6</v>
       </c>
@@ -9488,7 +9494,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="35"/>
+      <c r="A127" s="29"/>
       <c r="B127" s="8">
         <v>7</v>
       </c>
@@ -9497,7 +9503,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="36"/>
+      <c r="A128" s="30"/>
       <c r="B128" s="8">
         <v>8</v>
       </c>
@@ -9506,7 +9512,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="28" t="s">
+      <c r="A129" s="31" t="s">
         <v>51</v>
       </c>
       <c r="B129" s="8">
@@ -9517,7 +9523,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="29"/>
+      <c r="A130" s="32"/>
       <c r="B130" s="8">
         <v>1</v>
       </c>
@@ -9526,7 +9532,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="28" t="s">
+      <c r="A131" s="31" t="s">
         <v>53</v>
       </c>
       <c r="B131" s="8">
@@ -9537,7 +9543,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="29"/>
+      <c r="A132" s="32"/>
       <c r="B132" s="8">
         <v>1</v>
       </c>
@@ -9546,7 +9552,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="28" t="s">
+      <c r="A133" s="31" t="s">
         <v>55</v>
       </c>
       <c r="B133" s="8">
@@ -9557,7 +9563,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="29"/>
+      <c r="A134" s="32"/>
       <c r="B134" s="8">
         <v>1</v>
       </c>
@@ -9566,7 +9572,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="28" t="s">
+      <c r="A135" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B135" s="8">
@@ -9577,7 +9583,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="29"/>
+      <c r="A136" s="32"/>
       <c r="B136" s="8">
         <v>1</v>
       </c>
@@ -9586,7 +9592,7 @@
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="28" t="s">
+      <c r="A137" s="31" t="s">
         <v>59</v>
       </c>
       <c r="B137" s="8">
@@ -9597,7 +9603,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="29"/>
+      <c r="A138" s="32"/>
       <c r="B138" s="8">
         <v>1</v>
       </c>
@@ -9606,7 +9612,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="28" t="s">
+      <c r="A139" s="31" t="s">
         <v>61</v>
       </c>
       <c r="B139" s="8">
@@ -9617,7 +9623,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="29"/>
+      <c r="A140" s="32"/>
       <c r="B140" s="8">
         <v>1</v>
       </c>
@@ -9626,7 +9632,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="28" t="s">
+      <c r="A141" s="31" t="s">
         <v>63</v>
       </c>
       <c r="B141" s="8">
@@ -9637,7 +9643,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="29"/>
+      <c r="A142" s="32"/>
       <c r="B142" s="8">
         <v>1</v>
       </c>
@@ -9646,7 +9652,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="28" t="s">
+      <c r="A143" s="31" t="s">
         <v>65</v>
       </c>
       <c r="B143" s="8">
@@ -9657,7 +9663,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="37"/>
+      <c r="A144" s="35"/>
       <c r="B144" s="8">
         <v>2</v>
       </c>
@@ -9666,7 +9672,7 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="37"/>
+      <c r="A145" s="35"/>
       <c r="B145" s="8">
         <v>3</v>
       </c>
@@ -9675,7 +9681,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="29"/>
+      <c r="A146" s="32"/>
       <c r="B146" s="8">
         <v>4</v>
       </c>
@@ -9684,7 +9690,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="34" t="s">
+      <c r="A147" s="28" t="s">
         <v>66</v>
       </c>
       <c r="B147" s="8">
@@ -9695,7 +9701,7 @@
       </c>
     </row>
     <row r="148" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="35"/>
+      <c r="A148" s="29"/>
       <c r="B148" s="8">
         <v>2</v>
       </c>
@@ -9704,7 +9710,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="35"/>
+      <c r="A149" s="29"/>
       <c r="B149" s="8">
         <v>3</v>
       </c>
@@ -9713,7 +9719,7 @@
       </c>
     </row>
     <row r="150" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="35"/>
+      <c r="A150" s="29"/>
       <c r="B150" s="8">
         <v>4</v>
       </c>
@@ -9722,7 +9728,7 @@
       </c>
     </row>
     <row r="151" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="35"/>
+      <c r="A151" s="29"/>
       <c r="B151" s="8">
         <v>5</v>
       </c>
@@ -9731,7 +9737,7 @@
       </c>
     </row>
     <row r="152" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="36"/>
+      <c r="A152" s="30"/>
       <c r="B152" s="8">
         <v>6</v>
       </c>
@@ -9740,7 +9746,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="28" t="s">
+      <c r="A153" s="31" t="s">
         <v>68</v>
       </c>
       <c r="B153" s="8">
@@ -9751,7 +9757,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="29"/>
+      <c r="A154" s="32"/>
       <c r="B154" s="8">
         <v>2</v>
       </c>
@@ -9760,7 +9766,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="34" t="s">
+      <c r="A155" s="28" t="s">
         <v>70</v>
       </c>
       <c r="B155" s="8">
@@ -9771,7 +9777,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="35"/>
+      <c r="A156" s="29"/>
       <c r="B156" s="8">
         <v>2</v>
       </c>
@@ -9780,7 +9786,7 @@
       </c>
     </row>
     <row r="157" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="35"/>
+      <c r="A157" s="29"/>
       <c r="B157" s="8">
         <v>3</v>
       </c>
@@ -9789,7 +9795,7 @@
       </c>
     </row>
     <row r="158" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="35"/>
+      <c r="A158" s="29"/>
       <c r="B158" s="8">
         <v>4</v>
       </c>
@@ -9798,7 +9804,7 @@
       </c>
     </row>
     <row r="159" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="35"/>
+      <c r="A159" s="29"/>
       <c r="B159" s="8">
         <v>5</v>
       </c>
@@ -9807,7 +9813,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="35"/>
+      <c r="A160" s="29"/>
       <c r="B160" s="8">
         <v>6</v>
       </c>
@@ -9816,7 +9822,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="35"/>
+      <c r="A161" s="29"/>
       <c r="B161" s="8">
         <v>7</v>
       </c>
@@ -9825,7 +9831,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="36"/>
+      <c r="A162" s="30"/>
       <c r="B162" s="8">
         <v>8</v>
       </c>
@@ -9834,16 +9840,16 @@
       </c>
     </row>
     <row r="163" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="38">
+      <c r="A163" s="39">
         <v>1</v>
       </c>
-      <c r="B163" s="39"/>
+      <c r="B163" s="40"/>
       <c r="C163" s="7" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="37" t="s">
+      <c r="A164" s="35" t="s">
         <v>73</v>
       </c>
       <c r="B164" s="8">
@@ -9854,7 +9860,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="29"/>
+      <c r="A165" s="32"/>
       <c r="B165" s="8">
         <v>3</v>
       </c>
@@ -9863,7 +9869,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="28" t="s">
+      <c r="A166" s="31" t="s">
         <v>74</v>
       </c>
       <c r="B166" s="8">
@@ -9874,7 +9880,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="29"/>
+      <c r="A167" s="32"/>
       <c r="B167" s="8">
         <v>2</v>
       </c>
@@ -9883,7 +9889,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="28" t="s">
+      <c r="A168" s="31" t="s">
         <v>75</v>
       </c>
       <c r="B168" s="8">
@@ -9894,7 +9900,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="37"/>
+      <c r="A169" s="35"/>
       <c r="B169" s="8">
         <v>2</v>
       </c>
@@ -9903,7 +9909,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="37"/>
+      <c r="A170" s="35"/>
       <c r="B170" s="8">
         <v>3</v>
       </c>
@@ -9912,7 +9918,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="29"/>
+      <c r="A171" s="32"/>
       <c r="B171" s="8">
         <v>4</v>
       </c>
@@ -9921,7 +9927,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="34" t="s">
+      <c r="A172" s="28" t="s">
         <v>76</v>
       </c>
       <c r="B172" s="8">
@@ -9932,7 +9938,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="35"/>
+      <c r="A173" s="29"/>
       <c r="B173" s="8">
         <v>2</v>
       </c>
@@ -9941,7 +9947,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="36"/>
+      <c r="A174" s="30"/>
       <c r="B174" s="8">
         <v>3</v>
       </c>
@@ -9950,7 +9956,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="28" t="s">
+      <c r="A175" s="31" t="s">
         <v>78</v>
       </c>
       <c r="B175" s="8">
@@ -9961,7 +9967,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="37"/>
+      <c r="A176" s="35"/>
       <c r="B176" s="8">
         <v>2</v>
       </c>
@@ -9970,7 +9976,7 @@
       </c>
     </row>
     <row r="177" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="37"/>
+      <c r="A177" s="35"/>
       <c r="B177" s="8">
         <v>3</v>
       </c>
@@ -9979,7 +9985,7 @@
       </c>
     </row>
     <row r="178" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="29"/>
+      <c r="A178" s="32"/>
       <c r="B178" s="8">
         <v>4</v>
       </c>
@@ -9988,7 +9994,7 @@
       </c>
     </row>
     <row r="179" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="34" t="s">
+      <c r="A179" s="28" t="s">
         <v>79</v>
       </c>
       <c r="B179" s="8">
@@ -9999,7 +10005,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="35"/>
+      <c r="A180" s="29"/>
       <c r="B180" s="8">
         <v>2</v>
       </c>
@@ -10008,7 +10014,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="36"/>
+      <c r="A181" s="30"/>
       <c r="B181" s="8">
         <v>3</v>
       </c>
@@ -10017,7 +10023,7 @@
       </c>
     </row>
     <row r="182" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="34" t="s">
+      <c r="A182" s="28" t="s">
         <v>80</v>
       </c>
       <c r="B182" s="8">
@@ -10028,7 +10034,7 @@
       </c>
     </row>
     <row r="183" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="35"/>
+      <c r="A183" s="29"/>
       <c r="B183" s="8">
         <v>2</v>
       </c>
@@ -10037,7 +10043,7 @@
       </c>
     </row>
     <row r="184" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="35"/>
+      <c r="A184" s="29"/>
       <c r="B184" s="8">
         <v>3</v>
       </c>
@@ -10046,7 +10052,7 @@
       </c>
     </row>
     <row r="185" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="35"/>
+      <c r="A185" s="29"/>
       <c r="B185" s="8">
         <v>4</v>
       </c>
@@ -10055,7 +10061,7 @@
       </c>
     </row>
     <row r="186" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="36"/>
+      <c r="A186" s="30"/>
       <c r="B186" s="8">
         <v>5</v>
       </c>
@@ -10064,7 +10070,7 @@
       </c>
     </row>
     <row r="187" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="28" t="s">
+      <c r="A187" s="31" t="s">
         <v>84</v>
       </c>
       <c r="B187" s="8">
@@ -10075,7 +10081,7 @@
       </c>
     </row>
     <row r="188" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="29"/>
+      <c r="A188" s="32"/>
       <c r="B188" s="8">
         <v>1</v>
       </c>
@@ -10084,7 +10090,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="28" t="s">
+      <c r="A189" s="31" t="s">
         <v>86</v>
       </c>
       <c r="B189" s="8">
@@ -10095,7 +10101,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="29"/>
+      <c r="A190" s="32"/>
       <c r="B190" s="8">
         <v>1</v>
       </c>
@@ -10104,7 +10110,7 @@
       </c>
     </row>
     <row r="191" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="28" t="s">
+      <c r="A191" s="31" t="s">
         <v>88</v>
       </c>
       <c r="B191" s="8">
@@ -10115,7 +10121,7 @@
       </c>
     </row>
     <row r="192" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="29"/>
+      <c r="A192" s="32"/>
       <c r="B192" s="8">
         <v>1</v>
       </c>
@@ -10124,7 +10130,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="28" t="s">
+      <c r="A193" s="31" t="s">
         <v>90</v>
       </c>
       <c r="B193" s="8">
@@ -10135,7 +10141,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="29"/>
+      <c r="A194" s="32"/>
       <c r="B194" s="8">
         <v>1</v>
       </c>
@@ -10144,7 +10150,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="28" t="s">
+      <c r="A195" s="31" t="s">
         <v>92</v>
       </c>
       <c r="B195" s="8">
@@ -10155,7 +10161,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="29"/>
+      <c r="A196" s="32"/>
       <c r="B196" s="8">
         <v>1</v>
       </c>
@@ -10164,7 +10170,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A197" s="28" t="s">
+      <c r="A197" s="31" t="s">
         <v>94</v>
       </c>
       <c r="B197" s="8">
@@ -10175,7 +10181,7 @@
       </c>
     </row>
     <row r="198" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A198" s="29"/>
+      <c r="A198" s="32"/>
       <c r="B198" s="8">
         <v>1</v>
       </c>
@@ -10184,7 +10190,7 @@
       </c>
     </row>
     <row r="199" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A199" s="28" t="s">
+      <c r="A199" s="31" t="s">
         <v>96</v>
       </c>
       <c r="B199" s="8">
@@ -10195,7 +10201,7 @@
       </c>
     </row>
     <row r="200" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A200" s="29"/>
+      <c r="A200" s="32"/>
       <c r="B200" s="8">
         <v>1</v>
       </c>
@@ -10204,7 +10210,7 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A201" s="28" t="s">
+      <c r="A201" s="31" t="s">
         <v>98</v>
       </c>
       <c r="B201" s="8">
@@ -10215,7 +10221,7 @@
       </c>
     </row>
     <row r="202" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A202" s="29"/>
+      <c r="A202" s="32"/>
       <c r="B202" s="8">
         <v>1</v>
       </c>
@@ -10224,7 +10230,7 @@
       </c>
     </row>
     <row r="203" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A203" s="28" t="s">
+      <c r="A203" s="31" t="s">
         <v>100</v>
       </c>
       <c r="B203" s="8">
@@ -10235,7 +10241,7 @@
       </c>
     </row>
     <row r="204" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A204" s="29"/>
+      <c r="A204" s="32"/>
       <c r="B204" s="8">
         <v>1</v>
       </c>
@@ -10244,7 +10250,7 @@
       </c>
     </row>
     <row r="205" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A205" s="28" t="s">
+      <c r="A205" s="31" t="s">
         <v>102</v>
       </c>
       <c r="B205" s="8">
@@ -10255,7 +10261,7 @@
       </c>
     </row>
     <row r="206" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A206" s="29"/>
+      <c r="A206" s="32"/>
       <c r="B206" s="8">
         <v>1</v>
       </c>
@@ -10264,7 +10270,7 @@
       </c>
     </row>
     <row r="207" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A207" s="28" t="s">
+      <c r="A207" s="31" t="s">
         <v>104</v>
       </c>
       <c r="B207" s="8">
@@ -10275,7 +10281,7 @@
       </c>
     </row>
     <row r="208" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A208" s="29"/>
+      <c r="A208" s="32"/>
       <c r="B208" s="8">
         <v>1</v>
       </c>
@@ -10284,7 +10290,7 @@
       </c>
     </row>
     <row r="209" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A209" s="28" t="s">
+      <c r="A209" s="31" t="s">
         <v>106</v>
       </c>
       <c r="B209" s="8">
@@ -10295,7 +10301,7 @@
       </c>
     </row>
     <row r="210" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A210" s="29"/>
+      <c r="A210" s="32"/>
       <c r="B210" s="8">
         <v>1</v>
       </c>
@@ -10304,7 +10310,7 @@
       </c>
     </row>
     <row r="211" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A211" s="28" t="s">
+      <c r="A211" s="31" t="s">
         <v>108</v>
       </c>
       <c r="B211" s="8">
@@ -10315,7 +10321,7 @@
       </c>
     </row>
     <row r="212" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A212" s="29"/>
+      <c r="A212" s="32"/>
       <c r="B212" s="8">
         <v>1</v>
       </c>
@@ -10325,47 +10331,6 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A39:A48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="A55:A62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A99"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="A104:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A121:A128"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="A133:A134"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A146"/>
-    <mergeCell ref="A147:A152"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="A155:A162"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="A168:A171"/>
-    <mergeCell ref="A172:A174"/>
-    <mergeCell ref="A175:A178"/>
-    <mergeCell ref="A179:A181"/>
-    <mergeCell ref="A182:A186"/>
-    <mergeCell ref="A205:A206"/>
-    <mergeCell ref="A187:A188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="A193:A194"/>
-    <mergeCell ref="A195:A196"/>
     <mergeCell ref="A207:A208"/>
     <mergeCell ref="A209:A210"/>
     <mergeCell ref="A211:A212"/>
@@ -10382,6 +10347,47 @@
     <mergeCell ref="A199:A200"/>
     <mergeCell ref="A201:A202"/>
     <mergeCell ref="A203:A204"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A187:A188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="A193:A194"/>
+    <mergeCell ref="A195:A196"/>
+    <mergeCell ref="A168:A171"/>
+    <mergeCell ref="A172:A174"/>
+    <mergeCell ref="A175:A178"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A182:A186"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="A155:A162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A146"/>
+    <mergeCell ref="A147:A152"/>
+    <mergeCell ref="A121:A128"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="A133:A134"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A39:A48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A55:A62"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A80"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10403,7 +10409,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>110</v>
       </c>
       <c r="B1" s="8">
@@ -10414,7 +10420,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="8">
         <v>92</v>
       </c>
@@ -10423,7 +10429,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="28" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="8">
@@ -10434,7 +10440,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -10443,7 +10449,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="8">
         <v>3</v>
       </c>
@@ -10452,7 +10458,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="31" t="s">
         <v>112</v>
       </c>
       <c r="B6" s="8">
@@ -10463,7 +10469,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="8">
         <v>1</v>
       </c>
@@ -10472,7 +10478,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>114</v>
       </c>
       <c r="B8" s="8">
@@ -10483,7 +10489,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="8">
         <v>1</v>
       </c>
@@ -10492,7 +10498,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="31" t="s">
         <v>116</v>
       </c>
       <c r="B10" s="8">
@@ -10503,7 +10509,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="8">
         <v>1</v>
       </c>
@@ -10512,7 +10518,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="31" t="s">
         <v>118</v>
       </c>
       <c r="B12" s="8">
@@ -10523,7 +10529,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="8">
         <v>1</v>
       </c>
@@ -10532,7 +10538,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="31" t="s">
         <v>120</v>
       </c>
       <c r="B14" s="8">
@@ -10543,7 +10549,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="8">
         <v>1</v>
       </c>
@@ -10552,7 +10558,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="31" t="s">
         <v>122</v>
       </c>
       <c r="B16" s="8">
@@ -10563,7 +10569,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="8">
         <v>2</v>
       </c>
@@ -10572,7 +10578,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="31" t="s">
         <v>124</v>
       </c>
       <c r="B18" s="8">
@@ -10583,7 +10589,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="8">
         <v>92</v>
       </c>
@@ -10592,7 +10598,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="28" t="s">
         <v>126</v>
       </c>
       <c r="B20" s="8">
@@ -10603,7 +10609,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="8">
         <v>2</v>
       </c>
@@ -10612,7 +10618,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="8">
         <v>3</v>
       </c>
@@ -10621,7 +10627,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="28" t="s">
         <v>128</v>
       </c>
       <c r="B23" s="8">
@@ -10632,7 +10638,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -10641,7 +10647,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -10650,7 +10656,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="31" t="s">
         <v>372</v>
       </c>
       <c r="B26" s="8">
@@ -10661,7 +10667,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="8">
         <v>2</v>
       </c>
@@ -10670,7 +10676,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="31" t="s">
         <v>130</v>
       </c>
       <c r="B28" s="8">
@@ -10681,7 +10687,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="8">
         <v>1</v>
       </c>
@@ -10690,7 +10696,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="31" t="s">
         <v>132</v>
       </c>
       <c r="B30" s="8">
@@ -10701,7 +10707,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="8">
         <v>1</v>
       </c>
@@ -10710,7 +10716,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="31" t="s">
         <v>134</v>
       </c>
       <c r="B32" s="8">
@@ -10721,7 +10727,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="8">
         <v>1</v>
       </c>
@@ -10730,7 +10736,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="31" t="s">
         <v>136</v>
       </c>
       <c r="B34" s="8">
@@ -10741,7 +10747,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="8">
         <v>1</v>
       </c>
@@ -10750,7 +10756,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="31" t="s">
         <v>138</v>
       </c>
       <c r="B36" s="8">
@@ -10761,7 +10767,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
+      <c r="A37" s="32"/>
       <c r="B37" s="8">
         <v>1</v>
       </c>
@@ -10770,7 +10776,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="31" t="s">
         <v>140</v>
       </c>
       <c r="B38" s="8">
@@ -10781,7 +10787,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="8">
         <v>1</v>
       </c>
@@ -10790,7 +10796,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="31" t="s">
         <v>142</v>
       </c>
       <c r="B40" s="8">
@@ -10801,7 +10807,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="8">
         <v>1</v>
       </c>
@@ -10810,7 +10816,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="31" t="s">
         <v>373</v>
       </c>
       <c r="B42" s="8">
@@ -10821,7 +10827,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="8">
         <v>2</v>
       </c>
@@ -10830,7 +10836,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="31" t="s">
         <v>146</v>
       </c>
       <c r="B44" s="8">
@@ -10841,7 +10847,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="8">
         <v>2</v>
       </c>
@@ -10850,7 +10856,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="37"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="8">
         <v>3</v>
       </c>
@@ -10859,7 +10865,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="8">
         <v>4</v>
       </c>
@@ -10868,7 +10874,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="28" t="s">
         <v>148</v>
       </c>
       <c r="B48" s="8">
@@ -10879,7 +10885,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="8">
         <v>2</v>
       </c>
@@ -10894,21 +10900,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:C50"/>
@@ -10917,6 +10908,21 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10938,7 +10944,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48"/>
+      <c r="A1" s="46"/>
       <c r="B1" s="8">
         <v>3</v>
       </c>
@@ -10947,7 +10953,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
+      <c r="A2" s="47"/>
       <c r="B2" s="8">
         <v>4</v>
       </c>
@@ -10956,7 +10962,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>150</v>
       </c>
       <c r="B3" s="8">
@@ -10967,7 +10973,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="8">
         <v>92</v>
       </c>
@@ -10976,7 +10982,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="31" t="s">
         <v>151</v>
       </c>
       <c r="B5" s="8">
@@ -10987,7 +10993,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="8">
         <v>2</v>
       </c>
@@ -10996,7 +11002,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="31" t="s">
         <v>152</v>
       </c>
       <c r="B7" s="8">
@@ -11007,7 +11013,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="8">
         <v>92</v>
       </c>
@@ -11016,7 +11022,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>156</v>
       </c>
       <c r="B9" s="8">
@@ -11027,7 +11033,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="8">
         <v>1</v>
       </c>
@@ -11036,7 +11042,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="31" t="s">
         <v>158</v>
       </c>
       <c r="B11" s="8">
@@ -11047,7 +11053,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="8">
         <v>1</v>
       </c>
@@ -11056,7 +11062,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="31" t="s">
         <v>160</v>
       </c>
       <c r="B13" s="8">
@@ -11067,7 +11073,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="8">
         <v>1</v>
       </c>
@@ -11076,7 +11082,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="31" t="s">
         <v>162</v>
       </c>
       <c r="B15" s="8">
@@ -11087,7 +11093,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="8">
         <v>1</v>
       </c>
@@ -11096,7 +11102,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="31" t="s">
         <v>164</v>
       </c>
       <c r="B17" s="8">
@@ -11107,7 +11113,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="8">
         <v>1</v>
       </c>
@@ -11116,7 +11122,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="31" t="s">
         <v>166</v>
       </c>
       <c r="B19" s="8">
@@ -11127,7 +11133,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="8">
         <v>1</v>
       </c>
@@ -11136,7 +11142,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="31" t="s">
         <v>168</v>
       </c>
       <c r="B21" s="8">
@@ -11147,7 +11153,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="8">
         <v>1</v>
       </c>
@@ -11156,7 +11162,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="28" t="s">
         <v>172</v>
       </c>
       <c r="B23" s="8">
@@ -11167,7 +11173,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -11176,7 +11182,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -11185,7 +11191,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="31" t="s">
         <v>174</v>
       </c>
       <c r="B26" s="8">
@@ -11196,7 +11202,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="8">
         <v>2</v>
       </c>
@@ -11205,7 +11211,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="8">
         <v>3</v>
       </c>
@@ -11214,7 +11220,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="8">
         <v>4</v>
       </c>
@@ -11223,7 +11229,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="28" t="s">
         <v>176</v>
       </c>
       <c r="B30" s="8">
@@ -11234,7 +11240,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="8">
         <v>2</v>
       </c>
@@ -11243,7 +11249,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="8">
         <v>3</v>
       </c>
@@ -11252,7 +11258,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="31" t="s">
         <v>178</v>
       </c>
       <c r="B33" s="8">
@@ -11263,7 +11269,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="8">
         <v>2</v>
       </c>
@@ -11272,7 +11278,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="8">
         <v>3</v>
       </c>
@@ -11281,7 +11287,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="8">
         <v>4</v>
       </c>
@@ -11290,7 +11296,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="28" t="s">
         <v>180</v>
       </c>
       <c r="B37" s="8">
@@ -11301,7 +11307,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="8">
         <v>2</v>
       </c>
@@ -11310,7 +11316,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="8">
         <v>3</v>
       </c>
@@ -11319,7 +11325,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="31" t="s">
         <v>182</v>
       </c>
       <c r="B40" s="8">
@@ -11330,7 +11336,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37"/>
+      <c r="A41" s="35"/>
       <c r="B41" s="8">
         <v>2</v>
       </c>
@@ -11339,7 +11345,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="8">
         <v>3</v>
       </c>
@@ -11348,7 +11354,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="8">
         <v>4</v>
       </c>
@@ -11357,7 +11363,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="28" t="s">
         <v>184</v>
       </c>
       <c r="B44" s="8">
@@ -11368,7 +11374,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="8">
         <v>2</v>
       </c>
@@ -11377,7 +11383,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="8">
         <v>3</v>
       </c>
@@ -11386,7 +11392,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="28" t="s">
         <v>186</v>
       </c>
       <c r="B47" s="8">
@@ -11397,7 +11403,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="8">
         <v>2</v>
       </c>
@@ -11406,7 +11412,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="8">
         <v>3</v>
       </c>
@@ -11415,16 +11421,16 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="46">
+      <c r="A50" s="48">
         <v>4</v>
       </c>
-      <c r="B50" s="47"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="7" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="28" t="s">
         <v>188</v>
       </c>
       <c r="B51" s="8">
@@ -11435,7 +11441,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="8">
         <v>2</v>
       </c>
@@ -11444,7 +11450,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="36"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="8">
         <v>3</v>
       </c>
@@ -11453,7 +11459,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="31" t="s">
         <v>190</v>
       </c>
       <c r="B54" s="8">
@@ -11464,7 +11470,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="37"/>
+      <c r="A55" s="35"/>
       <c r="B55" s="8">
         <v>2</v>
       </c>
@@ -11473,7 +11479,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="37"/>
+      <c r="A56" s="35"/>
       <c r="B56" s="8">
         <v>3</v>
       </c>
@@ -11482,7 +11488,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="8">
         <v>4</v>
       </c>
@@ -11491,7 +11497,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="28" t="s">
         <v>192</v>
       </c>
       <c r="B58" s="8">
@@ -11502,7 +11508,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="8">
         <v>2</v>
       </c>
@@ -11511,7 +11517,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="36"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="8">
         <v>3</v>
       </c>
@@ -11520,7 +11526,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="28" t="s">
+      <c r="A61" s="31" t="s">
         <v>194</v>
       </c>
       <c r="B61" s="8">
@@ -11531,7 +11537,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="37"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="8">
         <v>2</v>
       </c>
@@ -11540,7 +11546,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="37"/>
+      <c r="A63" s="35"/>
       <c r="B63" s="8">
         <v>3</v>
       </c>
@@ -11549,7 +11555,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="29"/>
+      <c r="A64" s="32"/>
       <c r="B64" s="8">
         <v>4</v>
       </c>
@@ -11558,7 +11564,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="28" t="s">
         <v>196</v>
       </c>
       <c r="B65" s="8">
@@ -11569,7 +11575,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+      <c r="A66" s="29"/>
       <c r="B66" s="8">
         <v>2</v>
       </c>
@@ -11578,7 +11584,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="36"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="8">
         <v>3</v>
       </c>
@@ -11587,7 +11593,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="28" t="s">
+      <c r="A68" s="31" t="s">
         <v>198</v>
       </c>
       <c r="B68" s="8">
@@ -11598,7 +11604,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="37"/>
+      <c r="A69" s="35"/>
       <c r="B69" s="8">
         <v>2</v>
       </c>
@@ -11607,7 +11613,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="37"/>
+      <c r="A70" s="35"/>
       <c r="B70" s="8">
         <v>3</v>
       </c>
@@ -11616,7 +11622,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="29"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="8">
         <v>4</v>
       </c>
@@ -11625,7 +11631,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="28" t="s">
         <v>200</v>
       </c>
       <c r="B72" s="8">
@@ -11636,7 +11642,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="35"/>
+      <c r="A73" s="29"/>
       <c r="B73" s="8">
         <v>2</v>
       </c>
@@ -11645,7 +11651,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="36"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="8">
         <v>3</v>
       </c>
@@ -11654,7 +11660,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="28" t="s">
+      <c r="A75" s="31" t="s">
         <v>202</v>
       </c>
       <c r="B75" s="8">
@@ -11665,7 +11671,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="37"/>
+      <c r="A76" s="35"/>
       <c r="B76" s="8">
         <v>2</v>
       </c>
@@ -11674,7 +11680,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="37"/>
+      <c r="A77" s="35"/>
       <c r="B77" s="8">
         <v>3</v>
       </c>
@@ -11683,7 +11689,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="29"/>
+      <c r="A78" s="32"/>
       <c r="B78" s="8">
         <v>4</v>
       </c>
@@ -11692,7 +11698,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="34" t="s">
+      <c r="A79" s="28" t="s">
         <v>204</v>
       </c>
       <c r="B79" s="8">
@@ -11703,7 +11709,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="35"/>
+      <c r="A80" s="29"/>
       <c r="B80" s="8">
         <v>2</v>
       </c>
@@ -11712,7 +11718,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="36"/>
+      <c r="A81" s="30"/>
       <c r="B81" s="8">
         <v>3</v>
       </c>
@@ -11721,7 +11727,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
+      <c r="A82" s="31" t="s">
         <v>206</v>
       </c>
       <c r="B82" s="8">
@@ -11732,7 +11738,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="37"/>
+      <c r="A83" s="35"/>
       <c r="B83" s="8">
         <v>2</v>
       </c>
@@ -11741,7 +11747,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="37"/>
+      <c r="A84" s="35"/>
       <c r="B84" s="8">
         <v>3</v>
       </c>
@@ -11750,7 +11756,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="29"/>
+      <c r="A85" s="32"/>
       <c r="B85" s="8">
         <v>4</v>
       </c>
@@ -11759,7 +11765,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="34" t="s">
+      <c r="A86" s="28" t="s">
         <v>208</v>
       </c>
       <c r="B86" s="8">
@@ -11770,7 +11776,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="35"/>
+      <c r="A87" s="29"/>
       <c r="B87" s="8">
         <v>2</v>
       </c>
@@ -11779,7 +11785,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="36"/>
+      <c r="A88" s="30"/>
       <c r="B88" s="8">
         <v>3</v>
       </c>
@@ -11788,7 +11794,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="34" t="s">
+      <c r="A89" s="28" t="s">
         <v>212</v>
       </c>
       <c r="B89" s="8">
@@ -11799,7 +11805,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="35"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="8">
         <v>2</v>
       </c>
@@ -11808,7 +11814,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="36"/>
+      <c r="A91" s="30"/>
       <c r="B91" s="8">
         <v>3</v>
       </c>
@@ -11817,7 +11823,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="34" t="s">
+      <c r="A92" s="28" t="s">
         <v>214</v>
       </c>
       <c r="B92" s="8">
@@ -11828,7 +11834,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="35"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="8">
         <v>2</v>
       </c>
@@ -11837,7 +11843,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="35"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="8">
         <v>3</v>
       </c>
@@ -11846,7 +11852,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="35"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="8">
         <v>4</v>
       </c>
@@ -11855,7 +11861,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="35"/>
+      <c r="A96" s="29"/>
       <c r="B96" s="8">
         <v>5</v>
       </c>
@@ -11864,7 +11870,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="36"/>
+      <c r="A97" s="30"/>
       <c r="B97" s="8">
         <v>6</v>
       </c>
@@ -11873,16 +11879,16 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="38">
+      <c r="A98" s="39">
         <v>1</v>
       </c>
-      <c r="B98" s="39"/>
+      <c r="B98" s="40"/>
       <c r="C98" s="7" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="35" t="s">
+      <c r="A99" s="29" t="s">
         <v>216</v>
       </c>
       <c r="B99" s="8">
@@ -11893,7 +11899,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="35"/>
+      <c r="A100" s="29"/>
       <c r="B100" s="8">
         <v>3</v>
       </c>
@@ -11902,7 +11908,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="35"/>
+      <c r="A101" s="29"/>
       <c r="B101" s="8">
         <v>4</v>
       </c>
@@ -11911,7 +11917,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="35"/>
+      <c r="A102" s="29"/>
       <c r="B102" s="8">
         <v>5</v>
       </c>
@@ -11920,7 +11926,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="35"/>
+      <c r="A103" s="29"/>
       <c r="B103" s="8">
         <v>6</v>
       </c>
@@ -11929,7 +11935,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="35"/>
+      <c r="A104" s="29"/>
       <c r="B104" s="8">
         <v>7</v>
       </c>
@@ -11938,7 +11944,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="35"/>
+      <c r="A105" s="29"/>
       <c r="B105" s="8">
         <v>8</v>
       </c>
@@ -11947,7 +11953,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="35"/>
+      <c r="A106" s="29"/>
       <c r="B106" s="8">
         <v>9</v>
       </c>
@@ -11956,7 +11962,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="35"/>
+      <c r="A107" s="29"/>
       <c r="B107" s="8">
         <v>10</v>
       </c>
@@ -11965,7 +11971,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="35"/>
+      <c r="A108" s="29"/>
       <c r="B108" s="8">
         <v>11</v>
       </c>
@@ -11974,7 +11980,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="35"/>
+      <c r="A109" s="29"/>
       <c r="B109" s="8">
         <v>12</v>
       </c>
@@ -11983,7 +11989,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="35"/>
+      <c r="A110" s="29"/>
       <c r="B110" s="8">
         <v>13</v>
       </c>
@@ -11992,7 +11998,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="35"/>
+      <c r="A111" s="29"/>
       <c r="B111" s="8">
         <v>14</v>
       </c>
@@ -12001,7 +12007,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="35"/>
+      <c r="A112" s="29"/>
       <c r="B112" s="8">
         <v>15</v>
       </c>
@@ -12010,7 +12016,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="36"/>
+      <c r="A113" s="30"/>
       <c r="B113" s="8">
         <v>16</v>
       </c>
@@ -12019,7 +12025,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="28" t="s">
+      <c r="A114" s="31" t="s">
         <v>226</v>
       </c>
       <c r="B114" s="8">
@@ -12030,7 +12036,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="29"/>
+      <c r="A115" s="32"/>
       <c r="B115" s="8">
         <v>2</v>
       </c>
@@ -12039,7 +12045,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="28" t="s">
+      <c r="A116" s="31" t="s">
         <v>230</v>
       </c>
       <c r="B116" s="8">
@@ -12050,7 +12056,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="37"/>
+      <c r="A117" s="35"/>
       <c r="B117" s="8">
         <v>2</v>
       </c>
@@ -12059,7 +12065,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="37"/>
+      <c r="A118" s="35"/>
       <c r="B118" s="8">
         <v>3</v>
       </c>
@@ -12068,7 +12074,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="29"/>
+      <c r="A119" s="32"/>
       <c r="B119" s="8">
         <v>4</v>
       </c>
@@ -12077,7 +12083,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="34" t="s">
+      <c r="A120" s="28" t="s">
         <v>232</v>
       </c>
       <c r="B120" s="8">
@@ -12088,7 +12094,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="35"/>
+      <c r="A121" s="29"/>
       <c r="B121" s="8">
         <v>2</v>
       </c>
@@ -12097,7 +12103,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="35"/>
+      <c r="A122" s="29"/>
       <c r="B122" s="8">
         <v>3</v>
       </c>
@@ -12106,7 +12112,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="35"/>
+      <c r="A123" s="29"/>
       <c r="B123" s="8">
         <v>4</v>
       </c>
@@ -12115,7 +12121,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="35"/>
+      <c r="A124" s="29"/>
       <c r="B124" s="8">
         <v>5</v>
       </c>
@@ -12124,7 +12130,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="35"/>
+      <c r="A125" s="29"/>
       <c r="B125" s="8">
         <v>6</v>
       </c>
@@ -12133,7 +12139,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="35"/>
+      <c r="A126" s="29"/>
       <c r="B126" s="8">
         <v>7</v>
       </c>
@@ -12142,7 +12148,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="35"/>
+      <c r="A127" s="29"/>
       <c r="B127" s="8">
         <v>8</v>
       </c>
@@ -12151,7 +12157,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="35"/>
+      <c r="A128" s="29"/>
       <c r="B128" s="8">
         <v>9</v>
       </c>
@@ -12160,7 +12166,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="35"/>
+      <c r="A129" s="29"/>
       <c r="B129" s="8">
         <v>10</v>
       </c>
@@ -12169,7 +12175,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
+      <c r="A130" s="29"/>
       <c r="B130" s="8">
         <v>11</v>
       </c>
@@ -12178,7 +12184,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="35"/>
+      <c r="A131" s="29"/>
       <c r="B131" s="8">
         <v>12</v>
       </c>
@@ -12187,7 +12193,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="36"/>
+      <c r="A132" s="30"/>
       <c r="B132" s="8">
         <v>13</v>
       </c>
@@ -12196,7 +12202,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="28" t="s">
+      <c r="A133" s="31" t="s">
         <v>235</v>
       </c>
       <c r="B133" s="8">
@@ -12207,7 +12213,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="37"/>
+      <c r="A134" s="35"/>
       <c r="B134" s="8">
         <v>2</v>
       </c>
@@ -12216,7 +12222,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="37"/>
+      <c r="A135" s="35"/>
       <c r="B135" s="8">
         <v>3</v>
       </c>
@@ -12225,7 +12231,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="29"/>
+      <c r="A136" s="32"/>
       <c r="B136" s="8">
         <v>4</v>
       </c>
@@ -12235,36 +12241,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A82:A85"/>
     <mergeCell ref="A114:A115"/>
     <mergeCell ref="A116:A119"/>
     <mergeCell ref="A120:A132"/>
@@ -12274,6 +12250,36 @@
     <mergeCell ref="A92:A97"/>
     <mergeCell ref="A98:B98"/>
     <mergeCell ref="A99:A113"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DAG (EMM and confounders)
</commit_message>
<xml_diff>
--- a/data dictionary/DICC_A434_M3_NINOS.RID.xlsx
+++ b/data dictionary/DICC_A434_M3_NINOS.RID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a5584703a9932d8/Documentos/RStudio/thesis/data dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{76951DC6-D1D1-4F7A-8241-5F94A5EAB1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39676F81-80B3-48B7-A816-9D19F0A32DE9}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{76951DC6-D1D1-4F7A-8241-5F94A5EAB1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{392634BD-A227-4310-B8A9-85A8D5DFE052}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="507">
   <si>
     <r>
       <rPr>
@@ -5672,6 +5672,9 @@
   </si>
   <si>
     <t>grupo de edad, no necesario para niños</t>
+  </si>
+  <si>
+    <t>Excluido porque tiene muchos Nas</t>
   </si>
 </sst>
 </file>
@@ -5903,7 +5906,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5989,43 +5992,10 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -6039,8 +6009,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -6048,14 +6057,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6363,8 +6381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="K122" sqref="K122"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6589,17 +6607,20 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="52">
         <v>39</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="53" t="s">
         <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6620,142 +6641,142 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="52">
         <v>41</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="54" t="s">
         <v>483</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="52">
         <v>42</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="52">
         <v>43</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="52">
         <v>44</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="52">
         <v>45</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="52">
         <v>46</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="52">
         <v>47</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="52">
         <v>48</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="52">
         <v>49</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="52">
         <v>50</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="53" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6906,58 +6927,58 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="52">
         <v>61</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="52">
         <v>62</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="54" t="s">
         <v>460</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="52">
         <v>63</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="52">
         <v>64</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="54" t="s">
         <v>470</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="53" t="s">
         <v>10</v>
       </c>
       <c r="F41" t="s">
@@ -6965,16 +6986,16 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="55" t="s">
         <v>488</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="52">
         <v>65</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="54" t="s">
         <v>462</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="53" t="s">
         <v>10</v>
       </c>
       <c r="E42" t="s">
@@ -6985,16 +7006,16 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="16">
+      <c r="B43" s="52">
         <v>66</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="54" t="s">
         <v>463</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="53" t="s">
         <v>10</v>
       </c>
       <c r="F43" t="s">
@@ -7002,16 +7023,16 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="16">
+      <c r="B44" s="52">
         <v>67</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="54" t="s">
         <v>461</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D44" s="53" t="s">
         <v>10</v>
       </c>
       <c r="F44" t="s">
@@ -7019,16 +7040,16 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="16">
+      <c r="B45" s="52">
         <v>68</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D45" s="53" t="s">
         <v>10</v>
       </c>
       <c r="F45" t="s">
@@ -7036,16 +7057,16 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="16">
+      <c r="B46" s="52">
         <v>69</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="54" t="s">
         <v>489</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="53" t="s">
         <v>10</v>
       </c>
       <c r="F46" t="s">
@@ -7053,16 +7074,16 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="52">
         <v>70</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="54" t="s">
         <v>468</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D47" s="53" t="s">
         <v>10</v>
       </c>
       <c r="F47" t="s">
@@ -8294,7 +8315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D212"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
+    <sheetView topLeftCell="A136" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -8306,25 +8327,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="31" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="44"/>
+      <c r="D2" s="33"/>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>243</v>
       </c>
       <c r="B3" s="8">
@@ -8333,20 +8354,20 @@
       <c r="C3" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D3" s="44"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="34" t="s">
         <v>246</v>
       </c>
       <c r="B5" s="8">
@@ -8355,30 +8376,30 @@
       <c r="C5" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="8">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D6" s="44"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="8">
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="D7" s="44"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>250</v>
       </c>
       <c r="B8" s="8">
@@ -8387,20 +8408,20 @@
       <c r="C8" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="D8" s="44"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="D9" s="44"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="8">
@@ -8409,20 +8430,20 @@
       <c r="C10" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="8">
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="D11" s="44"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="8">
@@ -8431,30 +8452,30 @@
       <c r="C12" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D12" s="44"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="8">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D13" s="44"/>
+      <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="8">
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D14" s="44"/>
+      <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="28" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="8">
@@ -8463,20 +8484,20 @@
       <c r="C15" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="D15" s="44"/>
+      <c r="D15" s="33"/>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="8">
         <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="33"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="34" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="8">
@@ -8487,7 +8508,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="8">
         <v>2</v>
       </c>
@@ -8496,7 +8517,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="8">
         <v>3</v>
       </c>
@@ -8505,7 +8526,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="8">
         <v>4</v>
       </c>
@@ -8514,7 +8535,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="8">
         <v>5</v>
       </c>
@@ -8523,7 +8544,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="8">
         <v>6</v>
       </c>
@@ -8532,7 +8553,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="34" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="8">
@@ -8543,7 +8564,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -8552,7 +8573,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -8561,7 +8582,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="8">
         <v>4</v>
       </c>
@@ -8570,7 +8591,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="8">
         <v>5</v>
       </c>
@@ -8579,7 +8600,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="8">
         <v>6</v>
       </c>
@@ -8588,7 +8609,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="28" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="8">
@@ -8599,7 +8620,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="8">
         <v>2</v>
       </c>
@@ -8608,7 +8629,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="28" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="8">
@@ -8619,7 +8640,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="8">
         <v>2</v>
       </c>
@@ -8628,7 +8649,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="34" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="8">
@@ -8639,7 +8660,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="8">
         <v>8</v>
       </c>
@@ -8648,7 +8669,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="8">
         <v>9</v>
       </c>
@@ -8657,7 +8678,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
+      <c r="A36" s="35"/>
       <c r="B36" s="8">
         <v>11</v>
       </c>
@@ -8666,7 +8687,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="8">
         <v>12</v>
       </c>
@@ -8675,7 +8696,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A38" s="36"/>
       <c r="B38" s="8">
         <v>13</v>
       </c>
@@ -8684,7 +8705,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="34" t="s">
         <v>28</v>
       </c>
       <c r="B39" s="8">
@@ -8695,7 +8716,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="8">
         <v>2</v>
       </c>
@@ -8704,7 +8725,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
+      <c r="A41" s="35"/>
       <c r="B41" s="8">
         <v>3</v>
       </c>
@@ -8713,7 +8734,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="8">
         <v>4</v>
       </c>
@@ -8722,7 +8743,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
+      <c r="A43" s="35"/>
       <c r="B43" s="8">
         <v>5</v>
       </c>
@@ -8731,7 +8752,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
+      <c r="A44" s="35"/>
       <c r="B44" s="8">
         <v>6</v>
       </c>
@@ -8740,7 +8761,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="8">
         <v>7</v>
       </c>
@@ -8749,7 +8770,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="8">
         <v>8</v>
       </c>
@@ -8758,7 +8779,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
+      <c r="A47" s="35"/>
       <c r="B47" s="8">
         <v>9</v>
       </c>
@@ -8767,7 +8788,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="36"/>
       <c r="B48" s="8">
         <v>10</v>
       </c>
@@ -8776,7 +8797,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="34" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="8">
@@ -8787,7 +8808,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="29"/>
+      <c r="A50" s="35"/>
       <c r="B50" s="8">
         <v>2</v>
       </c>
@@ -8796,7 +8817,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="29"/>
+      <c r="A51" s="35"/>
       <c r="B51" s="8">
         <v>3</v>
       </c>
@@ -8805,7 +8826,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
+      <c r="A52" s="35"/>
       <c r="B52" s="8">
         <v>4</v>
       </c>
@@ -8814,7 +8835,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
+      <c r="A53" s="35"/>
       <c r="B53" s="8">
         <v>5</v>
       </c>
@@ -8823,7 +8844,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="30"/>
+      <c r="A54" s="36"/>
       <c r="B54" s="8">
         <v>6</v>
       </c>
@@ -8832,7 +8853,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="34" t="s">
         <v>31</v>
       </c>
       <c r="B55" s="8">
@@ -8843,7 +8864,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
+      <c r="A56" s="35"/>
       <c r="B56" s="8">
         <v>2</v>
       </c>
@@ -8852,7 +8873,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
+      <c r="A57" s="35"/>
       <c r="B57" s="8">
         <v>3</v>
       </c>
@@ -8861,7 +8882,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="29"/>
+      <c r="A58" s="35"/>
       <c r="B58" s="8">
         <v>4</v>
       </c>
@@ -8870,7 +8891,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
+      <c r="A59" s="35"/>
       <c r="B59" s="8">
         <v>5</v>
       </c>
@@ -8879,7 +8900,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
+      <c r="A60" s="35"/>
       <c r="B60" s="8">
         <v>6</v>
       </c>
@@ -8888,7 +8909,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
+      <c r="A61" s="35"/>
       <c r="B61" s="8">
         <v>7</v>
       </c>
@@ -8897,7 +8918,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+      <c r="A62" s="36"/>
       <c r="B62" s="8">
         <v>8</v>
       </c>
@@ -8906,7 +8927,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
+      <c r="A63" s="44"/>
       <c r="B63" s="8">
         <v>1</v>
       </c>
@@ -8915,7 +8936,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="34"/>
+      <c r="A64" s="42"/>
       <c r="B64" s="8">
         <v>2</v>
       </c>
@@ -8924,7 +8945,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
+      <c r="A65" s="42"/>
       <c r="B65" s="8">
         <v>3</v>
       </c>
@@ -8933,7 +8954,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="35" t="s">
         <v>34</v>
       </c>
       <c r="B66" s="8">
@@ -8944,7 +8965,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="29"/>
+      <c r="A67" s="35"/>
       <c r="B67" s="8">
         <v>5</v>
       </c>
@@ -8953,7 +8974,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="29"/>
+      <c r="A68" s="35"/>
       <c r="B68" s="8">
         <v>6</v>
       </c>
@@ -8962,7 +8983,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="29"/>
+      <c r="A69" s="35"/>
       <c r="B69" s="8">
         <v>7</v>
       </c>
@@ -8971,7 +8992,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="29"/>
+      <c r="A70" s="35"/>
       <c r="B70" s="8">
         <v>8</v>
       </c>
@@ -8980,7 +9001,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="29"/>
+      <c r="A71" s="35"/>
       <c r="B71" s="8">
         <v>9</v>
       </c>
@@ -8989,7 +9010,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="29"/>
+      <c r="A72" s="35"/>
       <c r="B72" s="8">
         <v>10</v>
       </c>
@@ -8998,7 +9019,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
+      <c r="A73" s="35"/>
       <c r="B73" s="8">
         <v>11</v>
       </c>
@@ -9007,7 +9028,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="29"/>
+      <c r="A74" s="35"/>
       <c r="B74" s="8">
         <v>12</v>
       </c>
@@ -9016,7 +9037,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="29"/>
+      <c r="A75" s="35"/>
       <c r="B75" s="8">
         <v>13</v>
       </c>
@@ -9025,7 +9046,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="A76" s="35"/>
       <c r="B76" s="8">
         <v>14</v>
       </c>
@@ -9034,7 +9055,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="35"/>
       <c r="B77" s="8">
         <v>15</v>
       </c>
@@ -9043,7 +9064,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="29"/>
+      <c r="A78" s="35"/>
       <c r="B78" s="8">
         <v>16</v>
       </c>
@@ -9052,7 +9073,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="29"/>
+      <c r="A79" s="35"/>
       <c r="B79" s="8">
         <v>17</v>
       </c>
@@ -9061,7 +9082,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
+      <c r="A80" s="36"/>
       <c r="B80" s="8">
         <v>18</v>
       </c>
@@ -9070,7 +9091,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="31" t="s">
+      <c r="A81" s="28" t="s">
         <v>38</v>
       </c>
       <c r="B81" s="8">
@@ -9081,7 +9102,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="32"/>
+      <c r="A82" s="29"/>
       <c r="B82" s="8">
         <v>2</v>
       </c>
@@ -9090,7 +9111,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="s">
+      <c r="A83" s="34" t="s">
         <v>40</v>
       </c>
       <c r="B83" s="8">
@@ -9101,7 +9122,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
+      <c r="A84" s="35"/>
       <c r="B84" s="8">
         <v>2</v>
       </c>
@@ -9110,7 +9131,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="29"/>
+      <c r="A85" s="35"/>
       <c r="B85" s="8">
         <v>3</v>
       </c>
@@ -9119,7 +9140,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="29"/>
+      <c r="A86" s="35"/>
       <c r="B86" s="8">
         <v>4</v>
       </c>
@@ -9128,7 +9149,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="29"/>
+      <c r="A87" s="35"/>
       <c r="B87" s="8">
         <v>5</v>
       </c>
@@ -9137,7 +9158,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="29"/>
+      <c r="A88" s="35"/>
       <c r="B88" s="8">
         <v>6</v>
       </c>
@@ -9146,7 +9167,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="29"/>
+      <c r="A89" s="35"/>
       <c r="B89" s="8">
         <v>7</v>
       </c>
@@ -9155,7 +9176,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="29"/>
+      <c r="A90" s="35"/>
       <c r="B90" s="8">
         <v>8</v>
       </c>
@@ -9164,7 +9185,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="29"/>
+      <c r="A91" s="35"/>
       <c r="B91" s="8">
         <v>9</v>
       </c>
@@ -9173,7 +9194,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="29"/>
+      <c r="A92" s="35"/>
       <c r="B92" s="8">
         <v>10</v>
       </c>
@@ -9182,7 +9203,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
+      <c r="A93" s="35"/>
       <c r="B93" s="8">
         <v>11</v>
       </c>
@@ -9191,7 +9212,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
+      <c r="A94" s="35"/>
       <c r="B94" s="8">
         <v>12</v>
       </c>
@@ -9200,7 +9221,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="29"/>
+      <c r="A95" s="35"/>
       <c r="B95" s="8">
         <v>13</v>
       </c>
@@ -9209,7 +9230,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="29"/>
+      <c r="A96" s="35"/>
       <c r="B96" s="8">
         <v>14</v>
       </c>
@@ -9218,7 +9239,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="29"/>
+      <c r="A97" s="35"/>
       <c r="B97" s="8">
         <v>15</v>
       </c>
@@ -9227,7 +9248,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="29"/>
+      <c r="A98" s="35"/>
       <c r="B98" s="8">
         <v>16</v>
       </c>
@@ -9236,7 +9257,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="30"/>
+      <c r="A99" s="36"/>
       <c r="B99" s="8">
         <v>18</v>
       </c>
@@ -9245,7 +9266,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="31" t="s">
+      <c r="A100" s="28" t="s">
         <v>44</v>
       </c>
       <c r="B100" s="8">
@@ -9256,7 +9277,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="35"/>
+      <c r="A101" s="37"/>
       <c r="B101" s="8">
         <v>2</v>
       </c>
@@ -9265,7 +9286,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="35"/>
+      <c r="A102" s="37"/>
       <c r="B102" s="8">
         <v>3</v>
       </c>
@@ -9274,7 +9295,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="32"/>
+      <c r="A103" s="29"/>
       <c r="B103" s="8">
         <v>4</v>
       </c>
@@ -9283,7 +9304,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="36" t="s">
+      <c r="A104" s="40" t="s">
         <v>46</v>
       </c>
       <c r="B104" s="8">
@@ -9294,7 +9315,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="37"/>
+      <c r="A105" s="41"/>
       <c r="B105" s="8">
         <v>2</v>
       </c>
@@ -9303,7 +9324,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="37"/>
+      <c r="A106" s="41"/>
       <c r="B106" s="8">
         <v>3</v>
       </c>
@@ -9312,7 +9333,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="37"/>
+      <c r="A107" s="41"/>
       <c r="B107" s="8">
         <v>4</v>
       </c>
@@ -9321,7 +9342,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="37"/>
+      <c r="A108" s="41"/>
       <c r="B108" s="8">
         <v>5</v>
       </c>
@@ -9330,7 +9351,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="37"/>
+      <c r="A109" s="41"/>
       <c r="B109" s="8">
         <v>6</v>
       </c>
@@ -9339,7 +9360,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="37"/>
+      <c r="A110" s="41"/>
       <c r="B110" s="8">
         <v>7</v>
       </c>
@@ -9348,7 +9369,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="37"/>
+      <c r="A111" s="41"/>
       <c r="B111" s="8">
         <v>8</v>
       </c>
@@ -9357,7 +9378,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="37"/>
+      <c r="A112" s="41"/>
       <c r="B112" s="8">
         <v>9</v>
       </c>
@@ -9366,7 +9387,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="37"/>
+      <c r="A113" s="41"/>
       <c r="B113" s="8">
         <v>10</v>
       </c>
@@ -9375,7 +9396,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="37"/>
+      <c r="A114" s="41"/>
       <c r="B114" s="8">
         <v>11</v>
       </c>
@@ -9384,7 +9405,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="34"/>
+      <c r="A115" s="42"/>
       <c r="B115" s="8">
         <v>12</v>
       </c>
@@ -9393,7 +9414,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
+      <c r="A116" s="42"/>
       <c r="B116" s="8">
         <v>13</v>
       </c>
@@ -9402,7 +9423,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
+      <c r="A117" s="42"/>
       <c r="B117" s="8">
         <v>14</v>
       </c>
@@ -9411,7 +9432,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
+      <c r="A118" s="42"/>
       <c r="B118" s="8">
         <v>15</v>
       </c>
@@ -9420,7 +9441,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
+      <c r="A119" s="42"/>
       <c r="B119" s="8">
         <v>16</v>
       </c>
@@ -9429,7 +9450,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="38"/>
+      <c r="A120" s="43"/>
       <c r="B120" s="8">
         <v>17</v>
       </c>
@@ -9438,7 +9459,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="28" t="s">
+      <c r="A121" s="34" t="s">
         <v>50</v>
       </c>
       <c r="B121" s="8">
@@ -9449,7 +9470,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="29"/>
+      <c r="A122" s="35"/>
       <c r="B122" s="8">
         <v>2</v>
       </c>
@@ -9458,7 +9479,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="29"/>
+      <c r="A123" s="35"/>
       <c r="B123" s="8">
         <v>3</v>
       </c>
@@ -9467,7 +9488,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="29"/>
+      <c r="A124" s="35"/>
       <c r="B124" s="8">
         <v>4</v>
       </c>
@@ -9476,7 +9497,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="29"/>
+      <c r="A125" s="35"/>
       <c r="B125" s="8">
         <v>5</v>
       </c>
@@ -9485,7 +9506,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="29"/>
+      <c r="A126" s="35"/>
       <c r="B126" s="8">
         <v>6</v>
       </c>
@@ -9494,7 +9515,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="29"/>
+      <c r="A127" s="35"/>
       <c r="B127" s="8">
         <v>7</v>
       </c>
@@ -9503,7 +9524,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="30"/>
+      <c r="A128" s="36"/>
       <c r="B128" s="8">
         <v>8</v>
       </c>
@@ -9512,7 +9533,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="31" t="s">
+      <c r="A129" s="28" t="s">
         <v>51</v>
       </c>
       <c r="B129" s="8">
@@ -9523,7 +9544,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="32"/>
+      <c r="A130" s="29"/>
       <c r="B130" s="8">
         <v>1</v>
       </c>
@@ -9532,7 +9553,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="31" t="s">
+      <c r="A131" s="28" t="s">
         <v>53</v>
       </c>
       <c r="B131" s="8">
@@ -9543,7 +9564,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="32"/>
+      <c r="A132" s="29"/>
       <c r="B132" s="8">
         <v>1</v>
       </c>
@@ -9552,7 +9573,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="31" t="s">
+      <c r="A133" s="28" t="s">
         <v>55</v>
       </c>
       <c r="B133" s="8">
@@ -9563,7 +9584,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="32"/>
+      <c r="A134" s="29"/>
       <c r="B134" s="8">
         <v>1</v>
       </c>
@@ -9572,7 +9593,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="31" t="s">
+      <c r="A135" s="28" t="s">
         <v>57</v>
       </c>
       <c r="B135" s="8">
@@ -9583,7 +9604,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="32"/>
+      <c r="A136" s="29"/>
       <c r="B136" s="8">
         <v>1</v>
       </c>
@@ -9592,7 +9613,7 @@
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="31" t="s">
+      <c r="A137" s="28" t="s">
         <v>59</v>
       </c>
       <c r="B137" s="8">
@@ -9603,7 +9624,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="32"/>
+      <c r="A138" s="29"/>
       <c r="B138" s="8">
         <v>1</v>
       </c>
@@ -9612,7 +9633,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="31" t="s">
+      <c r="A139" s="28" t="s">
         <v>61</v>
       </c>
       <c r="B139" s="8">
@@ -9623,7 +9644,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="32"/>
+      <c r="A140" s="29"/>
       <c r="B140" s="8">
         <v>1</v>
       </c>
@@ -9632,7 +9653,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="31" t="s">
+      <c r="A141" s="28" t="s">
         <v>63</v>
       </c>
       <c r="B141" s="8">
@@ -9643,7 +9664,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="32"/>
+      <c r="A142" s="29"/>
       <c r="B142" s="8">
         <v>1</v>
       </c>
@@ -9652,7 +9673,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="31" t="s">
+      <c r="A143" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B143" s="8">
@@ -9663,7 +9684,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="35"/>
+      <c r="A144" s="37"/>
       <c r="B144" s="8">
         <v>2</v>
       </c>
@@ -9672,7 +9693,7 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="35"/>
+      <c r="A145" s="37"/>
       <c r="B145" s="8">
         <v>3</v>
       </c>
@@ -9681,7 +9702,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="32"/>
+      <c r="A146" s="29"/>
       <c r="B146" s="8">
         <v>4</v>
       </c>
@@ -9690,7 +9711,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="28" t="s">
+      <c r="A147" s="34" t="s">
         <v>66</v>
       </c>
       <c r="B147" s="8">
@@ -9701,7 +9722,7 @@
       </c>
     </row>
     <row r="148" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="29"/>
+      <c r="A148" s="35"/>
       <c r="B148" s="8">
         <v>2</v>
       </c>
@@ -9710,7 +9731,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="29"/>
+      <c r="A149" s="35"/>
       <c r="B149" s="8">
         <v>3</v>
       </c>
@@ -9719,7 +9740,7 @@
       </c>
     </row>
     <row r="150" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="29"/>
+      <c r="A150" s="35"/>
       <c r="B150" s="8">
         <v>4</v>
       </c>
@@ -9728,7 +9749,7 @@
       </c>
     </row>
     <row r="151" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="29"/>
+      <c r="A151" s="35"/>
       <c r="B151" s="8">
         <v>5</v>
       </c>
@@ -9737,7 +9758,7 @@
       </c>
     </row>
     <row r="152" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="30"/>
+      <c r="A152" s="36"/>
       <c r="B152" s="8">
         <v>6</v>
       </c>
@@ -9746,7 +9767,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="31" t="s">
+      <c r="A153" s="28" t="s">
         <v>68</v>
       </c>
       <c r="B153" s="8">
@@ -9757,7 +9778,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="32"/>
+      <c r="A154" s="29"/>
       <c r="B154" s="8">
         <v>2</v>
       </c>
@@ -9766,7 +9787,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="28" t="s">
+      <c r="A155" s="34" t="s">
         <v>70</v>
       </c>
       <c r="B155" s="8">
@@ -9777,7 +9798,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="29"/>
+      <c r="A156" s="35"/>
       <c r="B156" s="8">
         <v>2</v>
       </c>
@@ -9786,7 +9807,7 @@
       </c>
     </row>
     <row r="157" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="29"/>
+      <c r="A157" s="35"/>
       <c r="B157" s="8">
         <v>3</v>
       </c>
@@ -9795,7 +9816,7 @@
       </c>
     </row>
     <row r="158" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="29"/>
+      <c r="A158" s="35"/>
       <c r="B158" s="8">
         <v>4</v>
       </c>
@@ -9804,7 +9825,7 @@
       </c>
     </row>
     <row r="159" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="29"/>
+      <c r="A159" s="35"/>
       <c r="B159" s="8">
         <v>5</v>
       </c>
@@ -9813,7 +9834,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="29"/>
+      <c r="A160" s="35"/>
       <c r="B160" s="8">
         <v>6</v>
       </c>
@@ -9822,7 +9843,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="29"/>
+      <c r="A161" s="35"/>
       <c r="B161" s="8">
         <v>7</v>
       </c>
@@ -9831,7 +9852,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="30"/>
+      <c r="A162" s="36"/>
       <c r="B162" s="8">
         <v>8</v>
       </c>
@@ -9840,16 +9861,16 @@
       </c>
     </row>
     <row r="163" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="39">
+      <c r="A163" s="38">
         <v>1</v>
       </c>
-      <c r="B163" s="40"/>
+      <c r="B163" s="39"/>
       <c r="C163" s="7" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="35" t="s">
+      <c r="A164" s="37" t="s">
         <v>73</v>
       </c>
       <c r="B164" s="8">
@@ -9860,7 +9881,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="32"/>
+      <c r="A165" s="29"/>
       <c r="B165" s="8">
         <v>3</v>
       </c>
@@ -9869,7 +9890,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="31" t="s">
+      <c r="A166" s="28" t="s">
         <v>74</v>
       </c>
       <c r="B166" s="8">
@@ -9880,7 +9901,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="32"/>
+      <c r="A167" s="29"/>
       <c r="B167" s="8">
         <v>2</v>
       </c>
@@ -9889,7 +9910,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="31" t="s">
+      <c r="A168" s="28" t="s">
         <v>75</v>
       </c>
       <c r="B168" s="8">
@@ -9900,7 +9921,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="35"/>
+      <c r="A169" s="37"/>
       <c r="B169" s="8">
         <v>2</v>
       </c>
@@ -9909,7 +9930,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="35"/>
+      <c r="A170" s="37"/>
       <c r="B170" s="8">
         <v>3</v>
       </c>
@@ -9918,7 +9939,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="32"/>
+      <c r="A171" s="29"/>
       <c r="B171" s="8">
         <v>4</v>
       </c>
@@ -9927,7 +9948,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="28" t="s">
+      <c r="A172" s="34" t="s">
         <v>76</v>
       </c>
       <c r="B172" s="8">
@@ -9938,7 +9959,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="29"/>
+      <c r="A173" s="35"/>
       <c r="B173" s="8">
         <v>2</v>
       </c>
@@ -9947,7 +9968,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="30"/>
+      <c r="A174" s="36"/>
       <c r="B174" s="8">
         <v>3</v>
       </c>
@@ -9956,7 +9977,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="31" t="s">
+      <c r="A175" s="28" t="s">
         <v>78</v>
       </c>
       <c r="B175" s="8">
@@ -9967,7 +9988,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="35"/>
+      <c r="A176" s="37"/>
       <c r="B176" s="8">
         <v>2</v>
       </c>
@@ -9976,7 +9997,7 @@
       </c>
     </row>
     <row r="177" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="35"/>
+      <c r="A177" s="37"/>
       <c r="B177" s="8">
         <v>3</v>
       </c>
@@ -9985,7 +10006,7 @@
       </c>
     </row>
     <row r="178" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="32"/>
+      <c r="A178" s="29"/>
       <c r="B178" s="8">
         <v>4</v>
       </c>
@@ -9994,7 +10015,7 @@
       </c>
     </row>
     <row r="179" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="28" t="s">
+      <c r="A179" s="34" t="s">
         <v>79</v>
       </c>
       <c r="B179" s="8">
@@ -10005,7 +10026,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="29"/>
+      <c r="A180" s="35"/>
       <c r="B180" s="8">
         <v>2</v>
       </c>
@@ -10014,7 +10035,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="30"/>
+      <c r="A181" s="36"/>
       <c r="B181" s="8">
         <v>3</v>
       </c>
@@ -10023,7 +10044,7 @@
       </c>
     </row>
     <row r="182" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="28" t="s">
+      <c r="A182" s="34" t="s">
         <v>80</v>
       </c>
       <c r="B182" s="8">
@@ -10034,7 +10055,7 @@
       </c>
     </row>
     <row r="183" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="29"/>
+      <c r="A183" s="35"/>
       <c r="B183" s="8">
         <v>2</v>
       </c>
@@ -10043,7 +10064,7 @@
       </c>
     </row>
     <row r="184" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="29"/>
+      <c r="A184" s="35"/>
       <c r="B184" s="8">
         <v>3</v>
       </c>
@@ -10052,7 +10073,7 @@
       </c>
     </row>
     <row r="185" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="29"/>
+      <c r="A185" s="35"/>
       <c r="B185" s="8">
         <v>4</v>
       </c>
@@ -10061,7 +10082,7 @@
       </c>
     </row>
     <row r="186" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="30"/>
+      <c r="A186" s="36"/>
       <c r="B186" s="8">
         <v>5</v>
       </c>
@@ -10070,7 +10091,7 @@
       </c>
     </row>
     <row r="187" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="31" t="s">
+      <c r="A187" s="28" t="s">
         <v>84</v>
       </c>
       <c r="B187" s="8">
@@ -10081,7 +10102,7 @@
       </c>
     </row>
     <row r="188" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="32"/>
+      <c r="A188" s="29"/>
       <c r="B188" s="8">
         <v>1</v>
       </c>
@@ -10090,7 +10111,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="31" t="s">
+      <c r="A189" s="28" t="s">
         <v>86</v>
       </c>
       <c r="B189" s="8">
@@ -10101,7 +10122,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="32"/>
+      <c r="A190" s="29"/>
       <c r="B190" s="8">
         <v>1</v>
       </c>
@@ -10110,7 +10131,7 @@
       </c>
     </row>
     <row r="191" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="31" t="s">
+      <c r="A191" s="28" t="s">
         <v>88</v>
       </c>
       <c r="B191" s="8">
@@ -10121,7 +10142,7 @@
       </c>
     </row>
     <row r="192" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="32"/>
+      <c r="A192" s="29"/>
       <c r="B192" s="8">
         <v>1</v>
       </c>
@@ -10130,7 +10151,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="31" t="s">
+      <c r="A193" s="28" t="s">
         <v>90</v>
       </c>
       <c r="B193" s="8">
@@ -10141,7 +10162,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="32"/>
+      <c r="A194" s="29"/>
       <c r="B194" s="8">
         <v>1</v>
       </c>
@@ -10150,7 +10171,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="31" t="s">
+      <c r="A195" s="28" t="s">
         <v>92</v>
       </c>
       <c r="B195" s="8">
@@ -10161,7 +10182,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="32"/>
+      <c r="A196" s="29"/>
       <c r="B196" s="8">
         <v>1</v>
       </c>
@@ -10170,7 +10191,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A197" s="31" t="s">
+      <c r="A197" s="28" t="s">
         <v>94</v>
       </c>
       <c r="B197" s="8">
@@ -10181,7 +10202,7 @@
       </c>
     </row>
     <row r="198" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A198" s="32"/>
+      <c r="A198" s="29"/>
       <c r="B198" s="8">
         <v>1</v>
       </c>
@@ -10190,7 +10211,7 @@
       </c>
     </row>
     <row r="199" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A199" s="31" t="s">
+      <c r="A199" s="28" t="s">
         <v>96</v>
       </c>
       <c r="B199" s="8">
@@ -10201,7 +10222,7 @@
       </c>
     </row>
     <row r="200" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A200" s="32"/>
+      <c r="A200" s="29"/>
       <c r="B200" s="8">
         <v>1</v>
       </c>
@@ -10210,7 +10231,7 @@
       </c>
     </row>
     <row r="201" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A201" s="31" t="s">
+      <c r="A201" s="28" t="s">
         <v>98</v>
       </c>
       <c r="B201" s="8">
@@ -10221,7 +10242,7 @@
       </c>
     </row>
     <row r="202" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A202" s="32"/>
+      <c r="A202" s="29"/>
       <c r="B202" s="8">
         <v>1</v>
       </c>
@@ -10230,7 +10251,7 @@
       </c>
     </row>
     <row r="203" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A203" s="31" t="s">
+      <c r="A203" s="28" t="s">
         <v>100</v>
       </c>
       <c r="B203" s="8">
@@ -10241,7 +10262,7 @@
       </c>
     </row>
     <row r="204" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A204" s="32"/>
+      <c r="A204" s="29"/>
       <c r="B204" s="8">
         <v>1</v>
       </c>
@@ -10250,7 +10271,7 @@
       </c>
     </row>
     <row r="205" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A205" s="31" t="s">
+      <c r="A205" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B205" s="8">
@@ -10261,7 +10282,7 @@
       </c>
     </row>
     <row r="206" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A206" s="32"/>
+      <c r="A206" s="29"/>
       <c r="B206" s="8">
         <v>1</v>
       </c>
@@ -10270,7 +10291,7 @@
       </c>
     </row>
     <row r="207" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A207" s="31" t="s">
+      <c r="A207" s="28" t="s">
         <v>104</v>
       </c>
       <c r="B207" s="8">
@@ -10281,7 +10302,7 @@
       </c>
     </row>
     <row r="208" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A208" s="32"/>
+      <c r="A208" s="29"/>
       <c r="B208" s="8">
         <v>1</v>
       </c>
@@ -10290,7 +10311,7 @@
       </c>
     </row>
     <row r="209" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A209" s="31" t="s">
+      <c r="A209" s="28" t="s">
         <v>106</v>
       </c>
       <c r="B209" s="8">
@@ -10301,7 +10322,7 @@
       </c>
     </row>
     <row r="210" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A210" s="32"/>
+      <c r="A210" s="29"/>
       <c r="B210" s="8">
         <v>1</v>
       </c>
@@ -10310,7 +10331,7 @@
       </c>
     </row>
     <row r="211" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A211" s="31" t="s">
+      <c r="A211" s="28" t="s">
         <v>108</v>
       </c>
       <c r="B211" s="8">
@@ -10321,7 +10342,7 @@
       </c>
     </row>
     <row r="212" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A212" s="32"/>
+      <c r="A212" s="29"/>
       <c r="B212" s="8">
         <v>1</v>
       </c>
@@ -10331,6 +10352,47 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A39:A48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A55:A62"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A114"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="A121:A128"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="A133:A134"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A146"/>
+    <mergeCell ref="A147:A152"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="A155:A162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="A168:A171"/>
+    <mergeCell ref="A172:A174"/>
+    <mergeCell ref="A175:A178"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A182:A186"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A187:A188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="A193:A194"/>
+    <mergeCell ref="A195:A196"/>
     <mergeCell ref="A207:A208"/>
     <mergeCell ref="A209:A210"/>
     <mergeCell ref="A211:A212"/>
@@ -10347,47 +10409,6 @@
     <mergeCell ref="A199:A200"/>
     <mergeCell ref="A201:A202"/>
     <mergeCell ref="A203:A204"/>
-    <mergeCell ref="A205:A206"/>
-    <mergeCell ref="A187:A188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="A193:A194"/>
-    <mergeCell ref="A195:A196"/>
-    <mergeCell ref="A168:A171"/>
-    <mergeCell ref="A172:A174"/>
-    <mergeCell ref="A175:A178"/>
-    <mergeCell ref="A179:A181"/>
-    <mergeCell ref="A182:A186"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="A155:A162"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A146"/>
-    <mergeCell ref="A147:A152"/>
-    <mergeCell ref="A121:A128"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="A133:A134"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A99"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="A104:A114"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="A39:A48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="A55:A62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A80"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10409,7 +10430,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>110</v>
       </c>
       <c r="B1" s="8">
@@ -10420,7 +10441,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
+      <c r="A2" s="29"/>
       <c r="B2" s="8">
         <v>92</v>
       </c>
@@ -10429,7 +10450,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="34" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="8">
@@ -10440,7 +10461,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -10449,7 +10470,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="8">
         <v>3</v>
       </c>
@@ -10458,7 +10479,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>112</v>
       </c>
       <c r="B6" s="8">
@@ -10469,7 +10490,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="8">
         <v>1</v>
       </c>
@@ -10478,7 +10499,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>114</v>
       </c>
       <c r="B8" s="8">
@@ -10489,7 +10510,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="8">
         <v>1</v>
       </c>
@@ -10498,7 +10519,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="28" t="s">
         <v>116</v>
       </c>
       <c r="B10" s="8">
@@ -10509,7 +10530,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="8">
         <v>1</v>
       </c>
@@ -10518,7 +10539,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="28" t="s">
         <v>118</v>
       </c>
       <c r="B12" s="8">
@@ -10529,7 +10550,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="8">
         <v>1</v>
       </c>
@@ -10538,7 +10559,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="28" t="s">
         <v>120</v>
       </c>
       <c r="B14" s="8">
@@ -10549,7 +10570,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="8">
         <v>1</v>
       </c>
@@ -10558,7 +10579,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B16" s="8">
@@ -10569,7 +10590,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="8">
         <v>2</v>
       </c>
@@ -10578,7 +10599,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="28" t="s">
         <v>124</v>
       </c>
       <c r="B18" s="8">
@@ -10589,7 +10610,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="8">
         <v>92</v>
       </c>
@@ -10598,7 +10619,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="34" t="s">
         <v>126</v>
       </c>
       <c r="B20" s="8">
@@ -10609,7 +10630,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="8">
         <v>2</v>
       </c>
@@ -10618,7 +10639,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="8">
         <v>3</v>
       </c>
@@ -10627,7 +10648,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="34" t="s">
         <v>128</v>
       </c>
       <c r="B23" s="8">
@@ -10638,7 +10659,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -10647,7 +10668,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -10656,7 +10677,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="28" t="s">
         <v>372</v>
       </c>
       <c r="B26" s="8">
@@ -10667,7 +10688,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="8">
         <v>2</v>
       </c>
@@ -10676,7 +10697,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="28" t="s">
         <v>130</v>
       </c>
       <c r="B28" s="8">
@@ -10687,7 +10708,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="8">
         <v>1</v>
       </c>
@@ -10696,7 +10717,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="28" t="s">
         <v>132</v>
       </c>
       <c r="B30" s="8">
@@ -10707,7 +10728,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="8">
         <v>1</v>
       </c>
@@ -10716,7 +10737,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="28" t="s">
         <v>134</v>
       </c>
       <c r="B32" s="8">
@@ -10727,7 +10748,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="8">
         <v>1</v>
       </c>
@@ -10736,7 +10757,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="28" t="s">
         <v>136</v>
       </c>
       <c r="B34" s="8">
@@ -10747,7 +10768,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="8">
         <v>1</v>
       </c>
@@ -10756,7 +10777,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="28" t="s">
         <v>138</v>
       </c>
       <c r="B36" s="8">
@@ -10767,7 +10788,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="8">
         <v>1</v>
       </c>
@@ -10776,7 +10797,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="28" t="s">
         <v>140</v>
       </c>
       <c r="B38" s="8">
@@ -10787,7 +10808,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="8">
         <v>1</v>
       </c>
@@ -10796,7 +10817,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="28" t="s">
         <v>142</v>
       </c>
       <c r="B40" s="8">
@@ -10807,7 +10828,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="8">
         <v>1</v>
       </c>
@@ -10816,7 +10837,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="28" t="s">
         <v>373</v>
       </c>
       <c r="B42" s="8">
@@ -10827,7 +10848,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="8">
         <v>2</v>
       </c>
@@ -10836,7 +10857,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="28" t="s">
         <v>146</v>
       </c>
       <c r="B44" s="8">
@@ -10847,7 +10868,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="8">
         <v>2</v>
       </c>
@@ -10856,7 +10877,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
+      <c r="A46" s="37"/>
       <c r="B46" s="8">
         <v>3</v>
       </c>
@@ -10865,7 +10886,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="8">
         <v>4</v>
       </c>
@@ -10874,7 +10895,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="34" t="s">
         <v>148</v>
       </c>
       <c r="B48" s="8">
@@ -10885,7 +10906,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="8">
         <v>2</v>
       </c>
@@ -10900,6 +10921,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:C50"/>
@@ -10908,21 +10944,6 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10944,7 +10965,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46"/>
+      <c r="A1" s="48"/>
       <c r="B1" s="8">
         <v>3</v>
       </c>
@@ -10953,7 +10974,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
+      <c r="A2" s="49"/>
       <c r="B2" s="8">
         <v>4</v>
       </c>
@@ -10962,7 +10983,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>150</v>
       </c>
       <c r="B3" s="8">
@@ -10973,7 +10994,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="8">
         <v>92</v>
       </c>
@@ -10982,7 +11003,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="28" t="s">
         <v>151</v>
       </c>
       <c r="B5" s="8">
@@ -10993,7 +11014,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="8">
         <v>2</v>
       </c>
@@ -11002,7 +11023,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="28" t="s">
         <v>152</v>
       </c>
       <c r="B7" s="8">
@@ -11013,7 +11034,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="8">
         <v>92</v>
       </c>
@@ -11022,7 +11043,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="28" t="s">
         <v>156</v>
       </c>
       <c r="B9" s="8">
@@ -11033,7 +11054,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="8">
         <v>1</v>
       </c>
@@ -11042,7 +11063,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="28" t="s">
         <v>158</v>
       </c>
       <c r="B11" s="8">
@@ -11053,7 +11074,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="8">
         <v>1</v>
       </c>
@@ -11062,7 +11083,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="28" t="s">
         <v>160</v>
       </c>
       <c r="B13" s="8">
@@ -11073,7 +11094,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="8">
         <v>1</v>
       </c>
@@ -11082,7 +11103,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="28" t="s">
         <v>162</v>
       </c>
       <c r="B15" s="8">
@@ -11093,7 +11114,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="8">
         <v>1</v>
       </c>
@@ -11102,7 +11123,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="28" t="s">
         <v>164</v>
       </c>
       <c r="B17" s="8">
@@ -11113,7 +11134,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="8">
         <v>1</v>
       </c>
@@ -11122,7 +11143,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="28" t="s">
         <v>166</v>
       </c>
       <c r="B19" s="8">
@@ -11133,7 +11154,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="8">
         <v>1</v>
       </c>
@@ -11142,7 +11163,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="28" t="s">
         <v>168</v>
       </c>
       <c r="B21" s="8">
@@ -11153,7 +11174,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="8">
         <v>1</v>
       </c>
@@ -11162,7 +11183,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="34" t="s">
         <v>172</v>
       </c>
       <c r="B23" s="8">
@@ -11173,7 +11194,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="8">
         <v>2</v>
       </c>
@@ -11182,7 +11203,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -11191,7 +11212,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="28" t="s">
         <v>174</v>
       </c>
       <c r="B26" s="8">
@@ -11202,7 +11223,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="8">
         <v>2</v>
       </c>
@@ -11211,7 +11232,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="8">
         <v>3</v>
       </c>
@@ -11220,7 +11241,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="8">
         <v>4</v>
       </c>
@@ -11229,7 +11250,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="34" t="s">
         <v>176</v>
       </c>
       <c r="B30" s="8">
@@ -11240,7 +11261,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="8">
         <v>2</v>
       </c>
@@ -11249,7 +11270,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="8">
         <v>3</v>
       </c>
@@ -11258,7 +11279,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="28" t="s">
         <v>178</v>
       </c>
       <c r="B33" s="8">
@@ -11269,7 +11290,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="8">
         <v>2</v>
       </c>
@@ -11278,7 +11299,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="8">
         <v>3</v>
       </c>
@@ -11287,7 +11308,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="8">
         <v>4</v>
       </c>
@@ -11296,7 +11317,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="34" t="s">
         <v>180</v>
       </c>
       <c r="B37" s="8">
@@ -11307,7 +11328,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="8">
         <v>2</v>
       </c>
@@ -11316,7 +11337,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="36"/>
       <c r="B39" s="8">
         <v>3</v>
       </c>
@@ -11325,7 +11346,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B40" s="8">
@@ -11336,7 +11357,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
+      <c r="A41" s="37"/>
       <c r="B41" s="8">
         <v>2</v>
       </c>
@@ -11345,7 +11366,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="8">
         <v>3</v>
       </c>
@@ -11354,7 +11375,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="8">
         <v>4</v>
       </c>
@@ -11363,7 +11384,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="34" t="s">
         <v>184</v>
       </c>
       <c r="B44" s="8">
@@ -11374,7 +11395,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="8">
         <v>2</v>
       </c>
@@ -11383,7 +11404,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="8">
         <v>3</v>
       </c>
@@ -11392,7 +11413,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="34" t="s">
         <v>186</v>
       </c>
       <c r="B47" s="8">
@@ -11403,7 +11424,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="8">
         <v>2</v>
       </c>
@@ -11412,7 +11433,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="8">
         <v>3</v>
       </c>
@@ -11421,16 +11442,16 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="48">
+      <c r="A50" s="46">
         <v>4</v>
       </c>
-      <c r="B50" s="49"/>
+      <c r="B50" s="47"/>
       <c r="C50" s="7" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="34" t="s">
         <v>188</v>
       </c>
       <c r="B51" s="8">
@@ -11441,7 +11462,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
+      <c r="A52" s="35"/>
       <c r="B52" s="8">
         <v>2</v>
       </c>
@@ -11450,7 +11471,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="36"/>
       <c r="B53" s="8">
         <v>3</v>
       </c>
@@ -11459,7 +11480,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="28" t="s">
         <v>190</v>
       </c>
       <c r="B54" s="8">
@@ -11470,7 +11491,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35"/>
+      <c r="A55" s="37"/>
       <c r="B55" s="8">
         <v>2</v>
       </c>
@@ -11479,7 +11500,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35"/>
+      <c r="A56" s="37"/>
       <c r="B56" s="8">
         <v>3</v>
       </c>
@@ -11488,7 +11509,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
+      <c r="A57" s="29"/>
       <c r="B57" s="8">
         <v>4</v>
       </c>
@@ -11497,7 +11518,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="34" t="s">
         <v>192</v>
       </c>
       <c r="B58" s="8">
@@ -11508,7 +11529,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
+      <c r="A59" s="35"/>
       <c r="B59" s="8">
         <v>2</v>
       </c>
@@ -11517,7 +11538,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+      <c r="A60" s="36"/>
       <c r="B60" s="8">
         <v>3</v>
       </c>
@@ -11526,7 +11547,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="28" t="s">
         <v>194</v>
       </c>
       <c r="B61" s="8">
@@ -11537,7 +11558,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
+      <c r="A62" s="37"/>
       <c r="B62" s="8">
         <v>2</v>
       </c>
@@ -11546,7 +11567,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
+      <c r="A63" s="37"/>
       <c r="B63" s="8">
         <v>3</v>
       </c>
@@ -11555,7 +11576,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
+      <c r="A64" s="29"/>
       <c r="B64" s="8">
         <v>4</v>
       </c>
@@ -11564,7 +11585,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="34" t="s">
         <v>196</v>
       </c>
       <c r="B65" s="8">
@@ -11575,7 +11596,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="29"/>
+      <c r="A66" s="35"/>
       <c r="B66" s="8">
         <v>2</v>
       </c>
@@ -11584,7 +11605,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
+      <c r="A67" s="36"/>
       <c r="B67" s="8">
         <v>3</v>
       </c>
@@ -11593,7 +11614,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="31" t="s">
+      <c r="A68" s="28" t="s">
         <v>198</v>
       </c>
       <c r="B68" s="8">
@@ -11604,7 +11625,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="35"/>
+      <c r="A69" s="37"/>
       <c r="B69" s="8">
         <v>2</v>
       </c>
@@ -11613,7 +11634,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="35"/>
+      <c r="A70" s="37"/>
       <c r="B70" s="8">
         <v>3</v>
       </c>
@@ -11622,7 +11643,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="32"/>
+      <c r="A71" s="29"/>
       <c r="B71" s="8">
         <v>4</v>
       </c>
@@ -11631,7 +11652,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="28" t="s">
+      <c r="A72" s="34" t="s">
         <v>200</v>
       </c>
       <c r="B72" s="8">
@@ -11642,7 +11663,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
+      <c r="A73" s="35"/>
       <c r="B73" s="8">
         <v>2</v>
       </c>
@@ -11651,7 +11672,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="36"/>
       <c r="B74" s="8">
         <v>3</v>
       </c>
@@ -11660,7 +11681,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="31" t="s">
+      <c r="A75" s="28" t="s">
         <v>202</v>
       </c>
       <c r="B75" s="8">
@@ -11671,7 +11692,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="35"/>
+      <c r="A76" s="37"/>
       <c r="B76" s="8">
         <v>2</v>
       </c>
@@ -11680,7 +11701,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="35"/>
+      <c r="A77" s="37"/>
       <c r="B77" s="8">
         <v>3</v>
       </c>
@@ -11689,7 +11710,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="32"/>
+      <c r="A78" s="29"/>
       <c r="B78" s="8">
         <v>4</v>
       </c>
@@ -11698,7 +11719,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="s">
+      <c r="A79" s="34" t="s">
         <v>204</v>
       </c>
       <c r="B79" s="8">
@@ -11709,7 +11730,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="29"/>
+      <c r="A80" s="35"/>
       <c r="B80" s="8">
         <v>2</v>
       </c>
@@ -11718,7 +11739,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
+      <c r="A81" s="36"/>
       <c r="B81" s="8">
         <v>3</v>
       </c>
@@ -11727,7 +11748,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="31" t="s">
+      <c r="A82" s="28" t="s">
         <v>206</v>
       </c>
       <c r="B82" s="8">
@@ -11738,7 +11759,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="35"/>
+      <c r="A83" s="37"/>
       <c r="B83" s="8">
         <v>2</v>
       </c>
@@ -11747,7 +11768,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="35"/>
+      <c r="A84" s="37"/>
       <c r="B84" s="8">
         <v>3</v>
       </c>
@@ -11756,7 +11777,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="32"/>
+      <c r="A85" s="29"/>
       <c r="B85" s="8">
         <v>4</v>
       </c>
@@ -11765,7 +11786,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="28" t="s">
+      <c r="A86" s="34" t="s">
         <v>208</v>
       </c>
       <c r="B86" s="8">
@@ -11776,7 +11797,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="29"/>
+      <c r="A87" s="35"/>
       <c r="B87" s="8">
         <v>2</v>
       </c>
@@ -11785,7 +11806,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+      <c r="A88" s="36"/>
       <c r="B88" s="8">
         <v>3</v>
       </c>
@@ -11794,7 +11815,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="28" t="s">
+      <c r="A89" s="34" t="s">
         <v>212</v>
       </c>
       <c r="B89" s="8">
@@ -11805,7 +11826,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="29"/>
+      <c r="A90" s="35"/>
       <c r="B90" s="8">
         <v>2</v>
       </c>
@@ -11814,7 +11835,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="30"/>
+      <c r="A91" s="36"/>
       <c r="B91" s="8">
         <v>3</v>
       </c>
@@ -11823,7 +11844,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="34" t="s">
         <v>214</v>
       </c>
       <c r="B92" s="8">
@@ -11834,7 +11855,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
+      <c r="A93" s="35"/>
       <c r="B93" s="8">
         <v>2</v>
       </c>
@@ -11843,7 +11864,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
+      <c r="A94" s="35"/>
       <c r="B94" s="8">
         <v>3</v>
       </c>
@@ -11852,7 +11873,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="29"/>
+      <c r="A95" s="35"/>
       <c r="B95" s="8">
         <v>4</v>
       </c>
@@ -11861,7 +11882,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="29"/>
+      <c r="A96" s="35"/>
       <c r="B96" s="8">
         <v>5</v>
       </c>
@@ -11870,7 +11891,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
+      <c r="A97" s="36"/>
       <c r="B97" s="8">
         <v>6</v>
       </c>
@@ -11879,16 +11900,16 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="39">
+      <c r="A98" s="38">
         <v>1</v>
       </c>
-      <c r="B98" s="40"/>
+      <c r="B98" s="39"/>
       <c r="C98" s="7" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="29" t="s">
+      <c r="A99" s="35" t="s">
         <v>216</v>
       </c>
       <c r="B99" s="8">
@@ -11899,7 +11920,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="29"/>
+      <c r="A100" s="35"/>
       <c r="B100" s="8">
         <v>3</v>
       </c>
@@ -11908,7 +11929,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="29"/>
+      <c r="A101" s="35"/>
       <c r="B101" s="8">
         <v>4</v>
       </c>
@@ -11917,7 +11938,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
+      <c r="A102" s="35"/>
       <c r="B102" s="8">
         <v>5</v>
       </c>
@@ -11926,7 +11947,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="29"/>
+      <c r="A103" s="35"/>
       <c r="B103" s="8">
         <v>6</v>
       </c>
@@ -11935,7 +11956,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="29"/>
+      <c r="A104" s="35"/>
       <c r="B104" s="8">
         <v>7</v>
       </c>
@@ -11944,7 +11965,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="29"/>
+      <c r="A105" s="35"/>
       <c r="B105" s="8">
         <v>8</v>
       </c>
@@ -11953,7 +11974,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="29"/>
+      <c r="A106" s="35"/>
       <c r="B106" s="8">
         <v>9</v>
       </c>
@@ -11962,7 +11983,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="29"/>
+      <c r="A107" s="35"/>
       <c r="B107" s="8">
         <v>10</v>
       </c>
@@ -11971,7 +11992,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="29"/>
+      <c r="A108" s="35"/>
       <c r="B108" s="8">
         <v>11</v>
       </c>
@@ -11980,7 +12001,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="29"/>
+      <c r="A109" s="35"/>
       <c r="B109" s="8">
         <v>12</v>
       </c>
@@ -11989,7 +12010,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="29"/>
+      <c r="A110" s="35"/>
       <c r="B110" s="8">
         <v>13</v>
       </c>
@@ -11998,7 +12019,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="29"/>
+      <c r="A111" s="35"/>
       <c r="B111" s="8">
         <v>14</v>
       </c>
@@ -12007,7 +12028,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="29"/>
+      <c r="A112" s="35"/>
       <c r="B112" s="8">
         <v>15</v>
       </c>
@@ -12016,7 +12037,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="30"/>
+      <c r="A113" s="36"/>
       <c r="B113" s="8">
         <v>16</v>
       </c>
@@ -12025,7 +12046,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="31" t="s">
+      <c r="A114" s="28" t="s">
         <v>226</v>
       </c>
       <c r="B114" s="8">
@@ -12036,7 +12057,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="32"/>
+      <c r="A115" s="29"/>
       <c r="B115" s="8">
         <v>2</v>
       </c>
@@ -12045,7 +12066,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="31" t="s">
+      <c r="A116" s="28" t="s">
         <v>230</v>
       </c>
       <c r="B116" s="8">
@@ -12056,7 +12077,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="35"/>
+      <c r="A117" s="37"/>
       <c r="B117" s="8">
         <v>2</v>
       </c>
@@ -12065,7 +12086,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="35"/>
+      <c r="A118" s="37"/>
       <c r="B118" s="8">
         <v>3</v>
       </c>
@@ -12074,7 +12095,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="32"/>
+      <c r="A119" s="29"/>
       <c r="B119" s="8">
         <v>4</v>
       </c>
@@ -12083,7 +12104,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="28" t="s">
+      <c r="A120" s="34" t="s">
         <v>232</v>
       </c>
       <c r="B120" s="8">
@@ -12094,7 +12115,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="29"/>
+      <c r="A121" s="35"/>
       <c r="B121" s="8">
         <v>2</v>
       </c>
@@ -12103,7 +12124,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="29"/>
+      <c r="A122" s="35"/>
       <c r="B122" s="8">
         <v>3</v>
       </c>
@@ -12112,7 +12133,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="29"/>
+      <c r="A123" s="35"/>
       <c r="B123" s="8">
         <v>4</v>
       </c>
@@ -12121,7 +12142,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="29"/>
+      <c r="A124" s="35"/>
       <c r="B124" s="8">
         <v>5</v>
       </c>
@@ -12130,7 +12151,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="29"/>
+      <c r="A125" s="35"/>
       <c r="B125" s="8">
         <v>6</v>
       </c>
@@ -12139,7 +12160,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="29"/>
+      <c r="A126" s="35"/>
       <c r="B126" s="8">
         <v>7</v>
       </c>
@@ -12148,7 +12169,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="29"/>
+      <c r="A127" s="35"/>
       <c r="B127" s="8">
         <v>8</v>
       </c>
@@ -12157,7 +12178,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="29"/>
+      <c r="A128" s="35"/>
       <c r="B128" s="8">
         <v>9</v>
       </c>
@@ -12166,7 +12187,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="29"/>
+      <c r="A129" s="35"/>
       <c r="B129" s="8">
         <v>10</v>
       </c>
@@ -12175,7 +12196,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="29"/>
+      <c r="A130" s="35"/>
       <c r="B130" s="8">
         <v>11</v>
       </c>
@@ -12184,7 +12205,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="29"/>
+      <c r="A131" s="35"/>
       <c r="B131" s="8">
         <v>12</v>
       </c>
@@ -12193,7 +12214,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="30"/>
+      <c r="A132" s="36"/>
       <c r="B132" s="8">
         <v>13</v>
       </c>
@@ -12202,7 +12223,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="31" t="s">
+      <c r="A133" s="28" t="s">
         <v>235</v>
       </c>
       <c r="B133" s="8">
@@ -12213,7 +12234,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="35"/>
+      <c r="A134" s="37"/>
       <c r="B134" s="8">
         <v>2</v>
       </c>
@@ -12222,7 +12243,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="35"/>
+      <c r="A135" s="37"/>
       <c r="B135" s="8">
         <v>3</v>
       </c>
@@ -12231,7 +12252,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="32"/>
+      <c r="A136" s="29"/>
       <c r="B136" s="8">
         <v>4</v>
       </c>
@@ -12241,6 +12262,36 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A82:A85"/>
     <mergeCell ref="A114:A115"/>
     <mergeCell ref="A116:A119"/>
     <mergeCell ref="A120:A132"/>
@@ -12250,36 +12301,6 @@
     <mergeCell ref="A92:A97"/>
     <mergeCell ref="A98:B98"/>
     <mergeCell ref="A99:A113"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>